<commit_message>
Song list update Sep 17th, 2025, Rev2
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mit3uri\mit3uri-song-list\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D663F00-E02A-48AE-B629-F60A436E0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB76FD8-0C48-48D7-8598-3C98A44B5A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="1140" windowWidth="28800" windowHeight="15435" xr2:uid="{1DAD23D6-F6F7-4BBB-811A-57551CBA627F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1588">
   <si>
     <t>序号</t>
   </si>
@@ -4773,6 +4773,33 @@
   </si>
   <si>
     <t>2025/09/17，2025/09/15</t>
+  </si>
+  <si>
+    <t>2025/04/04，2025/09/02</t>
+  </si>
+  <si>
+    <t>黑色幽默</t>
+  </si>
+  <si>
+    <t>我最亲爱的</t>
+  </si>
+  <si>
+    <t>宠爱</t>
+  </si>
+  <si>
+    <t>慢慢喜欢你</t>
+  </si>
+  <si>
+    <t>萱草花</t>
+  </si>
+  <si>
+    <t>张小斐</t>
+  </si>
+  <si>
+    <t>How long will I Love you</t>
+  </si>
+  <si>
+    <t>Ellie Goulding</t>
   </si>
 </sst>
 </file>
@@ -4992,7 +5019,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5329,10 +5356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8030F645-0AE7-49C3-B587-33454A6B20BA}">
-  <dimension ref="A1:I651"/>
+  <dimension ref="A1:I657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A617" workbookViewId="0">
-      <selection activeCell="B645" sqref="B645"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12061,15 +12088,15 @@
       <c r="D288" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="E288" s="9">
-        <v>45751</v>
+      <c r="E288" s="7" t="s">
+        <v>1579</v>
       </c>
       <c r="F288" s="8"/>
       <c r="G288" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H288" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I288" s="8"/>
     </row>
@@ -20036,7 +20063,7 @@
         <v>1545</v>
       </c>
       <c r="C634" s="8"/>
-      <c r="D634" s="21" t="s">
+      <c r="D634" s="11" t="s">
         <v>1546</v>
       </c>
       <c r="E634" s="7" t="s">
@@ -20059,7 +20086,7 @@
         <v>1548</v>
       </c>
       <c r="C635" s="8"/>
-      <c r="D635" s="21" t="s">
+      <c r="D635" s="11" t="s">
         <v>1549</v>
       </c>
       <c r="E635" s="9">
@@ -20197,7 +20224,7 @@
         <v>1558</v>
       </c>
       <c r="C641" s="8"/>
-      <c r="D641" s="21" t="s">
+      <c r="D641" s="11" t="s">
         <v>1559</v>
       </c>
       <c r="E641" s="9">
@@ -20266,7 +20293,7 @@
         <v>1563</v>
       </c>
       <c r="C644" s="8"/>
-      <c r="D644" s="21" t="s">
+      <c r="D644" s="11" t="s">
         <v>1564</v>
       </c>
       <c r="E644" s="9">
@@ -20335,7 +20362,7 @@
         <v>1569</v>
       </c>
       <c r="C647" s="8"/>
-      <c r="D647" s="22" t="s">
+      <c r="D647" s="15" t="s">
         <v>1570</v>
       </c>
       <c r="E647" s="9">
@@ -20441,6 +20468,144 @@
         <v>2</v>
       </c>
       <c r="I651" s="8"/>
+    </row>
+    <row r="652" spans="1:9">
+      <c r="A652" s="6">
+        <v>651</v>
+      </c>
+      <c r="B652" s="7" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C652" s="8"/>
+      <c r="D652" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E652" s="9">
+        <v>45917</v>
+      </c>
+      <c r="F652" s="8"/>
+      <c r="G652" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H652" s="6">
+        <v>1</v>
+      </c>
+      <c r="I652" s="8"/>
+    </row>
+    <row r="653" spans="1:9">
+      <c r="A653" s="6">
+        <v>652</v>
+      </c>
+      <c r="B653" s="7" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C653" s="8"/>
+      <c r="D653" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E653" s="9">
+        <v>45902</v>
+      </c>
+      <c r="F653" s="8"/>
+      <c r="G653" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H653" s="6">
+        <v>1</v>
+      </c>
+      <c r="I653" s="8"/>
+    </row>
+    <row r="654" spans="1:9">
+      <c r="A654" s="6">
+        <v>653</v>
+      </c>
+      <c r="B654" s="7" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C654" s="8"/>
+      <c r="D654" s="7" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E654" s="9">
+        <v>45902</v>
+      </c>
+      <c r="F654" s="8"/>
+      <c r="G654" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H654" s="6">
+        <v>1</v>
+      </c>
+      <c r="I654" s="8"/>
+    </row>
+    <row r="655" spans="1:9">
+      <c r="A655" s="6">
+        <v>654</v>
+      </c>
+      <c r="B655" s="7" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C655" s="8"/>
+      <c r="D655" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E655" s="9">
+        <v>45915</v>
+      </c>
+      <c r="F655" s="8"/>
+      <c r="G655" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H655" s="6">
+        <v>1</v>
+      </c>
+      <c r="I655" s="8"/>
+    </row>
+    <row r="656" spans="1:9">
+      <c r="A656" s="6">
+        <v>655</v>
+      </c>
+      <c r="B656" s="7" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C656" s="8"/>
+      <c r="D656" s="21" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E656" s="9">
+        <v>45915</v>
+      </c>
+      <c r="F656" s="8"/>
+      <c r="G656" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H656" s="6">
+        <v>1</v>
+      </c>
+      <c r="I656" s="8"/>
+    </row>
+    <row r="657" spans="1:9">
+      <c r="A657" s="6">
+        <v>656</v>
+      </c>
+      <c r="B657" s="7" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C657" s="8"/>
+      <c r="D657" s="7" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E657" s="9">
+        <v>45915</v>
+      </c>
+      <c r="F657" s="8"/>
+      <c r="G657" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H657" s="6">
+        <v>1</v>
+      </c>
+      <c r="I657" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed some errors in the song list
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -22632,7 +22632,7 @@
       <c r="F619" t="inlineStr"/>
       <c r="G619" t="inlineStr">
         <is>
-          <t>日语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H619" t="inlineStr">
@@ -22706,7 +22706,7 @@
       <c r="F621" t="inlineStr"/>
       <c r="G621" t="inlineStr">
         <is>
-          <t>日语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H621" t="inlineStr">

</xml_diff>

<commit_message>
Update song list to Jan 29, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I788"/>
+  <dimension ref="A1:I789"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,7 +979,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19</t>
+          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/28</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -990,7 +990,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/25</t>
+          <t>2025/03/04，2025/05/25，2026/1/28</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1809,10 +1809,14 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>BV1jn6cBFEN1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2803,7 +2807,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/28</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2814,7 +2818,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3994,7 +3998,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/04/13，2025/04/19，2025/05/06，2025/06/03，2025/08/28，2025/09/17，2025/10/10，2025/11/17，2025/11/22，2025/12/24，2026/1/15</t>
+          <t>2025/03/13，2025/04/13，2025/04/19，2025/05/06，2025/06/03，2025/08/28，2025/09/17，2025/10/10，2025/11/17，2025/11/22，2025/12/24，2026/1/15，2026/1/28</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -4005,10 +4009,14 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>BV1iRhUzZECK</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4597,7 +4605,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/11，2025/04/25，2025/06/05，2025/06/15，2025/07/07，2025/09/11，2025/10/10，2025/11/14，2025/12/9</t>
+          <t>2025/03/14，2025/04/11，2025/04/25，2025/06/05，2025/06/15，2025/07/07，2025/09/11，2025/10/10，2025/11/14，2025/12/9，2026/1/28</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -4608,10 +4616,14 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr"/>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>BV1bZvxBGEiJ</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5192,7 +5204,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21</t>
+          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/28</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -5203,7 +5215,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -5480,7 +5492,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/06/05，2025/06/05，2025/06/23，2025/08/12，2025/09/12，2025/09/02，2025/11/9，2025/12/4，2026/1/1</t>
+          <t>2025/03/17，2025/06/05，2025/06/05，2025/06/23，2025/08/12，2025/09/12，2025/09/02，2025/11/9，2025/12/4，2026/1/1，2026/1/28</t>
         </is>
       </c>
       <c r="F137" t="inlineStr"/>
@@ -5491,10 +5503,14 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I137" t="inlineStr"/>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>BV1CF2LBhEi1</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -6107,7 +6123,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/05/23，2025/07/21，2025/08/08，2025/09/05</t>
+          <t>2025/03/20，2025/05/23，2025/07/21，2025/08/08，2025/09/05，2026/1/28</t>
         </is>
       </c>
       <c r="F154" t="inlineStr"/>
@@ -6118,10 +6134,14 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>BV14fJwzJEZQ</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7134,7 +7154,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23</t>
+          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23，2026/1/28</t>
         </is>
       </c>
       <c r="F183" t="inlineStr"/>
@@ -7145,7 +7165,7 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>29</t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
@@ -7278,7 +7298,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13</t>
+          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13，2026/1/28</t>
         </is>
       </c>
       <c r="F187" t="inlineStr"/>
@@ -7289,7 +7309,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -8593,7 +8613,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>2025/03/28，2025/05/05，2025/05/08，2025/05/15，2025/05/30，2025/06/13，2025/06/23，2025/07/10，2025/07/24，2025/08/04，2025/09/03，2025/09/21，2025/11/9，2025/11/26，2026/1/16</t>
+          <t>2025/03/28，2025/05/05，2025/05/08，2025/05/15，2025/05/30，2025/06/13，2025/06/23，2025/07/10，2025/07/24，2025/08/04，2025/09/03，2025/09/21，2025/11/9，2025/11/26，2026/1/16，2026/1/28</t>
         </is>
       </c>
       <c r="F224" t="inlineStr"/>
@@ -8604,10 +8624,14 @@
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="I224" t="inlineStr"/>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>BV1ZtE2zsEfw</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -10480,7 +10504,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>2025/04/03，2025/04/15，2025/05/22，2025/05/29，2025/06/02，2025/06/07，2025/06/12，2025/06/21，2025/06/23，2025/07/08，2025/07/13，2025/07/21，2025/08/01，2025/08/03，2025/09/02，2025/09/19，2025/10/10，2025/11/12，2025/11/26，2025/12/6，2026/1/9</t>
+          <t>2025/04/03，2025/04/15，2025/05/22，2025/05/29，2025/06/02，2025/06/07，2025/06/12，2025/06/21，2025/06/23，2025/07/08，2025/07/13，2025/07/21，2025/08/01，2025/08/03，2025/09/02，2025/09/19，2025/10/10，2025/11/12，2025/11/26，2025/12/6，2026/1/9，2026/1/28</t>
         </is>
       </c>
       <c r="F277" t="inlineStr"/>
@@ -10491,7 +10515,7 @@
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="I277" t="inlineStr">
@@ -10694,7 +10718,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>2025/04/04</t>
+          <t>2025/04/04，2026/1/28</t>
         </is>
       </c>
       <c r="F283" t="inlineStr"/>
@@ -10705,7 +10729,7 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I283" t="inlineStr"/>
@@ -11429,7 +11453,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>2025/04/07，2025/04/24，2025/05/03，2025/05/23，2025/06/07，2025/06/12，2025/06/23，2025/06/29，2025/07/15，2025/07/25，2025/09/24，2025/10/18，2025/11/12，2025/11/24，2025/12/23</t>
+          <t>2025/04/07，2025/04/24，2025/05/03，2025/05/23，2025/06/07，2025/06/12，2025/06/23，2025/06/29，2025/07/15，2025/07/25，2025/09/24，2025/10/18，2025/11/12，2025/11/24，2025/12/23，2026/1/28</t>
         </is>
       </c>
       <c r="F304" t="inlineStr"/>
@@ -11440,7 +11464,7 @@
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I304" t="inlineStr">
@@ -12079,7 +12103,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21</t>
+          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21，2026/1/28</t>
         </is>
       </c>
       <c r="F322" t="inlineStr"/>
@@ -12090,10 +12114,14 @@
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="I322" t="inlineStr"/>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>BV1TP7LzmEnU</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -13838,7 +13866,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>2025/04/20，2025/04/27，2025/05/05，2025/05/09，2025/05/18，2025/06/07，2025/06/13，2025/06/21，2025/07/05，2025/07/15，2025/07/25，2025/08/08，2025/08/26，2025/08/28，2025/09/14，2025/09/30，2025/10/03，2025/10/24，2025/10/31，2025/11/9，2025/11/26，2025/12/5，2025/12/6，2026/1/1</t>
+          <t>2025/04/20，2025/04/27，2025/05/05，2025/05/09，2025/05/18，2025/06/07，2025/06/13，2025/06/21，2025/07/05，2025/07/15，2025/07/25，2025/08/08，2025/08/26，2025/08/28，2025/09/14，2025/09/30，2025/10/03，2025/10/24，2025/10/31，2025/11/9，2025/11/26，2025/12/5，2025/12/6，2026/1/1，2026/1/28</t>
         </is>
       </c>
       <c r="F371" t="inlineStr"/>
@@ -13849,7 +13877,7 @@
       </c>
       <c r="H371" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="I371" t="inlineStr">
@@ -14908,7 +14936,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24</t>
+          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24，2026/1/28</t>
         </is>
       </c>
       <c r="F401" t="inlineStr"/>
@@ -14919,10 +14947,14 @@
       </c>
       <c r="H401" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I401" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>BV196BQBhEf1</t>
+        </is>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -22739,7 +22771,7 @@
       </c>
       <c r="E622" t="inlineStr">
         <is>
-          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9</t>
+          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9，2026/1/28</t>
         </is>
       </c>
       <c r="F622" t="inlineStr"/>
@@ -22750,10 +22782,14 @@
       </c>
       <c r="H622" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I622" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I622" t="inlineStr">
+        <is>
+          <t>BV1LYvKzmEyV</t>
+        </is>
+      </c>
     </row>
     <row r="623">
       <c r="A623" t="inlineStr">
@@ -25482,7 +25518,7 @@
       </c>
       <c r="E699" t="inlineStr">
         <is>
-          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26</t>
+          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26，2026/1/28</t>
         </is>
       </c>
       <c r="F699" t="inlineStr"/>
@@ -25493,7 +25529,7 @@
       </c>
       <c r="H699" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I699" t="inlineStr"/>
@@ -27583,7 +27619,7 @@
       </c>
       <c r="E758" t="inlineStr">
         <is>
-          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17</t>
+          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/28</t>
         </is>
       </c>
       <c r="F758" t="inlineStr"/>
@@ -27594,7 +27630,7 @@
       </c>
       <c r="H758" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I758" t="inlineStr">
@@ -27867,7 +27903,7 @@
       </c>
       <c r="E766" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23</t>
+          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23，2026/1/28</t>
         </is>
       </c>
       <c r="F766" t="inlineStr"/>
@@ -27878,7 +27914,7 @@
       </c>
       <c r="H766" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I766" t="inlineStr">
@@ -28315,7 +28351,7 @@
       </c>
       <c r="E778" t="inlineStr">
         <is>
-          <t>2026/1/15</t>
+          <t>2026/1/15，2026/1/28</t>
         </is>
       </c>
       <c r="F778" t="inlineStr"/>
@@ -28326,7 +28362,7 @@
       </c>
       <c r="H778" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I778" t="inlineStr">
@@ -28692,6 +28728,41 @@
         </is>
       </c>
       <c r="I788" t="inlineStr"/>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr"/>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>爱要坦荡荡(R&amp;B版)</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr"/>
+      <c r="D789" t="inlineStr">
+        <is>
+          <t>顾叮当</t>
+        </is>
+      </c>
+      <c r="E789" t="inlineStr">
+        <is>
+          <t>2026/1/28</t>
+        </is>
+      </c>
+      <c r="F789" t="inlineStr"/>
+      <c r="G789" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H789" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I789" t="inlineStr">
+        <is>
+          <t>BV1Xx6cBRE14</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed the wrong dates in the song list
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -979,7 +979,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/28</t>
+          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/29</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/25，2026/1/28</t>
+          <t>2025/03/04，2025/05/25，2026/1/29</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/28</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/04/13，2025/04/19，2025/05/06，2025/06/03，2025/08/28，2025/09/17，2025/10/10，2025/11/17，2025/11/22，2025/12/24，2026/1/15，2026/1/28</t>
+          <t>2025/03/13，2025/04/13，2025/04/19，2025/05/06，2025/06/03，2025/08/28，2025/09/17，2025/10/10，2025/11/17，2025/11/22，2025/12/24，2026/1/15，2026/1/29</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/11，2025/04/25，2025/06/05，2025/06/15，2025/07/07，2025/09/11，2025/10/10，2025/11/14，2025/12/9，2026/1/28</t>
+          <t>2025/03/14，2025/04/11，2025/04/25，2025/06/05，2025/06/15，2025/07/07，2025/09/11，2025/10/10，2025/11/14，2025/12/9</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -5204,7 +5204,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/28</t>
+          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/06/05，2025/06/05，2025/06/23，2025/08/12，2025/09/12，2025/09/02，2025/11/9，2025/12/4，2026/1/1，2026/1/28</t>
+          <t>2025/03/17，2025/06/05，2025/06/05，2025/06/23，2025/08/12，2025/09/12，2025/09/02，2025/11/9，2025/12/4，2026/1/1，2026/1/29</t>
         </is>
       </c>
       <c r="F137" t="inlineStr"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/05/23，2025/07/21，2025/08/08，2025/09/05，2026/1/28</t>
+          <t>2025/03/20，2025/05/23，2025/07/21，2025/08/08，2025/09/05，2026/1/29</t>
         </is>
       </c>
       <c r="F154" t="inlineStr"/>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23，2026/1/28</t>
+          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23，2026/1/29</t>
         </is>
       </c>
       <c r="F183" t="inlineStr"/>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13，2026/1/28</t>
+          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13，2026/1/29</t>
         </is>
       </c>
       <c r="F187" t="inlineStr"/>
@@ -8613,7 +8613,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>2025/03/28，2025/05/05，2025/05/08，2025/05/15，2025/05/30，2025/06/13，2025/06/23，2025/07/10，2025/07/24，2025/08/04，2025/09/03，2025/09/21，2025/11/9，2025/11/26，2026/1/16，2026/1/28</t>
+          <t>2025/03/28，2025/05/05，2025/05/08，2025/05/15，2025/05/30，2025/06/13，2025/06/23，2025/07/10，2025/07/24，2025/08/04，2025/09/03，2025/09/21，2025/11/9，2025/11/26，2026/1/16，2026/1/29</t>
         </is>
       </c>
       <c r="F224" t="inlineStr"/>
@@ -10504,7 +10504,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>2025/04/03，2025/04/15，2025/05/22，2025/05/29，2025/06/02，2025/06/07，2025/06/12，2025/06/21，2025/06/23，2025/07/08，2025/07/13，2025/07/21，2025/08/01，2025/08/03，2025/09/02，2025/09/19，2025/10/10，2025/11/12，2025/11/26，2025/12/6，2026/1/9，2026/1/28</t>
+          <t>2025/04/03，2025/04/15，2025/05/22，2025/05/29，2025/06/02，2025/06/07，2025/06/12，2025/06/21，2025/06/23，2025/07/08，2025/07/13，2025/07/21，2025/08/01，2025/08/03，2025/09/02，2025/09/19，2025/10/10，2025/11/12，2025/11/26，2025/12/6，2026/1/9，2026/1/29</t>
         </is>
       </c>
       <c r="F277" t="inlineStr"/>
@@ -10718,7 +10718,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>2025/04/04，2026/1/28</t>
+          <t>2025/04/04，2026/1/29</t>
         </is>
       </c>
       <c r="F283" t="inlineStr"/>
@@ -11453,7 +11453,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>2025/04/07，2025/04/24，2025/05/03，2025/05/23，2025/06/07，2025/06/12，2025/06/23，2025/06/29，2025/07/15，2025/07/25，2025/09/24，2025/10/18，2025/11/12，2025/11/24，2025/12/23，2026/1/28</t>
+          <t>2025/04/07，2025/04/24，2025/05/03，2025/05/23，2025/06/07，2025/06/12，2025/06/23，2025/06/29，2025/07/15，2025/07/25，2025/09/24，2025/10/18，2025/11/12，2025/11/24，2025/12/23，2026/1/29</t>
         </is>
       </c>
       <c r="F304" t="inlineStr"/>
@@ -12103,7 +12103,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21，2026/1/28</t>
+          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21，2026/1/29</t>
         </is>
       </c>
       <c r="F322" t="inlineStr"/>
@@ -13866,7 +13866,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>2025/04/20，2025/04/27，2025/05/05，2025/05/09，2025/05/18，2025/06/07，2025/06/13，2025/06/21，2025/07/05，2025/07/15，2025/07/25，2025/08/08，2025/08/26，2025/08/28，2025/09/14，2025/09/30，2025/10/03，2025/10/24，2025/10/31，2025/11/9，2025/11/26，2025/12/5，2025/12/6，2026/1/1，2026/1/28</t>
+          <t>2025/04/20，2025/04/27，2025/05/05，2025/05/09，2025/05/18，2025/06/07，2025/06/13，2025/06/21，2025/07/05，2025/07/15，2025/07/25，2025/08/08，2025/08/26，2025/08/28，2025/09/14，2025/09/30，2025/10/03，2025/10/24，2025/10/31，2025/11/9，2025/11/26，2025/12/5，2025/12/6，2026/1/1，2026/1/29</t>
         </is>
       </c>
       <c r="F371" t="inlineStr"/>
@@ -14936,7 +14936,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24，2026/1/28</t>
+          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24，2026/1/29</t>
         </is>
       </c>
       <c r="F401" t="inlineStr"/>
@@ -22771,7 +22771,7 @@
       </c>
       <c r="E622" t="inlineStr">
         <is>
-          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9，2026/1/28</t>
+          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9，2026/1/29</t>
         </is>
       </c>
       <c r="F622" t="inlineStr"/>
@@ -25518,7 +25518,7 @@
       </c>
       <c r="E699" t="inlineStr">
         <is>
-          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26，2026/1/28</t>
+          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26，2026/1/29</t>
         </is>
       </c>
       <c r="F699" t="inlineStr"/>
@@ -27619,7 +27619,7 @@
       </c>
       <c r="E758" t="inlineStr">
         <is>
-          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/28</t>
+          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/29</t>
         </is>
       </c>
       <c r="F758" t="inlineStr"/>
@@ -27903,7 +27903,7 @@
       </c>
       <c r="E766" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23，2026/1/28</t>
+          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23，2026/1/29</t>
         </is>
       </c>
       <c r="F766" t="inlineStr"/>
@@ -28351,7 +28351,7 @@
       </c>
       <c r="E778" t="inlineStr">
         <is>
-          <t>2026/1/15，2026/1/28</t>
+          <t>2026/1/15，2026/1/29</t>
         </is>
       </c>
       <c r="F778" t="inlineStr"/>
@@ -28744,7 +28744,7 @@
       </c>
       <c r="E789" t="inlineStr">
         <is>
-          <t>2026/1/28</t>
+          <t>2026/1/29</t>
         </is>
       </c>
       <c r="F789" t="inlineStr"/>

</xml_diff>

<commit_message>
Update song list to Jan 30, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I789"/>
+  <dimension ref="A1:I790"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,7 +538,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025/03/01，2025/03/15，2025/04/01，2025/04/15，2025/04/26，2025/05/09，2025/05/30，2025/06/08，2025/07/05，2025/07/11，2025/08/13，2025/09/17，2025/09/02，2025/09/07，2025/09/19，2025/10/01，2025/10/09，2025/10/16，2025/10/24，2025/10/30，2025/11/9，2025/11/14，2025/12/24，2025/12/26，2026/1/16，2026/1/24，2026/1/28</t>
+          <t>2025/03/01，2025/03/15，2025/04/01，2025/04/15，2025/04/26，2025/05/09，2025/05/30，2025/06/08，2025/07/05，2025/07/11，2025/08/13，2025/09/17，2025/09/02，2025/09/07，2025/09/19，2025/10/01，2025/10/09，2025/10/16，2025/10/24，2025/10/30，2025/11/9，2025/11/14，2025/12/24，2025/12/26，2026/1/16，2026/1/24，2026/1/28，2026/1/30</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>28</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/04/07，2025/05/29，2025/06/06，2025/06/19，2025/06/26，2025/07/10，2025/07/11，2025/07/14，2025/08/02，2025/09/03，2025/09/26，2025/10/03，2025/11/9，2025/11/24，2025/11/26，2026/1/5</t>
+          <t>2025/03/04，2025/04/07，2025/05/29，2025/06/06，2025/06/19，2025/06/26，2025/07/10，2025/07/11，2025/07/14，2025/08/02，2025/09/03，2025/09/26，2025/10/03，2025/11/9，2025/11/24，2025/11/26，2026/1/5，2026/1/30</t>
         </is>
       </c>
       <c r="F26" t="inlineStr"/>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/05/01，2025/05/09，2025/05/26，2025/06/17，2025/06/20，2025/07/13，2025/09/12，2025/09/26，2025/10/11，2026/1/12</t>
+          <t>2025/03/07，2025/05/01，2025/05/09，2025/05/26，2025/06/17，2025/06/20，2025/07/13，2025/09/12，2025/09/26，2025/10/11，2026/1/12，2026/1/30</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -2931,10 +2931,14 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr"/>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>BV1MQKPzdEA5</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4784,7 +4788,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/03/28，2025/04/18，2025/09/20，2025/10/12，2025/10/22，2026/1/2</t>
+          <t>2025/03/14，2025/03/28，2025/04/18，2025/09/20，2025/10/12，2025/10/22，2026/1/2，2026/1/30</t>
         </is>
       </c>
       <c r="F117" t="inlineStr"/>
@@ -4795,10 +4799,14 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>BV1sv4gzWELe</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5605,7 +5613,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2025/03/19，2025/04/07，2025/04/21，2025/05/01，2025/05/10，2025/05/27，2025/06/09，2025/06/23，2025/06/26，2025/07/03，2025/09/15，2025/09/28，2025/10/01，2025/10/17，2026/1/3，2026/1/5</t>
+          <t>2025/03/19，2025/04/07，2025/04/21，2025/05/01，2025/05/10，2025/05/27，2025/06/09，2025/06/23，2025/06/26，2025/07/03，2025/09/15，2025/09/28，2025/10/01，2025/10/17，2026/1/3，2026/1/5，2026/1/30</t>
         </is>
       </c>
       <c r="F140" t="inlineStr"/>
@@ -5616,7 +5624,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -10648,7 +10656,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>2025/04/04，2025/05/12，2025/05/18，2025/06/20，2025/07/05，2025/07/14，2025/12/23</t>
+          <t>2025/04/04，2025/05/12，2025/05/18，2025/06/20，2025/07/05，2025/07/14，2025/12/23，2026/1/30</t>
         </is>
       </c>
       <c r="F281" t="inlineStr"/>
@@ -10659,10 +10667,14 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I281" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>BV1zgKNzkEV1</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -16173,7 +16185,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>2025/05/12，2025/05/22，2025/05/25，2025/07/20，2025/09/12，2026/1/15，2026/1/24</t>
+          <t>2025/05/12，2025/05/22，2025/05/25，2025/07/20，2025/09/12，2026/1/15，2026/1/24，2026/1/30</t>
         </is>
       </c>
       <c r="F436" t="inlineStr"/>
@@ -16184,10 +16196,14 @@
       </c>
       <c r="H436" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I436" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>BV12U6zBWEfw</t>
+        </is>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
@@ -20997,7 +21013,7 @@
       </c>
       <c r="E572" t="inlineStr">
         <is>
-          <t>2025/07/07，2025/07/31，2025/09/11，2025/10/11，2025/11/7，2025/11/12，2025/12/9，2026/1/14</t>
+          <t>2025/07/07，2025/07/31，2025/09/11，2025/10/11，2025/11/7，2025/11/12，2025/12/9，2026/1/14，2026/1/30</t>
         </is>
       </c>
       <c r="F572" t="inlineStr"/>
@@ -21008,10 +21024,14 @@
       </c>
       <c r="H572" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I572" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I572" t="inlineStr">
+        <is>
+          <t>BV1FCrWBiE7J</t>
+        </is>
+      </c>
     </row>
     <row r="573">
       <c r="A573" t="inlineStr">
@@ -22055,7 +22075,7 @@
       </c>
       <c r="E602" t="inlineStr">
         <is>
-          <t>2025/07/26，2025/09/24，2025/10/28，2025/11/12，2025/12/16，2026/1/14</t>
+          <t>2025/07/26，2025/09/24，2025/10/28，2025/11/12，2025/12/16，2026/1/14，2026/1/30</t>
         </is>
       </c>
       <c r="F602" t="inlineStr"/>
@@ -22066,10 +22086,14 @@
       </c>
       <c r="H602" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I602" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I602" t="inlineStr">
+        <is>
+          <t>BV146rrBaERP</t>
+        </is>
+      </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
@@ -26693,7 +26717,7 @@
       </c>
       <c r="E732" t="inlineStr">
         <is>
-          <t>2025/11/12，2025/11/14，2025/11/24，2025/12/6，2025/12/12，2025/12/26，2026/1/5</t>
+          <t>2025/11/12，2025/11/14，2025/11/24，2025/12/6，2025/12/12，2025/12/26，2026/1/5，2026/1/30</t>
         </is>
       </c>
       <c r="F732" t="inlineStr"/>
@@ -26704,7 +26728,7 @@
       </c>
       <c r="H732" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I732" t="inlineStr">
@@ -28713,7 +28737,7 @@
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25</t>
+          <t>2026/1/25，2026/1/30</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
@@ -28724,7 +28748,7 @@
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I788" t="inlineStr"/>
@@ -28763,6 +28787,37 @@
           <t>BV1Xx6cBRE14</t>
         </is>
       </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr"/>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Long Live</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr"/>
+      <c r="D790" t="inlineStr">
+        <is>
+          <t>Taylor Swift</t>
+        </is>
+      </c>
+      <c r="E790" t="inlineStr">
+        <is>
+          <t>2026/1/30</t>
+        </is>
+      </c>
+      <c r="F790" t="inlineStr"/>
+      <c r="G790" t="inlineStr">
+        <is>
+          <t>英语</t>
+        </is>
+      </c>
+      <c r="H790" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I790" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed an error in the song list
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -13220,7 +13220,11 @@
           <t>扉をあけて</t>
         </is>
       </c>
-      <c r="C353" t="inlineStr"/>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>打开心扉/魔法少女小樱</t>
+        </is>
+      </c>
       <c r="D353" t="inlineStr">
         <is>
           <t>ANZA</t>
@@ -13242,7 +13246,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I353" t="inlineStr"/>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>BV1t87rzREqq</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -13255,11 +13263,7 @@
           <t>安静了</t>
         </is>
       </c>
-      <c r="C354" t="inlineStr">
-        <is>
-          <t>打开心扉/魔法少女小樱</t>
-        </is>
-      </c>
+      <c r="C354" t="inlineStr"/>
       <c r="D354" t="inlineStr">
         <is>
           <t>S.H.E</t>

</xml_diff>

<commit_message>
Update song list to Jan 31, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -8341,7 +8341,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>2025/03/28，2025/04/22，2025/05/20，2025/06/27，2025/09/12，2025/11/9，2025/11/14，2025/12/9</t>
+          <t>2025/03/28，2025/04/22，2025/05/20，2025/06/27，2025/09/12，2025/11/9，2025/11/14，2025/12/9，2026/1/31</t>
         </is>
       </c>
       <c r="F216" t="inlineStr"/>
@@ -8352,10 +8352,14 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I216" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>BV1AzJhzdE3s</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -28192,7 +28196,7 @@
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23</t>
+          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31</t>
         </is>
       </c>
       <c r="F773" t="inlineStr"/>
@@ -28203,7 +28207,7 @@
       </c>
       <c r="H773" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I773" t="inlineStr">

</xml_diff>

<commit_message>
Update song list to Feb 2, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I790"/>
+  <dimension ref="A1:I791"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,7 +698,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025/03/02，2025/03/14，2025/03/28，2025/04/17，2025/04/25，2025/05/12，2025/05/12，2025/05/18，2025/05/29，2025/06/02，2025/06/05，2025/06/12，2025/06/27，2025/07/10，2025/08/04，2025/08/08，2025/08/21，2025/08/28，2025/09/10，2025/09/22，2025/09/30，2025/10/12，2025/11/17，2025/12/2，2025/12/31</t>
+          <t>2025/03/02，2025/03/14，2025/03/28，2025/04/17，2025/04/25，2025/05/12，2025/05/12，2025/05/18，2025/05/29，2025/06/02，2025/06/05，2025/06/12，2025/06/27，2025/07/10，2025/08/04，2025/08/08，2025/08/21，2025/08/28，2025/09/10，2025/09/22，2025/09/30，2025/10/12，2025/11/17，2025/12/2，2025/12/31，2026/2/2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/01，2025/05/08，2025/05/26，2025/06/05，2025/06/23，2025/06/26，2025/07/03，2025/07/20，2025/07/26，2025/08/03，2025/08/12，2025/08/30，2025/09/21，2025/09/29，2025/11/9，2025/11/12，2025/11/27，2025/12/4，2025/12/28，2026/1/22</t>
+          <t>2025/03/04，2025/05/01，2025/05/08，2025/05/26，2025/06/05，2025/06/23，2025/06/26，2025/07/03，2025/07/20，2025/07/26，2025/08/03，2025/08/12，2025/08/30，2025/09/21，2025/09/29，2025/11/9，2025/11/12，2025/11/27，2025/12/4，2025/12/28，2026/1/22，2026/2/2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2807,7 +2807,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/03/24，2025/04/06，2025/04/21，2025/04/28，2025/05/08，2025/05/20，2025/06/08，2025/07/08，2025/07/28，2025/09/24，2025/09/30，2025/11/18，2025/12/24</t>
+          <t>2025/03/09，2025/03/24，2025/04/06，2025/04/21，2025/04/28，2025/05/08，2025/05/20，2025/06/08，2025/07/08，2025/07/28，2025/09/24，2025/09/30，2025/11/18，2025/12/24，2026/2/2</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -3040,10 +3040,14 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I68" t="inlineStr"/>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>BV1Qky3BbEbV</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3138,7 +3142,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/03/14，2025/04/07，2025/04/15，2025/04/27，2025/05/12，2025/05/27，2025/06/05，2025/06/08，2025/07/20，2025/08/01，2025/09/21，2025/09/28，2025/10/07，2025/10/18，2025/10/24，2025/11/10，2025/12/1，2026/1/16</t>
+          <t>2025/03/09，2025/03/14，2025/04/07，2025/04/15，2025/04/27，2025/05/12，2025/05/27，2025/06/05，2025/06/08，2025/07/20，2025/08/01，2025/09/21，2025/09/28，2025/10/07，2025/10/18，2025/10/24，2025/11/10，2025/12/1，2026/1/16，2026/2/2</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -3149,10 +3153,14 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr"/>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>BV1bVqVBkEJz</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4286,7 +4294,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/02，2025/05/12，2025/05/23，2025/06/26，2025/07/08，2025/07/31，2025/08/22，2025/09/02，2025/09/15，2025/10/10，2025/11/3</t>
+          <t>2025/03/14，2025/04/02，2025/05/12，2025/05/23，2025/06/26，2025/07/08，2025/07/31，2025/08/22，2025/09/02，2025/09/15，2025/10/10，2025/11/3，2026/2/2</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -4297,10 +4305,14 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I103" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>BV1KaauzNE4s</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5539,7 +5551,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>2025/03/18，2025/03/25，2025/04/02，2025/04/17，2025/05/01，2025/05/08，2025/05/10，2025/05/24，2025/05/29，2025/06/23，2025/06/27，2025/07/08，2025/07/28，2025/08/03，2025/09/08，2025/09/22，2025/10/03，2025/10/11，2025/10/16，2025/10/24，2025/11/18，2025/12/2，2025/12/17，2026/1/9，2026/1/15</t>
+          <t>2025/03/18，2025/03/25，2025/04/02，2025/04/17，2025/05/01，2025/05/08，2025/05/10，2025/05/24，2025/05/29，2025/06/23，2025/06/27，2025/07/08，2025/07/28，2025/08/03，2025/09/08，2025/09/22，2025/10/03，2025/10/11，2025/10/16，2025/10/24，2025/11/18，2025/12/2，2025/12/17，2026/1/9，2026/1/15，2026/2/2</t>
         </is>
       </c>
       <c r="F138" t="inlineStr"/>
@@ -5550,7 +5562,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -5761,7 +5773,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>2025/03/19，2025/04/08，2025/04/18，2025/05/12，2025/05/23，2025/06/27，2025/07/24，2025/08/28，2025/10/11，2025/10/31，2025/11/24，2025/12/19</t>
+          <t>2025/03/19，2025/04/08，2025/04/18，2025/05/12，2025/05/23，2025/06/27，2025/07/24，2025/08/28，2025/10/11，2025/10/31，2025/11/24，2025/12/19，2026/2/2</t>
         </is>
       </c>
       <c r="F144" t="inlineStr"/>
@@ -5772,10 +5784,14 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I144" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>BV1GTK6zaEPD</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6057,7 +6073,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16</t>
+          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16，2026/2/2</t>
         </is>
       </c>
       <c r="F152" t="inlineStr"/>
@@ -6068,10 +6084,14 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="I152" t="inlineStr"/>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>BV1gHpBzAEnJ</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -8306,7 +8326,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>2025/03/27，2025/05/06，2025/05/16，2025/06/10，2025/07/03，2025/07/13，2025/08/22，2025/10/05，2025/10/23，2025/11/10，2026/1/16</t>
+          <t>2025/03/27，2025/05/06，2025/05/16，2025/06/10，2025/07/03，2025/07/13，2025/08/22，2025/10/05，2025/10/23，2025/11/10，2026/1/16，2026/2/2</t>
         </is>
       </c>
       <c r="F215" t="inlineStr"/>
@@ -8317,10 +8337,14 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="I215" t="inlineStr"/>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>BV1yYMVz2E5E</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -9882,7 +9906,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5</t>
+          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5，2026/2/2</t>
         </is>
       </c>
       <c r="F259" t="inlineStr"/>
@@ -9893,10 +9917,14 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I259" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>BV1QbqABDEAJ</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -13999,7 +14027,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>2025/04/20</t>
+          <t>2025/04/20，2026/2/2</t>
         </is>
       </c>
       <c r="F374" t="inlineStr"/>
@@ -14010,10 +14038,14 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I374" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>BV1jkEuznE5L</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -14886,7 +14918,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>2025/04/26，2025/05/02，2025/07/23，2025/09/19，2025/11/21</t>
+          <t>2025/04/26，2025/05/02，2025/07/23，2025/09/19，2025/11/21，2026/2/2</t>
         </is>
       </c>
       <c r="F399" t="inlineStr"/>
@@ -14897,10 +14929,14 @@
       </c>
       <c r="H399" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I399" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>BV1LzU7B8EJn</t>
+        </is>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -15060,12 +15096,12 @@
       <c r="C404" t="inlineStr"/>
       <c r="D404" t="inlineStr">
         <is>
-          <t>汪苏泷/单依纯</t>
+          <t>戚薇</t>
         </is>
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>2025/04/27，2025/07/13，2025/09/12，2025/10/09，2026/1/22</t>
+          <t>2025/04/27，2025/07/13，2025/09/12，2025/10/09，2026/1/22，2026/2/2</t>
         </is>
       </c>
       <c r="F404" t="inlineStr"/>
@@ -15076,10 +15112,14 @@
       </c>
       <c r="H404" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I404" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>BV1K9zcBCE5z</t>
+        </is>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -16302,7 +16342,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>2025/05/15，2025/06/13，2025/06/23，2025/07/18，2025/08/02，2025/09/04，2025/09/15，2025/10/03，2025/10/28，2025/11/9，2025/11/14，2025/12/5</t>
+          <t>2025/05/15，2025/06/13，2025/06/23，2025/07/18，2025/08/02，2025/09/04，2025/09/15，2025/10/03，2025/10/28，2025/11/9，2025/11/14，2025/12/5，2026/2/2</t>
         </is>
       </c>
       <c r="F439" t="inlineStr"/>
@@ -16313,10 +16353,14 @@
       </c>
       <c r="H439" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I439" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>BV1LXE1zJEVV</t>
+        </is>
+      </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
@@ -17002,7 +17046,11 @@
           <t>たばこ</t>
         </is>
       </c>
-      <c r="C459" t="inlineStr"/>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>烟草</t>
+        </is>
+      </c>
       <c r="D459" t="inlineStr">
         <is>
           <t>コレサワ</t>
@@ -17010,7 +17058,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>2025/05/22，2025/05/25，2025/05/31，2025/06/03，2025/06/10，2025/06/13，2025/06/23，2025/07/23，2025/07/24，2025/07/27，2025/08/22，2025/09/06，2025/10/28，2025/10/30</t>
+          <t>2025/05/22，2025/05/25，2025/05/31，2025/06/03，2025/06/10，2025/06/13，2025/06/23，2025/07/23，2025/07/24，2025/07/27，2025/08/22，2025/09/06，2025/10/28，2025/10/30，2026/2/2</t>
         </is>
       </c>
       <c r="F459" t="inlineStr"/>
@@ -17021,10 +17069,14 @@
       </c>
       <c r="H459" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I459" t="inlineStr"/>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I459" t="inlineStr">
+        <is>
+          <t>BV1RDMVzNEXV</t>
+        </is>
+      </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
@@ -18360,7 +18412,7 @@
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t>2025/06/01，2026/1/23</t>
+          <t>2025/06/01，2026/1/23，2026/2/2</t>
         </is>
       </c>
       <c r="F497" t="inlineStr"/>
@@ -18371,10 +18423,14 @@
       </c>
       <c r="H497" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I497" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>BV1VuzuB1EQf</t>
+        </is>
+      </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
@@ -18819,7 +18875,7 @@
       </c>
       <c r="E510" t="inlineStr">
         <is>
-          <t>2025/06/08，2025/06/13，2025/06/16，2025/06/28，2025/07/18，2025/07/29，2025/08/18，2025/09/03，2025/09/11，2025/09/30，2025/10/05，2025/10/30，2025/11/17，2025/12/24</t>
+          <t>2025/06/08，2025/06/13，2025/06/16，2025/06/28，2025/07/18，2025/07/29，2025/08/18，2025/09/03，2025/09/11，2025/09/30，2025/10/05，2025/10/30，2025/11/17，2025/12/24，2026/2/2</t>
         </is>
       </c>
       <c r="F510" t="inlineStr"/>
@@ -18830,10 +18886,14 @@
       </c>
       <c r="H510" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I510" t="inlineStr"/>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>BV1ArTRzbEkx</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
@@ -19558,7 +19618,7 @@
       </c>
       <c r="E531" t="inlineStr">
         <is>
-          <t>2025/06/19，2025/07/14，2025/07/17，2025/07/28，2025/08/03，2025/08/08，2025/08/22，2025/09/17，2025/09/26，2025/09/30，2025/10/12，2025/10/16，2025/11/7，2025/11/21，2025/12/2，2025/12/17，2026/1/1，2026/1/5，2026/1/14，2026/1/22，2026/1/24</t>
+          <t>2025/06/19，2025/07/14，2025/07/17，2025/07/28，2025/08/03，2025/08/08，2025/08/22，2025/09/17，2025/09/26，2025/09/30，2025/10/12，2025/10/16，2025/11/7，2025/11/21，2025/12/2，2025/12/17，2026/1/1，2026/1/5，2026/1/14，2026/1/22，2026/1/24，2026/2/2</t>
         </is>
       </c>
       <c r="F531" t="inlineStr"/>
@@ -19569,7 +19629,7 @@
       </c>
       <c r="H531" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="I531" t="inlineStr">
@@ -22472,7 +22532,7 @@
       </c>
       <c r="E613" t="inlineStr">
         <is>
-          <t>2025/08/09，2025/08/10，2025/08/13，2025/08/22，2025/08/25，2025/09/03，2025/09/05，2025/09/20，2025/09/29，2025/10/05，2025/10/22，2025/11/14，2025/12/2，2025/12/17，2026/1/14</t>
+          <t>2025/08/09，2025/08/10，2025/08/13，2025/08/22，2025/08/25，2025/09/03，2025/09/05，2025/09/20，2025/09/29，2025/10/05，2025/10/22，2025/11/14，2025/12/2，2025/12/17，2026/1/14，2026/2/2</t>
         </is>
       </c>
       <c r="F613" t="inlineStr"/>
@@ -22483,7 +22543,7 @@
       </c>
       <c r="H613" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I613" t="inlineStr">
@@ -22624,7 +22684,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>2025/08/21，2026/1/16</t>
+          <t>2025/08/21，2026/1/16，2026/2/2</t>
         </is>
       </c>
       <c r="F617" t="inlineStr"/>
@@ -22635,7 +22695,7 @@
       </c>
       <c r="H617" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I617" t="inlineStr"/>
@@ -27577,7 +27637,7 @@
       </c>
       <c r="E756" t="inlineStr">
         <is>
-          <t>2025/12/9</t>
+          <t>2025/12/9，2026/2/2</t>
         </is>
       </c>
       <c r="F756" t="inlineStr"/>
@@ -27588,7 +27648,7 @@
       </c>
       <c r="H756" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I756" t="inlineStr"/>
@@ -28597,7 +28657,7 @@
       </c>
       <c r="E784" t="inlineStr">
         <is>
-          <t>2026/1/24，2026/1/25，2026/1/26</t>
+          <t>2026/1/24，2026/1/25，2026/1/26，2026/2/2</t>
         </is>
       </c>
       <c r="F784" t="inlineStr"/>
@@ -28608,7 +28668,7 @@
       </c>
       <c r="H784" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I784" t="inlineStr">
@@ -28745,7 +28805,7 @@
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/1/30</t>
+          <t>2026/1/25，2026/1/30，2026/2/2</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
@@ -28756,10 +28816,14 @@
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I788" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I788" t="inlineStr">
+        <is>
+          <t>BV1Dv6qBsEXr</t>
+        </is>
+      </c>
     </row>
     <row r="789">
       <c r="A789" t="inlineStr"/>
@@ -28826,6 +28890,41 @@
         </is>
       </c>
       <c r="I790" t="inlineStr"/>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr"/>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>身不由己</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr"/>
+      <c r="D791" t="inlineStr">
+        <is>
+          <t>大都会乐团</t>
+        </is>
+      </c>
+      <c r="E791" t="inlineStr">
+        <is>
+          <t>2026/2/2</t>
+        </is>
+      </c>
+      <c r="F791" t="inlineStr"/>
+      <c r="G791" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H791" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I791" t="inlineStr">
+        <is>
+          <t>BV1fxFMzqEDd</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 4, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -2328,7 +2328,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/04/13，2025/05/01，2025/06/15，2025/07/24，2025/08/30，2025/09/05，2025/10/09，2025/11/3，2025/12/12</t>
+          <t>2025/03/06，2025/04/13，2025/05/01，2025/06/15，2025/07/24，2025/08/30，2025/09/05，2025/10/09，2025/11/3，2025/12/12，2026/2/4</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
@@ -3680,10 +3680,14 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>주세요 (Give Me Your)</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr"/>
+          <t>주세요</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Give Me Your</t>
+        </is>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t>(G)I-DLE</t>
@@ -3691,7 +3695,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025/03/12，2025/04/13，2025/05/01，2025/05/06，2025/05/24，2025/06/09，2025/06/24，2025/07/08，2025/08/19，2025/08/16，2025/09/08，2025/10/07，2025/10/28，2025/11/18，2025/12/11，2026/1/14</t>
+          <t>2025/03/12，2025/04/13，2025/05/01，2025/05/06，2025/05/24，2025/06/09，2025/06/24，2025/07/08，2025/08/19，2025/08/16，2025/09/08，2025/10/07，2025/10/28，2025/11/18，2025/12/11，2026/1/14，2026/2/4</t>
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
@@ -3702,7 +3706,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I86" t="inlineStr"/>
@@ -11610,7 +11614,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>2025/04/07，2025/04/17，2025/05/08，2025/05/20，2025/05/30，2025/06/16，2025/08/29，2025/09/12，2025/10/09，2025/10/16，2025/11/18</t>
+          <t>2025/04/07，2025/04/17，2025/05/08，2025/05/20，2025/05/30，2025/06/16，2025/08/29，2025/09/12，2025/10/09，2025/10/16，2025/11/18，2026/2/4</t>
         </is>
       </c>
       <c r="F307" t="inlineStr"/>
@@ -11621,7 +11625,7 @@
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I307" t="inlineStr"/>

</xml_diff>

<commit_message>
Update song list to Feb 5, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -2342,7 +2342,11 @@
           <t>11</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>BV1wtmoB7ERp</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3709,7 +3713,11 @@
           <t>17</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>BV1EpmjBbEte</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6412,7 +6420,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/03/29，2025/05/09，2025/05/18，2025/05/22，2025/05/26，2025/06/13，2025/06/23，2025/07/07，2025/07/14，2025/07/18，2025/08/07，2025/08/19，2025/08/28，2025/09/12，2025/09/28，2025/10/09，2025/12/26，2026/1/5，2026/1/24</t>
+          <t>2025/03/20，2025/03/29，2025/05/09，2025/05/18，2025/05/22，2025/05/26，2025/06/13，2025/06/23，2025/07/07，2025/07/14，2025/07/18，2025/08/07，2025/08/19，2025/08/28，2025/09/12，2025/09/28，2025/10/09，2025/12/26，2026/1/5，2026/1/24，2026/2/5</t>
         </is>
       </c>
       <c r="F161" t="inlineStr"/>
@@ -6423,7 +6431,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -11628,7 +11636,11 @@
           <t>12</t>
         </is>
       </c>
-      <c r="I307" t="inlineStr"/>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>BV1BYyVBVELL</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -23155,7 +23167,7 @@
       </c>
       <c r="E630" t="inlineStr">
         <is>
-          <t>2025/09/10，2025/09/22，2025/09/24，2025/10/23，2025/12/6，2026/1/24</t>
+          <t>2025/09/10，2025/09/22，2025/09/24，2025/10/23，2025/12/6，2026/1/24，2026/2/5</t>
         </is>
       </c>
       <c r="F630" t="inlineStr"/>
@@ -23166,7 +23178,7 @@
       </c>
       <c r="H630" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I630" t="inlineStr">
@@ -24648,12 +24660,12 @@
       <c r="C672" t="inlineStr"/>
       <c r="D672" t="inlineStr">
         <is>
-          <t>J.Sheon/街巷</t>
+          <t>J.Sheon</t>
         </is>
       </c>
       <c r="E672" t="inlineStr">
         <is>
-          <t>2025/09/24，2025/09/26，2025/09/28，2025/09/29，2025/10/01，2025/10/07，2025/10/10，2025/10/11，2025/10/17，2025/10/23，2025/10/28，2025/12/26</t>
+          <t>2025/09/24，2025/09/26，2025/09/28，2025/09/29，2025/10/01，2025/10/07，2025/10/10，2025/10/11，2025/10/17，2025/10/23，2025/10/28，2025/12/26，2026/2/5</t>
         </is>
       </c>
       <c r="F672" t="inlineStr"/>
@@ -24664,10 +24676,14 @@
       </c>
       <c r="H672" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I672" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I672" t="inlineStr">
+        <is>
+          <t>BV1szBrBHEVt</t>
+        </is>
+      </c>
     </row>
     <row r="673">
       <c r="A673" t="inlineStr">
@@ -27676,7 +27692,7 @@
       </c>
       <c r="E757" t="inlineStr">
         <is>
-          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23</t>
+          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5</t>
         </is>
       </c>
       <c r="F757" t="inlineStr"/>
@@ -27687,7 +27703,7 @@
       </c>
       <c r="H757" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I757" t="inlineStr">
@@ -28591,7 +28607,7 @@
       </c>
       <c r="E782" t="inlineStr">
         <is>
-          <t>2026/1/23，2026/1/25</t>
+          <t>2026/1/23，2026/1/25，2026/2/5</t>
         </is>
       </c>
       <c r="F782" t="inlineStr"/>
@@ -28602,7 +28618,7 @@
       </c>
       <c r="H782" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I782" t="inlineStr"/>

</xml_diff>

<commit_message>
Update song list to Feb 8, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I793"/>
+  <dimension ref="A1:I796"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/17，2025/04/25，2025/06/23，2025/08/30，2025/09/12，2025/09/15，2025/11/19</t>
+          <t>2025/03/14，2025/04/17，2025/04/25，2025/06/23，2025/08/30，2025/09/12，2025/09/15，2025/11/19，2026/2/8</t>
         </is>
       </c>
       <c r="F105" t="inlineStr"/>
@@ -4395,10 +4395,14 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>BV14uypBDERJ</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -9915,7 +9919,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/04/24，2025/05/12，2025/05/26，2025/06/23，2025/06/27，2025/07/20，2025/08/30，2025/09/15，2025/09/22，2025/10/07，2025/10/28，2025/11/26，2025/12/28</t>
+          <t>2025/04/01，2025/04/24，2025/05/12，2025/05/26，2025/06/23，2025/06/27，2025/07/20，2025/08/30，2025/09/15，2025/09/22，2025/10/07，2025/10/28，2025/11/26，2025/12/28，2026/2/8</t>
         </is>
       </c>
       <c r="F258" t="inlineStr"/>
@@ -9926,7 +9930,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
@@ -12666,7 +12670,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>2025/04/13，2025/05/26，2025/06/07，2025/06/21，2025/07/05，2025/08/21，2025/09/15，2025/10/23，2025/11/24，2025/12/23，2026/1/9</t>
+          <t>2025/04/13，2025/05/26，2025/06/07，2025/06/21，2025/07/05，2025/08/21，2025/09/15，2025/10/23，2025/11/24，2025/12/23，2026/1/9，2026/2/8</t>
         </is>
       </c>
       <c r="F335" t="inlineStr"/>
@@ -12677,10 +12681,14 @@
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="I335" t="inlineStr"/>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>BV1jEBuB1EAY</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -26390,7 +26398,7 @@
       </c>
       <c r="E719" t="inlineStr">
         <is>
-          <t>2025/10/28，2025/11/12，2025/12/19</t>
+          <t>2025/10/28，2025/11/12，2025/12/19，2026/2/8</t>
         </is>
       </c>
       <c r="F719" t="inlineStr"/>
@@ -26401,10 +26409,14 @@
       </c>
       <c r="H719" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I719" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>BV1bscPz1EEj</t>
+        </is>
+      </c>
     </row>
     <row r="720">
       <c r="A720" t="inlineStr">
@@ -28106,7 +28118,7 @@
       </c>
       <c r="E767" t="inlineStr">
         <is>
-          <t>2025/12/19</t>
+          <t>2025/12/19，2026/2/8</t>
         </is>
       </c>
       <c r="F767" t="inlineStr"/>
@@ -28117,10 +28129,14 @@
       </c>
       <c r="H767" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I767" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I767" t="inlineStr">
+        <is>
+          <t>BV1WVqrBLEc2</t>
+        </is>
+      </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
@@ -28768,7 +28784,7 @@
       </c>
       <c r="E785" t="inlineStr">
         <is>
-          <t>2026/1/24</t>
+          <t>2026/1/24，2026/2/8</t>
         </is>
       </c>
       <c r="F785" t="inlineStr"/>
@@ -28779,10 +28795,14 @@
       </c>
       <c r="H785" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I785" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I785" t="inlineStr">
+        <is>
+          <t>BV1zPz1BRExW</t>
+        </is>
+      </c>
     </row>
     <row r="786">
       <c r="A786" t="inlineStr">
@@ -28877,7 +28897,7 @@
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/1/30，2026/2/2</t>
+          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
@@ -28888,7 +28908,7 @@
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I788" t="inlineStr">
@@ -29063,6 +29083,103 @@
           <t>BV1wGF4zFEBM</t>
         </is>
       </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr"/>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>相亲相爱</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr"/>
+      <c r="D794" t="inlineStr">
+        <is>
+          <t>陈慧琳/张惠妹/孙楠/古淖文</t>
+        </is>
+      </c>
+      <c r="E794" t="inlineStr">
+        <is>
+          <t>2026/2/8</t>
+        </is>
+      </c>
+      <c r="F794" t="inlineStr"/>
+      <c r="G794" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H794" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I794" t="inlineStr"/>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr"/>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>混入人类计划</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr"/>
+      <c r="D795" t="inlineStr">
+        <is>
+          <t>ChiliChill</t>
+        </is>
+      </c>
+      <c r="E795" t="inlineStr">
+        <is>
+          <t>2026/2/8</t>
+        </is>
+      </c>
+      <c r="F795" t="inlineStr"/>
+      <c r="G795" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H795" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I795" t="inlineStr">
+        <is>
+          <t>BV1JncczQEuJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr"/>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>纸飞机</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr"/>
+      <c r="D796" t="inlineStr">
+        <is>
+          <t>鸣潮先约电台/飞行雪绒</t>
+        </is>
+      </c>
+      <c r="E796" t="inlineStr">
+        <is>
+          <t>2026/2/8</t>
+        </is>
+      </c>
+      <c r="F796" t="inlineStr"/>
+      <c r="G796" t="inlineStr">
+        <is>
+          <t>英语</t>
+        </is>
+      </c>
+      <c r="H796" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I796" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 9, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I796"/>
+  <dimension ref="A1:I797"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025/03/02，2025/03/25，2025/03/28，2025/04/17，2025/05/03，2025/05/09，2025/05/16，2025/05/30，2025/06/14，2025/06/19，2025/07/05，2025/07/18，2025/08/21，2025/08/25，2025/09/05，2025/09/22，2025/09/26，2026/1/19，2026/1/21</t>
+          <t>2025/03/02，2025/03/25，2025/03/28，2025/04/17，2025/05/03，2025/05/09，2025/05/16，2025/05/30，2025/06/14，2025/06/19，2025/07/05，2025/07/18，2025/08/21，2025/08/25，2025/09/05，2025/09/22，2025/09/26，2026/1/19，2026/1/21，2026/2/9</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/25，2026/1/29</t>
+          <t>2025/03/04，2025/05/25，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/04/04，2025/04/28，2025/07/08，2025/07/21，2025/08/18</t>
+          <t>2025/03/09，2025/04/04，2025/04/28，2025/07/08，2025/07/21，2025/08/18，2026/2/9</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -3301,10 +3301,14 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>BV1GUGwzrE6o</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3539,7 +3543,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025/03/12，2025/04/11，2025/05/04，2025/05/18，2025/06/06，2025/06/27，2025/07/15，2025/08/16，2025/09/11，2025/09/18，2025/10/05，2025/12/2</t>
+          <t>2025/03/12，2025/04/11，2025/05/04，2025/05/18，2025/06/06，2025/06/27，2025/07/15，2025/08/16，2025/09/11，2025/09/18，2025/10/05，2025/12/2，2026/2/9</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -3550,10 +3554,14 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>BV12BWNzNE2b</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5252,7 +5260,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29</t>
+          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F129" t="inlineStr"/>
@@ -5263,7 +5271,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>35</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -6623,7 +6631,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>2025/03/21，2025/05/19，2025/06/13，2025/07/22，2025/07/23，2025/08/25，2025/09/12，2025/10/26，2025/12/17</t>
+          <t>2025/03/21，2025/05/19，2025/06/13，2025/07/22，2025/07/23，2025/08/25，2025/09/12，2025/10/26，2025/12/17，2026/2/9</t>
         </is>
       </c>
       <c r="F166" t="inlineStr"/>
@@ -6634,10 +6642,14 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I166" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>BV13AXCYLEaV</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -7366,7 +7378,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13，2026/1/29</t>
+          <t>2025/03/23，2025/03/28，2025/04/06，2025/05/15，2025/05/22，2025/05/29，2025/06/07，2025/06/09，2025/07/06，2025/07/15，2025/09/06，2025/09/14，2025/09/30，2025/11/13，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F187" t="inlineStr"/>
@@ -7377,7 +7389,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -9020,7 +9032,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>2025/03/29，2025/05/29，2025/06/17，2025/07/24，2025/08/16，2025/09/21，2025/10/30</t>
+          <t>2025/03/29，2025/05/29，2025/06/17，2025/07/24，2025/08/16，2025/09/21，2025/10/30，2026/2/9</t>
         </is>
       </c>
       <c r="F233" t="inlineStr"/>
@@ -9031,10 +9043,14 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I233" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>BV18bWAzeEFa</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -9168,7 +9184,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>2025/03/29，2025/08/22，2025/09/21，2025/10/20，2025/12/2</t>
+          <t>2025/03/29，2025/08/22，2025/09/21，2025/10/20，2025/12/2，2026/2/9</t>
         </is>
       </c>
       <c r="F237" t="inlineStr"/>
@@ -9179,10 +9195,14 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I237" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>BV1WFWAzWEug</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -9207,7 +9227,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>2025/03/29，2025/08/12，2025/10/20，2025/11/14，2025/12/2，2026/1/10</t>
+          <t>2025/03/29，2025/08/12，2025/10/20，2025/11/14，2025/12/2，2026/1/10，2026/2/9</t>
         </is>
       </c>
       <c r="F238" t="inlineStr"/>
@@ -9218,10 +9238,14 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I238" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>BV1KVWmzpEhZ</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -9382,7 +9406,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>2025/03/30，2025/04/24，2025/05/15，2025/05/29，2025/09/21，2025/09/27，2025/10/24，2026/1/5</t>
+          <t>2025/03/30，2025/04/24，2025/05/15，2025/05/29，2025/09/21，2025/09/27，2025/10/24，2026/1/5，2026/2/9</t>
         </is>
       </c>
       <c r="F243" t="inlineStr"/>
@@ -9393,10 +9417,14 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I243" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>BV1a7E1zVEhr</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -9958,7 +9986,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5，2026/2/2</t>
+          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5，2026/2/2，2026/2/9</t>
         </is>
       </c>
       <c r="F259" t="inlineStr"/>
@@ -9969,7 +9997,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
@@ -17593,7 +17621,7 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>2025/05/27，2025/05/29，2025/05/30，2025/05/31，2025/06/02，2025/06/03，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/11，2025/07/22，2025/08/21，2025/09/10，2025/09/26，2025/10/03，2025/10/11，2025/10/26，2025/11/7，2025/12/7，2025/12/23，2026/1/9，2026/1/24</t>
+          <t>2025/05/27，2025/05/29，2025/05/30，2025/05/31，2025/06/02，2025/06/03，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/11，2025/07/22，2025/08/21，2025/09/10，2025/09/26，2025/10/03，2025/10/11，2025/10/26，2025/11/7，2025/12/7，2025/12/23，2026/1/9，2026/1/24，2026/2/9</t>
         </is>
       </c>
       <c r="F472" t="inlineStr"/>
@@ -17604,7 +17632,7 @@
       </c>
       <c r="H472" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="I472" t="inlineStr">
@@ -20297,10 +20325,14 @@
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>2025/06/27，2025/09/08，2025/10/13，2025/10/16，2026/1/24</t>
-        </is>
-      </c>
-      <c r="F548" t="inlineStr"/>
+          <t>2025/06/27，2025/09/08，2025/10/13，2025/10/16，2026/1/24，2026/2/9</t>
+        </is>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>点歌大概率不唱</t>
+        </is>
+      </c>
       <c r="G548" t="inlineStr">
         <is>
           <t>华语</t>
@@ -20308,7 +20340,7 @@
       </c>
       <c r="H548" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I548" t="inlineStr">
@@ -22499,7 +22531,7 @@
       </c>
       <c r="E610" t="inlineStr">
         <is>
-          <t>2025/08/02，2025/10/12，2025/12/4，2026/1/9</t>
+          <t>2025/08/02，2025/10/12，2025/12/4，2026/1/9，2026/2/9</t>
         </is>
       </c>
       <c r="F610" t="inlineStr"/>
@@ -22510,10 +22542,14 @@
       </c>
       <c r="H610" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I610" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I610" t="inlineStr">
+        <is>
+          <t>BV1BV2LBXEVh</t>
+        </is>
+      </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
@@ -25690,7 +25726,7 @@
       </c>
       <c r="E699" t="inlineStr">
         <is>
-          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26，2026/1/29</t>
+          <t>2025/10/17，2025/10/24，2025/10/30，2025/11/14，2025/11/28，2025/12/12，2025/12/26，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F699" t="inlineStr"/>
@@ -25701,7 +25737,7 @@
       </c>
       <c r="H699" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I699" t="inlineStr"/>
@@ -26869,7 +26905,7 @@
       </c>
       <c r="E732" t="inlineStr">
         <is>
-          <t>2025/11/12，2025/11/14，2025/11/24，2025/12/6，2025/12/12，2025/12/26，2026/1/5，2026/1/30</t>
+          <t>2025/11/12，2025/11/14，2025/11/24，2025/12/6，2025/12/12，2025/12/26，2026/1/5，2026/1/30，2026/2/9</t>
         </is>
       </c>
       <c r="F732" t="inlineStr"/>
@@ -26880,7 +26916,7 @@
       </c>
       <c r="H732" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I732" t="inlineStr">
@@ -27795,7 +27831,7 @@
       </c>
       <c r="E758" t="inlineStr">
         <is>
-          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/29</t>
+          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F758" t="inlineStr"/>
@@ -27806,7 +27842,7 @@
       </c>
       <c r="H758" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I758" t="inlineStr">
@@ -28192,7 +28228,7 @@
       </c>
       <c r="E769" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25</t>
+          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25，2026/2/9</t>
         </is>
       </c>
       <c r="F769" t="inlineStr"/>
@@ -28203,7 +28239,7 @@
       </c>
       <c r="H769" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I769" t="inlineStr">
@@ -28309,7 +28345,7 @@
       </c>
       <c r="E772" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/19</t>
+          <t>2025/12/26，2026/1/19，2026/2/9</t>
         </is>
       </c>
       <c r="F772" t="inlineStr"/>
@@ -28320,10 +28356,14 @@
       </c>
       <c r="H772" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I772" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I772" t="inlineStr">
+        <is>
+          <t>BV1VUcuzvEaU</t>
+        </is>
+      </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
@@ -28453,7 +28493,7 @@
       </c>
       <c r="E776" t="inlineStr">
         <is>
-          <t>2025/12/27，2026/1/5，2026/1/6，2026/1/14，2026/1/23</t>
+          <t>2025/12/27，2026/1/5，2026/1/6，2026/1/14，2026/1/23，2026/2/9</t>
         </is>
       </c>
       <c r="F776" t="inlineStr"/>
@@ -28464,7 +28504,7 @@
       </c>
       <c r="H776" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I776" t="inlineStr">
@@ -28675,7 +28715,7 @@
       </c>
       <c r="E782" t="inlineStr">
         <is>
-          <t>2026/1/23，2026/1/25，2026/2/5</t>
+          <t>2026/1/23，2026/1/25，2026/2/5，2026/2/9</t>
         </is>
       </c>
       <c r="F782" t="inlineStr"/>
@@ -28686,7 +28726,7 @@
       </c>
       <c r="H782" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I782" t="inlineStr"/>
@@ -28998,7 +29038,7 @@
       </c>
       <c r="E791" t="inlineStr">
         <is>
-          <t>2026/2/2，2026/2/5</t>
+          <t>2026/2/2，2026/2/5，2026/2/9</t>
         </is>
       </c>
       <c r="F791" t="inlineStr"/>
@@ -29009,7 +29049,7 @@
       </c>
       <c r="H791" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I791" t="inlineStr">
@@ -29113,7 +29153,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I794" t="inlineStr"/>
+      <c r="I794" t="inlineStr">
+        <is>
+          <t>BV1U9cTzpEjm</t>
+        </is>
+      </c>
     </row>
     <row r="795">
       <c r="A795" t="inlineStr"/>
@@ -29130,7 +29174,7 @@
       </c>
       <c r="E795" t="inlineStr">
         <is>
-          <t>2026/2/8</t>
+          <t>2026/2/8，2026/2/9</t>
         </is>
       </c>
       <c r="F795" t="inlineStr"/>
@@ -29141,7 +29185,7 @@
       </c>
       <c r="H795" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I795" t="inlineStr">
@@ -29165,7 +29209,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8</t>
+          <t>2026/2/8，2026/2/9</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29176,10 +29220,45 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I796" t="inlineStr">
+        <is>
+          <t>BV1W4cuzSE8Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr"/>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>刻在我心底的名字</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr"/>
+      <c r="D797" t="inlineStr">
+        <is>
+          <t>卢广仲</t>
+        </is>
+      </c>
+      <c r="E797" t="inlineStr">
+        <is>
+          <t>2026/2/9</t>
+        </is>
+      </c>
+      <c r="F797" t="inlineStr"/>
+      <c r="G797" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H797" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I796" t="inlineStr"/>
+      <c r="I797" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed an error in statistical data
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -620,7 +620,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025/03/02，2025/03/25，2025/03/28，2025/04/17，2025/05/03，2025/05/09，2025/05/16，2025/05/30，2025/06/14，2025/06/19，2025/07/05，2025/07/18，2025/08/21，2025/08/25，2025/09/05，2025/09/22，2025/09/26，2026/1/19，2026/1/21，2026/2/9</t>
+          <t>2025/03/02，2025/03/25，2025/03/28，2025/04/17，2025/05/03，2025/05/09，2025/05/16，2025/05/30，2025/06/14，2025/06/19，2025/07/05，2025/07/18，2025/08/21，2025/08/25，2025/09/05，2025/09/22，2025/09/26，2026/1/19，2026/1/21</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/03/28，2025/04/19，2025/04/24，2025/05/03，2025/05/15，2025/05/16，2025/05/22，2025/05/30，2025/06/14，2025/06/19，2025/06/26，2025/07/18，2025/08/04，2025/09/10，2025/09/18，2025/10/03，2026/2/7</t>
+          <t>2025/03/06，2025/03/28，2025/04/19，2025/04/24，2025/05/03，2025/05/15，2025/05/16，2025/05/22，2025/05/30，2025/06/14，2025/06/19，2025/06/26，2025/07/18，2025/08/04，2025/09/10，2025/09/18，2025/10/03，2026/2/7，2026/2/9</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">

</xml_diff>

<commit_message>
Update song list to Feb 10, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025/03/01，2025/03/15，2025/04/01，2025/04/15，2025/04/26，2025/05/09，2025/05/30，2025/06/08，2025/07/05，2025/07/11，2025/08/13，2025/09/17，2025/09/02，2025/09/07，2025/09/19，2025/10/01，2025/10/09，2025/10/16，2025/10/24，2025/10/30，2025/11/9，2025/11/14，2025/12/24，2025/12/26，2026/1/16，2026/1/24，2026/1/28，2026/1/30</t>
+          <t>2025/03/01，2025/03/15，2025/04/01，2025/04/15，2025/04/26，2025/05/09，2025/05/30，2025/06/08，2025/07/05，2025/07/11，2025/08/13，2025/09/17，2025/09/02，2025/09/07，2025/09/19，2025/10/01，2025/10/09，2025/10/16，2025/10/24，2025/10/30，2025/11/9，2025/11/14，2025/12/24，2025/12/26，2026/1/16，2026/1/24，2026/1/28，2026/1/30，2026/2/10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>29</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025/03/03，2025/03/21，2025/04/17，2025/04/21，2025/05/12，2025/05/26，2025/05/30，2025/06/26，2025/07/07，2025/07/13，2025/07/26，2025/08/12，2025/08/22，2025/09/19，2025/10/03，2025/10/28，2025/11/9，2025/11/19，2025/12/16，2026/1/16，2026/1/28，2026/2/7</t>
+          <t>2025/03/03，2025/03/21，2025/04/17，2025/04/21，2025/05/12，2025/05/26，2025/05/30，2025/06/26，2025/07/07，2025/07/13，2025/07/26，2025/08/12，2025/08/22，2025/09/19，2025/10/03，2025/10/28，2025/11/9，2025/11/19，2025/12/16，2026/1/16，2026/1/28，2026/2/7，2026/2/10</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -752,7 +752,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/29</t>
+          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/29，2026/2/10</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -990,7 +990,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/25，2025/04/29，2025/05/13，2025/05/22，2025/05/26，2025/05/30，2025/06/08，2025/06/13，2025/06/20，2025/07/05，2025/07/14，2025/07/20，2025/08/01，2025/08/30，2025/09/12，2025/09/17，2025/09/02，2025/09/22，2025/09/24，2025/10/03，2025/10/12，2025/11/14，2025/11/21，2025/11/28，2025/12/17，2026/1/10，2026/1/22</t>
+          <t>2025/03/04，2025/03/25，2025/04/29，2025/05/13，2025/05/22，2025/05/26，2025/05/30，2025/06/08，2025/06/13，2025/06/20，2025/07/05，2025/07/14，2025/07/20，2025/08/01，2025/08/30，2025/09/12，2025/09/17，2025/09/02，2025/09/22，2025/09/24，2025/10/03，2025/10/12，2025/11/14，2025/11/21，2025/11/28，2025/12/17，2026/1/10，2026/1/22，2026/2/10</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>29</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/04，2025/04/12，2025/04/18，2025/04/24，2025/06/17，2025/06/19，2025/07/11，2025/07/18，2025/08/28，2025/09/05，2025/09/08，2025/09/27，2025/10/03，2025/12/11，2025/12/30，2026/1/21，2026/1/25</t>
+          <t>2025/03/07，2025/04/04，2025/04/12，2025/04/18，2025/04/24，2025/06/17，2025/06/19，2025/07/11，2025/07/18，2025/08/28，2025/09/05，2025/09/08，2025/09/27，2025/10/03，2025/12/11，2025/12/30，2026/1/21，2026/1/25，2026/2/10</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4108,7 +4108,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/03/14，2025/03/29，2025/04/19，2025/04/26，2025/05/09，2025/05/19，2025/05/22，2025/05/25，2025/07/03，2025/07/05，2025/07/28，2025/08/04，2025/08/21，2025/09/30，2025/11/14，2025/11/17</t>
+          <t>2025/03/13，2025/03/14，2025/03/29，2025/04/19，2025/04/26，2025/05/09，2025/05/19，2025/05/22，2025/05/25，2025/07/03，2025/07/05，2025/07/28，2025/08/04，2025/08/21，2025/09/30，2025/11/14，2025/11/17，2026/2/10</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -4119,10 +4119,14 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr"/>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>BV1zdrTBpETM</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5891,7 +5895,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>2025/03/19，2025/04/07，2025/04/17，2025/04/22，2025/05/22，2025/06/23，2025/07/09，2025/08/26，2025/09/28，2025/11/21，2025/12/4，2026/1/3</t>
+          <t>2025/03/19，2025/04/07，2025/04/17，2025/04/22，2025/05/22，2025/06/23，2025/07/09，2025/08/26，2025/09/28，2025/11/21，2025/12/4，2026/1/3，2026/2/10</t>
         </is>
       </c>
       <c r="F146" t="inlineStr"/>
@@ -5902,7 +5906,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -6269,7 +6273,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7</t>
+          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10</t>
         </is>
       </c>
       <c r="F156" t="inlineStr"/>
@@ -6280,7 +6284,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -11881,7 +11885,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>2025/04/08，2025/04/13，2025/04/22，2025/05/01，2025/05/22，2025/06/08，2025/06/29，2025/08/30，2025/09/15，2025/10/10，2025/11/9，2025/12/5，2025/12/19，2025/12/26，2026/1/10，2026/1/19</t>
+          <t>2025/04/08，2025/04/13，2025/04/22，2025/05/01，2025/05/22，2025/06/08，2025/06/29，2025/08/30，2025/09/15，2025/10/10，2025/11/9，2025/12/5，2025/12/19，2025/12/26，2026/1/10，2026/1/19，2026/2/10</t>
         </is>
       </c>
       <c r="F312" t="inlineStr"/>
@@ -11892,7 +11896,7 @@
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I312" t="inlineStr">
@@ -12235,7 +12239,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21，2026/1/29</t>
+          <t>2025/04/11，2025/05/25，2025/05/29，2025/06/28，2025/07/03，2025/08/13，2025/08/25，2025/09/12，2025/09/11，2025/09/28，2025/10/11，2025/10/30，2025/11/21，2026/1/29，2026/2/10</t>
         </is>
       </c>
       <c r="F322" t="inlineStr"/>
@@ -12246,7 +12250,7 @@
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
@@ -13753,7 +13757,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>2025/04/18，2025/05/18，2025/06/19，2025/07/15，2025/08/01，2025/09/17，2025/10/28，2025/11/13，2025/11/14</t>
+          <t>2025/04/18，2025/05/18，2025/06/19，2025/07/15，2025/08/01，2025/09/17，2025/10/28，2025/11/13，2025/11/14，2026/2/10</t>
         </is>
       </c>
       <c r="F364" t="inlineStr"/>
@@ -13764,10 +13768,14 @@
       </c>
       <c r="H364" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I364" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>BV1UgF9zLEPz</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -16512,7 +16520,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>2025/05/17，2025/05/31，2025/06/15，2025/07/23，2025/09/11，2026/1/1</t>
+          <t>2025/05/17，2025/05/31，2025/06/15，2025/07/23，2025/09/11，2026/1/1，2026/2/10</t>
         </is>
       </c>
       <c r="F441" t="inlineStr"/>
@@ -16523,10 +16531,14 @@
       </c>
       <c r="H441" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I441" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>BV1J67NzGEDg</t>
+        </is>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
@@ -18796,7 +18808,7 @@
       </c>
       <c r="E505" t="inlineStr">
         <is>
-          <t>2025/06/03，2025/09/20，2025/09/21，2025/09/24，2025/09/29，2025/10/10</t>
+          <t>2025/06/03，2025/09/20，2025/09/21，2025/09/24，2025/09/29，2025/10/10，2026/2/10</t>
         </is>
       </c>
       <c r="F505" t="inlineStr"/>
@@ -18807,10 +18819,14 @@
       </c>
       <c r="H505" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I505" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>BV18bJdzzEvN</t>
+        </is>
+      </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
@@ -19858,7 +19874,7 @@
       </c>
       <c r="E535" t="inlineStr">
         <is>
-          <t>2025/06/20，2025/06/23，2025/09/29，2026/1/9</t>
+          <t>2025/06/20，2025/06/23，2025/09/29，2026/1/9，2026/2/10</t>
         </is>
       </c>
       <c r="F535" t="inlineStr"/>
@@ -19869,10 +19885,14 @@
       </c>
       <c r="H535" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I535" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>BV1523azhEv6</t>
+        </is>
+      </c>
     </row>
     <row r="536">
       <c r="A536" t="inlineStr">
@@ -21784,7 +21804,7 @@
       </c>
       <c r="E589" t="inlineStr">
         <is>
-          <t>2025/07/15，2026/1/5，2026/1/10，2026/1/25</t>
+          <t>2025/07/15，2026/1/5，2026/1/10，2026/1/25，2026/2/10</t>
         </is>
       </c>
       <c r="F589" t="inlineStr"/>
@@ -21795,10 +21815,14 @@
       </c>
       <c r="H589" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I589" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I589" t="inlineStr">
+        <is>
+          <t>BV1yM6UBkE2q</t>
+        </is>
+      </c>
     </row>
     <row r="590">
       <c r="A590" t="inlineStr">
@@ -24364,7 +24388,7 @@
       </c>
       <c r="E661" t="inlineStr">
         <is>
-          <t>2025/09/21，2025/09/21，2025/09/22，2025/09/22，2025/09/24，2025/09/27，2025/09/29，2025/10/03，2025/10/05，2025/10/09，2025/10/18，2025/10/22，2025/10/26，2025/11/9，2025/11/19，2025/11/22，2025/11/28，2025/12/22，2026/1/5，2026/1/14，2026/1/22，2026/2/7</t>
+          <t>2025/09/21，2025/09/21，2025/09/22，2025/09/22，2025/09/24，2025/09/27，2025/09/29，2025/10/03，2025/10/05，2025/10/09，2025/10/18，2025/10/22，2025/10/26，2025/11/9，2025/11/19，2025/11/22，2025/11/28，2025/12/22，2026/1/5，2026/1/14，2026/1/22，2026/2/7，2026/2/10</t>
         </is>
       </c>
       <c r="F661" t="inlineStr"/>
@@ -24375,7 +24399,7 @@
       </c>
       <c r="H661" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I661" t="inlineStr">
@@ -26434,7 +26458,7 @@
       </c>
       <c r="E719" t="inlineStr">
         <is>
-          <t>2025/10/28，2025/11/12，2025/12/19，2026/2/8</t>
+          <t>2025/10/28，2025/11/12，2025/12/19，2026/2/8，2026/2/10</t>
         </is>
       </c>
       <c r="F719" t="inlineStr"/>
@@ -26445,7 +26469,7 @@
       </c>
       <c r="H719" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I719" t="inlineStr">
@@ -27792,7 +27816,7 @@
       </c>
       <c r="E757" t="inlineStr">
         <is>
-          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5</t>
+          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5，2026/2/10</t>
         </is>
       </c>
       <c r="F757" t="inlineStr"/>
@@ -27803,7 +27827,7 @@
       </c>
       <c r="H757" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I757" t="inlineStr">
@@ -28384,7 +28408,7 @@
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31</t>
+          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31，2026/2/10</t>
         </is>
       </c>
       <c r="F773" t="inlineStr"/>
@@ -28395,7 +28419,7 @@
       </c>
       <c r="H773" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I773" t="inlineStr">
@@ -28785,7 +28809,7 @@
       </c>
       <c r="E784" t="inlineStr">
         <is>
-          <t>2026/1/24，2026/1/25，2026/1/26，2026/2/2，2026/2/7</t>
+          <t>2026/1/24，2026/1/25，2026/1/26，2026/2/2，2026/2/7，2026/2/10</t>
         </is>
       </c>
       <c r="F784" t="inlineStr"/>
@@ -28796,7 +28820,7 @@
       </c>
       <c r="H784" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I784" t="inlineStr">
@@ -28902,7 +28926,7 @@
       </c>
       <c r="E787" t="inlineStr">
         <is>
-          <t>2026/1/25</t>
+          <t>2026/1/25，2026/2/10</t>
         </is>
       </c>
       <c r="F787" t="inlineStr"/>
@@ -28913,7 +28937,7 @@
       </c>
       <c r="H787" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I787" t="inlineStr"/>

</xml_diff>

<commit_message>
Update song list to Feb 12, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I797"/>
+  <dimension ref="A1:I798"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025/03/02，2025/03/29，2025/04/11，2025/04/17，2025/04/26，2025/05/04，2025/05/09，2025/05/17，2025/05/24，2025/06/02，2025/06/20，2025/06/27，2025/07/11，2025/07/21，2025/07/26，2025/08/08，2025/08/29，2025/09/02，2025/10/03，2025/10/09，2025/10/22，2025/11/9，2025/12/11，2026/1/15</t>
+          <t>2025/03/02，2025/03/29，2025/04/11，2025/04/17，2025/04/26，2025/05/04，2025/05/09，2025/05/17，2025/05/24，2025/06/02，2025/06/20，2025/06/27，2025/07/11，2025/07/21，2025/07/26，2025/08/08，2025/08/29，2025/09/02，2025/10/03，2025/10/09，2025/10/22，2025/11/9，2025/12/11，2026/1/15，2026/2/12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -670,7 +670,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/29，2026/2/10</t>
+          <t>2025/03/04，2025/03/19，2025/04/14，2025/04/22，2025/05/01，2025/05/13，2025/05/19，2025/05/27，2025/06/03，2025/06/12，2025/06/19，2025/06/27，2025/07/08，2025/07/14，2025/07/18，2025/07/20，2025/08/02，2025/08/08，2025/08/12，2025/09/02，2025/09/18，2025/10/01，2025/10/03，2025/10/11，2025/10/24，2025/11/13，2025/11/14，2025/11/28，2025/12/7，2025/12/17，2026/1/19，2026/1/29，2026/2/10，2026/2/12</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -990,7 +990,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/04/02，2025/04/17，2025/04/29，2025/05/12，2025/05/27，2025/06/10，2025/07/05，2025/08/10，2025/08/28，2025/09/05，2025/09/18，2025/11/12，2025/11/28，2026/1/9</t>
+          <t>2025/03/04，2025/04/02，2025/04/17，2025/04/29，2025/05/12，2025/05/27，2025/06/10，2025/07/05，2025/08/10，2025/08/28，2025/09/05，2025/09/18，2025/11/12，2025/11/28，2026/1/9，2026/2/12</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/04/03，2025/04/14，2025/05/05，2025/05/15，2025/05/29，2025/06/20，2025/06/27，2025/08/07，2025/08/24，2025/09/17，2025/10/16，2025/11/10，2025/12/9，2025/12/17，2026/1/21</t>
+          <t>2025/03/06，2025/04/03，2025/04/14，2025/05/05，2025/05/15，2025/05/29，2025/06/20，2025/06/27，2025/08/07，2025/08/24，2025/09/17，2025/10/16，2025/11/10，2025/12/9，2025/12/17，2026/1/21，2026/2/12</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -2140,10 +2140,14 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>BV15u75zsEE6</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3033,7 +3037,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/03/24，2025/04/06，2025/04/21，2025/04/28，2025/05/08，2025/05/20，2025/06/08，2025/07/08，2025/07/28，2025/09/24，2025/09/30，2025/11/18，2025/12/24，2026/2/2</t>
+          <t>2025/03/09，2025/03/24，2025/04/06，2025/04/21，2025/04/28，2025/05/08，2025/05/20，2025/06/08，2025/07/08，2025/07/28，2025/09/24，2025/09/30，2025/11/18，2025/12/24，2026/2/2，2026/2/12</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -3044,7 +3048,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -9702,7 +9706,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/04/11，2025/04/18，2025/04/29，2025/05/08，2025/07/22，2025/07/29，2025/08/04，2025/08/21，2025/09/06，2025/10/09，2025/12/12</t>
+          <t>2025/04/01，2025/04/11，2025/04/18，2025/04/29，2025/05/08，2025/07/22，2025/07/29，2025/08/04，2025/08/21，2025/09/06，2025/10/09，2025/12/12，2026/2/12</t>
         </is>
       </c>
       <c r="F251" t="inlineStr"/>
@@ -9713,10 +9717,14 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I251" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>BV19G5TztEGW</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -12745,7 +12753,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>2025/04/13，2025/04/21，2025/04/22，2025/04/25，2025/04/26，2025/04/29，2025/05/08，2025/05/12，2025/05/22，2025/05/30，2025/06/06，2025/06/08，2025/06/28，2025/07/13，2025/08/12，2025/08/24，2025/09/07，2025/09/30，2025/10/05，2025/11/21，2025/12/17，2026/1/14，2026/1/23</t>
+          <t>2025/04/13，2025/04/21，2025/04/22，2025/04/25，2025/04/26，2025/04/29，2025/05/08，2025/05/12，2025/05/22，2025/05/30，2025/06/06，2025/06/08，2025/06/28，2025/07/13，2025/08/12，2025/08/24，2025/09/07，2025/09/30，2025/10/05，2025/11/21，2025/12/17，2026/1/14，2026/1/23，2026/2/12</t>
         </is>
       </c>
       <c r="F336" t="inlineStr"/>
@@ -12756,7 +12764,7 @@
       </c>
       <c r="H336" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24</t>
         </is>
       </c>
       <c r="I336" t="inlineStr">
@@ -15283,7 +15291,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>2025/04/28，2025/05/06，2025/07/27，2025/09/17，2025/10/16，2025/11/9</t>
+          <t>2025/04/28，2025/05/06，2025/07/27，2025/09/17，2025/10/16，2025/11/9，2026/2/12</t>
         </is>
       </c>
       <c r="F406" t="inlineStr"/>
@@ -15294,10 +15302,14 @@
       </c>
       <c r="H406" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I406" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>BV1BMcBzsEnM</t>
+        </is>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -19026,7 +19038,7 @@
       </c>
       <c r="E511" t="inlineStr">
         <is>
-          <t>2025/06/09，2025/08/26，2025/09/17，2025/10/11</t>
+          <t>2025/06/09，2025/08/26，2025/09/17，2025/10/11，2026/2/12</t>
         </is>
       </c>
       <c r="F511" t="inlineStr"/>
@@ -19037,10 +19049,14 @@
       </c>
       <c r="H511" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I511" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>BV1EMcBzxEwJ</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
@@ -20131,7 +20147,7 @@
       </c>
       <c r="E542" t="inlineStr">
         <is>
-          <t>2025/06/23，2025/12/4，2025/12/5</t>
+          <t>2025/06/23，2025/12/4，2025/12/5，2026/2/12</t>
         </is>
       </c>
       <c r="F542" t="inlineStr"/>
@@ -20142,10 +20158,14 @@
       </c>
       <c r="H542" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I542" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I542" t="inlineStr">
+        <is>
+          <t>BV1d52iBrEwq</t>
+        </is>
+      </c>
     </row>
     <row r="543">
       <c r="A543" t="inlineStr">
@@ -20987,7 +21007,7 @@
       </c>
       <c r="E566" t="inlineStr">
         <is>
-          <t>2025/07/03，2025/07/07，2025/07/26，2025/08/28，2025/09/14，2025/10/11，2025/11/26，2025/12/9，2026/1/9，2026/1/23</t>
+          <t>2025/07/03，2025/07/07，2025/07/26，2025/08/28，2025/09/14，2025/10/11，2025/11/26，2025/12/9，2026/1/9，2026/1/23，2026/2/12</t>
         </is>
       </c>
       <c r="F566" t="inlineStr"/>
@@ -20998,7 +21018,7 @@
       </c>
       <c r="H566" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I566" t="inlineStr">
@@ -21485,7 +21505,7 @@
       </c>
       <c r="E580" t="inlineStr">
         <is>
-          <t>2025/07/11，2025/09/30，2025/10/31，2025/12/4，2026/1/23</t>
+          <t>2025/07/11，2025/09/30，2025/10/31，2025/12/4，2026/1/23，2026/2/12</t>
         </is>
       </c>
       <c r="F580" t="inlineStr"/>
@@ -21496,10 +21516,14 @@
       </c>
       <c r="H580" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I580" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I580" t="inlineStr">
+        <is>
+          <t>BV16AcBzZE4S</t>
+        </is>
+      </c>
     </row>
     <row r="581">
       <c r="A581" t="inlineStr">
@@ -22415,7 +22439,7 @@
       </c>
       <c r="E606" t="inlineStr">
         <is>
-          <t>2025/07/31，2025/08/01，2025/08/04，2025/08/09，2025/08/13，2025/08/21，2025/08/29，2025/09/10，2025/09/30，2025/10/30，2025/11/14，2025/12/24，2026/1/19</t>
+          <t>2025/07/31，2025/08/01，2025/08/04，2025/08/09，2025/08/13，2025/08/21，2025/08/29，2025/09/10，2025/09/30，2025/10/30，2025/11/14，2025/12/24，2026/1/19，2026/2/12</t>
         </is>
       </c>
       <c r="F606" t="inlineStr"/>
@@ -22426,10 +22450,14 @@
       </c>
       <c r="H606" t="inlineStr">
         <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="I606" t="inlineStr"/>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I606" t="inlineStr">
+        <is>
+          <t>BV1kfcqzhEv6</t>
+        </is>
+      </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
@@ -24209,7 +24237,7 @@
       </c>
       <c r="E656" t="inlineStr">
         <is>
-          <t>2025/09/19，2025/09/26，2025/10/16，2025/11/26</t>
+          <t>2025/09/19，2025/09/26，2025/10/16，2025/11/26，2026/2/12</t>
         </is>
       </c>
       <c r="F656" t="inlineStr"/>
@@ -24220,10 +24248,14 @@
       </c>
       <c r="H656" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I656" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I656" t="inlineStr">
+        <is>
+          <t>BV1B4cqzWEhs</t>
+        </is>
+      </c>
     </row>
     <row r="657">
       <c r="A657" t="inlineStr">
@@ -28940,7 +28972,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I787" t="inlineStr"/>
+      <c r="I787" t="inlineStr">
+        <is>
+          <t>BV1Gnc4zmEjA</t>
+        </is>
+      </c>
     </row>
     <row r="788">
       <c r="A788" t="inlineStr">
@@ -29233,7 +29269,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9</t>
+          <t>2026/2/8，2026/2/9，2026/2/12</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29244,7 +29280,7 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
@@ -29282,7 +29318,46 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I797" t="inlineStr"/>
+      <c r="I797" t="inlineStr">
+        <is>
+          <t>BV1EkcszREeP</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr"/>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>词不达意</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr"/>
+      <c r="D798" t="inlineStr">
+        <is>
+          <t>林忆莲</t>
+        </is>
+      </c>
+      <c r="E798" t="inlineStr">
+        <is>
+          <t>2026/2/12</t>
+        </is>
+      </c>
+      <c r="F798" t="inlineStr"/>
+      <c r="G798" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H798" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I798" t="inlineStr">
+        <is>
+          <t>BV1BNcBz4ECH</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 17, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I800"/>
+  <dimension ref="A1:I802"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/04，2025/04/19，2025/06/02，2025/06/17，2025/06/23，2025/07/20，2025/09/24，2025/10/09</t>
+          <t>2025/03/07，2025/04/04，2025/04/19，2025/06/02，2025/06/17，2025/06/23，2025/07/20，2025/09/24，2025/10/09，2026/2/17</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -2390,10 +2390,14 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>BV1UtJ9zaEWY</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3602,7 +3606,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025/03/12，2025/03/21，2025/04/04，2025/05/03，2025/06/21，2025/09/30，2025/10/22</t>
+          <t>2025/03/12，2025/03/21，2025/04/04，2025/05/03，2025/06/21，2025/09/30，2025/10/22，2026/2/17</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
@@ -3616,7 +3620,11 @@
           <t>7</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr"/>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>BV1JvZ1BuEc1</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -12669,7 +12677,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>2025/04/11，2025/06/02，2025/06/12，2025/09/27，2025/11/9，2025/12/19，2026/1/1</t>
+          <t>2025/04/11，2025/06/02，2025/06/12，2025/09/27，2025/11/9，2025/12/19，2026/1/1，2026/2/17</t>
         </is>
       </c>
       <c r="F332" t="inlineStr"/>
@@ -12680,10 +12688,14 @@
       </c>
       <c r="H332" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I332" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>BV1EvZ1BuEcQ</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -18297,7 +18309,7 @@
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>2025/06/01，2025/11/9，2025/11/28</t>
+          <t>2025/06/01，2025/11/9，2025/11/28，2026/2/17</t>
         </is>
       </c>
       <c r="F488" t="inlineStr"/>
@@ -18308,10 +18320,14 @@
       </c>
       <c r="H488" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I488" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I488" t="inlineStr">
+        <is>
+          <t>BV1zYZ1B6EL6</t>
+        </is>
+      </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
@@ -22010,7 +22026,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>Stronger Than You Response (ver. Frisk)</t>
+          <t>Stronger Than You(Frisk Parody)</t>
         </is>
       </c>
       <c r="C592" t="inlineStr"/>
@@ -22021,7 +22037,7 @@
       </c>
       <c r="E592" t="inlineStr">
         <is>
-          <t>2025/07/17，2025/09/06</t>
+          <t>2025/07/17，2025/09/06，2026/2/17</t>
         </is>
       </c>
       <c r="F592" t="inlineStr"/>
@@ -22032,7 +22048,7 @@
       </c>
       <c r="H592" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I592" t="inlineStr"/>
@@ -29516,6 +29532,72 @@
           <t>BV14GZEBgErZ</t>
         </is>
       </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr"/>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>发财发福中国年</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr"/>
+      <c r="D801" t="inlineStr">
+        <is>
+          <t>中国娃娃</t>
+        </is>
+      </c>
+      <c r="E801" t="inlineStr">
+        <is>
+          <t>2026/2/17</t>
+        </is>
+      </c>
+      <c r="F801" t="inlineStr"/>
+      <c r="G801" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H801" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I801" t="inlineStr">
+        <is>
+          <t>BV1EYZ1B6ECT</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr"/>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>恭喜发财</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr"/>
+      <c r="D802" t="inlineStr">
+        <is>
+          <t>刘德华</t>
+        </is>
+      </c>
+      <c r="E802" t="inlineStr">
+        <is>
+          <t>2026/2/17</t>
+        </is>
+      </c>
+      <c r="F802" t="inlineStr"/>
+      <c r="G802" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H802" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I802" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 18, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -3844,7 +3844,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/04/12，2025/05/19，2025/05/25，2025/07/05，2025/08/12，2025/09/03，2025/09/10，2025/11/14，2025/12/31</t>
+          <t>2025/03/13，2025/04/12，2025/05/19，2025/05/25，2025/07/05，2025/08/12，2025/09/03，2025/09/10，2025/11/14，2025/12/31，2026/2/18</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -3855,10 +3855,14 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr"/>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>BV1d33ozhE7x</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4027,7 +4031,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/03/28，2025/04/11，2025/04/25，2025/05/15，2025/05/29，2025/06/20，2025/07/13，2025/09/19，2025/10/05，2025/10/23，2025/11/9，2026/1/23</t>
+          <t>2025/03/13，2025/03/28，2025/04/11，2025/04/25，2025/05/15，2025/05/29，2025/06/20，2025/07/13，2025/09/19，2025/10/05，2025/10/23，2025/11/9，2026/1/23，2026/2/18</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
@@ -4038,10 +4042,14 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr"/>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>BV14jZRBVEJU</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7076,7 +7084,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>2025/03/21，2025/05/09，2025/05/30，2025/07/22，2025/09/28，2025/11/18</t>
+          <t>2025/03/21，2025/05/09，2025/05/30，2025/07/22，2025/09/28，2025/11/18，2026/2/18</t>
         </is>
       </c>
       <c r="F177" t="inlineStr"/>
@@ -7087,10 +7095,14 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I177" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>BV1s3nfzkEye</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -10529,7 +10541,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>2025/04/02，2025/04/03，2025/04/08，2025/05/26，2025/07/18，2025/08/16，2025/09/30，2025/11/26，2026/1/23</t>
+          <t>2025/04/02，2025/04/03，2025/04/08，2025/05/26，2025/07/18，2025/08/16，2025/09/30，2025/11/26，2026/1/23，2026/2/18</t>
         </is>
       </c>
       <c r="F272" t="inlineStr"/>
@@ -10540,7 +10552,7 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I272" t="inlineStr">
@@ -13608,7 +13620,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>2025/04/17，2025/04/29，2025/05/22，2025/05/25，2025/05/31，2025/08/29，2025/09/20，2025/10/09，2025/10/30，2025/12/11</t>
+          <t>2025/04/17，2025/04/29，2025/05/22，2025/05/25，2025/05/31，2025/08/29，2025/09/20，2025/10/09，2025/10/30，2025/12/11，2026/2/18</t>
         </is>
       </c>
       <c r="F357" t="inlineStr"/>
@@ -13619,10 +13631,14 @@
       </c>
       <c r="H357" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I357" t="inlineStr"/>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>BV1c5hRznES3</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -16382,7 +16398,7 @@
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr">
         <is>
-          <t>LBl利比</t>
+          <t>LBI利比</t>
         </is>
       </c>
       <c r="E434" t="inlineStr">
@@ -20084,7 +20100,7 @@
       </c>
       <c r="E537" t="inlineStr">
         <is>
-          <t>2025/06/20，2025/06/21，2025/07/08，2025/07/13，2025/07/18，2025/07/28，2025/08/01，2025/08/03，2025/08/04，2025/08/16，2025/09/03，2025/09/13，2025/09/19，2025/10/23，2025/10/28，2025/11/10，2025/11/13，2025/11/18，2025/12/11，2025/12/16</t>
+          <t>2025/06/20，2025/06/21，2025/07/08，2025/07/13，2025/07/18，2025/07/28，2025/08/01，2025/08/03，2025/08/04，2025/08/16，2025/09/03，2025/09/13，2025/09/19，2025/10/23，2025/10/28，2025/11/10，2025/11/13，2025/11/18，2025/12/11，2025/12/16，2026/2/18</t>
         </is>
       </c>
       <c r="F537" t="inlineStr"/>
@@ -20095,7 +20111,7 @@
       </c>
       <c r="H537" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I537" t="inlineStr">
@@ -21863,7 +21879,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>Where did u go</t>
+          <t>Where Did U Go</t>
         </is>
       </c>
       <c r="C587" t="inlineStr"/>
@@ -21874,7 +21890,7 @@
       </c>
       <c r="E587" t="inlineStr">
         <is>
-          <t>2025/07/14，2025/07/17，2025/07/18，2025/07/24，2025/07/28，2025/08/02，2025/08/03，2025/08/21，2025/09/05，2025/09/18，2025/09/30，2025/10/19，2025/11/3，2025/11/22，2026/1/5</t>
+          <t>2025/07/14，2025/07/17，2025/07/18，2025/07/24，2025/07/28，2025/08/02，2025/08/03，2025/08/21，2025/09/05，2025/09/18，2025/09/30，2025/10/19，2025/11/3，2025/11/22，2026/1/5，2026/2/18</t>
         </is>
       </c>
       <c r="F587" t="inlineStr"/>
@@ -21885,7 +21901,7 @@
       </c>
       <c r="H587" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I587" t="inlineStr">
@@ -22960,7 +22976,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>2025/08/12，2025/09/05，2025/09/05，2025/09/17，2025/09/24，2025/09/28，2025/10/01，2025/10/10，2025/10/17，2025/10/23，2025/11/26，2025/12/30，2026/1/10</t>
+          <t>2025/08/12，2025/09/05，2025/09/05，2025/09/17，2025/09/24，2025/09/28，2025/10/01，2025/10/10，2025/10/17，2025/10/23，2025/11/26，2025/12/30，2026/1/10，2026/2/18</t>
         </is>
       </c>
       <c r="F617" t="inlineStr"/>
@@ -22971,7 +22987,7 @@
       </c>
       <c r="H617" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I617" t="inlineStr">
@@ -24867,7 +24883,7 @@
       </c>
       <c r="E670" t="inlineStr">
         <is>
-          <t>2025/09/24，2025/09/29，2025/10/13，2025/10/17，2025/10/19，2025/10/20，2025/10/25，2025/10/28，2025/11/7，2025/11/26，2025/12/6，2025/12/12，2025/12/24，2026/1/5，2026/1/19</t>
+          <t>2025/09/24，2025/09/29，2025/10/13，2025/10/17，2025/10/19，2025/10/20，2025/10/25，2025/10/28，2025/11/7，2025/11/26，2025/12/6，2025/12/12，2025/12/24，2026/1/5，2026/1/19，2026/2/18</t>
         </is>
       </c>
       <c r="F670" t="inlineStr"/>
@@ -24878,7 +24894,7 @@
       </c>
       <c r="H670" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I670" t="inlineStr">

</xml_diff>

<commit_message>
Update song list to Feb 19, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I802"/>
+  <dimension ref="A1:I803"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +577,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025/03/02，2025/03/29，2025/05/06，2025/05/30，2025/06/28，2025/09/04，2025/09/18，2025/11/7，2026/1/14，2026/1/24</t>
+          <t>2025/03/02，2025/03/29，2025/05/06，2025/05/30，2025/06/28，2025/09/04，2025/09/18，2025/11/7，2026/1/14，2026/1/24，2026/2/19</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -588,7 +588,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/12，2025/03/17，2025/03/28，2025/04/07，2025/04/19，2025/04/26，2025/05/06，2025/05/16，2025/05/22，2025/05/30，2025/06/21，2025/07/06，2025/08/22，2025/09/06，2025/09/21，2025/10/23，2025/11/10，2025/11/13，2025/12/4，2026/1/24，2026/1/24</t>
+          <t>2025/03/04，2025/03/12，2025/03/17，2025/03/28，2025/04/07，2025/04/19，2025/04/26，2025/05/06，2025/05/16，2025/05/22，2025/05/30，2025/06/21，2025/07/06，2025/08/22，2025/09/06，2025/09/21，2025/10/23，2025/11/10，2025/11/13，2025/12/4，2026/1/24，2026/1/24，2026/2/19</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -951,7 +951,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/18，2025/07/26，2025/08/12</t>
+          <t>2025/03/04，2025/05/18，2025/07/26，2025/08/12，2025/11/28，2026/2/19</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -1996,10 +1996,14 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>BV15A9HYfEPQ</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2059,7 +2063,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/03/20，2025/04/02，2025/04/10，2025/04/19，2025/04/27，2025/05/13，2025/05/15，2025/05/18，2025/05/26，2025/06/06，2025/06/12，2025/06/21，2025/07/05，2025/07/10，2025/07/13，2025/07/27，2025/08/29，2025/09/13，2025/09/19，2025/09/28，2025/10/23，2025/10/28，2025/12/23，2026/1/14</t>
+          <t>2025/03/06，2025/03/20，2025/04/02，2025/04/10，2025/04/19，2025/04/27，2025/05/13，2025/05/15，2025/05/18，2025/05/26，2025/06/06，2025/06/12，2025/06/21，2025/07/05，2025/07/10，2025/07/13，2025/07/27，2025/08/29，2025/09/13，2025/09/19，2025/09/28，2025/10/23，2025/10/28，2025/12/23，2026/1/14，2026/2/19</t>
         </is>
       </c>
       <c r="F42" t="inlineStr"/>
@@ -2070,10 +2074,14 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>BV14fsGzZESX</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2558,7 +2566,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/20，2025/04/25，2025/05/18，2025/05/26，2025/06/02，2025/06/27，2025/07/07，2025/08/03，2025/09/14，2025/09/17，2025/10/03，2025/10/07，2025/12/7，2025/12/16，2025/12/28，2026/1/10，2026/1/15</t>
+          <t>2025/03/07，2025/04/20，2025/04/25，2025/05/18，2025/05/26，2025/06/02，2025/06/27，2025/07/07，2025/08/03，2025/09/14，2025/09/17，2025/10/03，2025/10/07，2025/12/7，2025/12/16，2025/12/28，2026/1/10，2026/1/15，2026/2/19</t>
         </is>
       </c>
       <c r="F55" t="inlineStr"/>
@@ -2569,7 +2577,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2827,7 +2835,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2838,7 +2846,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>36</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -2905,7 +2913,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/11，2025/04/29，2025/08/01，2025/10/26</t>
+          <t>2025/03/07，2025/04/11，2025/04/29，2025/08/01，2025/10/26，2026/2/19</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2916,10 +2924,14 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>BV12ksmzxE4b</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3131,7 +3143,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/04/06，2025/05/08，2025/05/24，2025/06/06，2025/07/05，2025/07/24，2025/08/04，2025/09/08，2025/09/19，2025/10/16，2025/10/28，2025/11/13，2025/12/16，2025/12/30</t>
+          <t>2025/03/09，2025/04/06，2025/05/08，2025/05/24，2025/06/06，2025/07/05，2025/07/24，2025/08/04，2025/09/08，2025/09/19，2025/10/16，2025/10/28，2025/11/13，2025/12/16，2025/12/30，2026/2/19</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -3142,10 +3154,14 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr"/>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>BV1way6BfE6d</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3692,7 +3708,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025/03/12，2025/04/07，2025/04/18，2025/05/10，2025/05/15，2025/05/29，2025/06/03，2025/06/16，2025/07/08，2025/07/08，2025/08/01，2025/09/04，2025/09/28，2025/10/25，2025/10/28，2025/11/3，2025/12/2，2025/12/4，2025/12/12，2026/1/5，2026/1/14</t>
+          <t>2025/03/12，2025/04/07，2025/04/18，2025/05/10，2025/05/15，2025/05/29，2025/06/03，2025/06/16，2025/07/08，2025/07/08，2025/08/01，2025/09/04，2025/09/28，2025/10/25，2025/10/28，2025/11/3，2025/12/2，2025/12/4，2025/12/12，2026/1/5，2026/1/14，2026/2/19</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -3703,7 +3719,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -4613,7 +4629,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>名为你的诗</t>
+          <t>All about you / 名为你的诗</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4623,7 +4639,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/05/19，2025/07/21，2025/10/20</t>
+          <t>2025/03/14，2025/05/19，2025/07/21，2025/10/20，2026/1/14，2026/2/19</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
@@ -4634,10 +4650,14 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I110" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>BV1eqzWBXE55</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4771,7 +4791,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/02，2025/05/10，2025/05/18，2025/05/23，2025/06/05，2025/06/08，2025/06/27，2025/09/03，2025/09/21，2025/10/30，2025/11/22，2025/12/9，2026/1/15</t>
+          <t>2025/03/14，2025/04/02，2025/05/10，2025/05/18，2025/05/23，2025/06/05，2025/06/08，2025/06/27，2025/09/03，2025/09/21，2025/10/30，2025/11/22，2025/12/9，2026/1/15，2026/2/19</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
@@ -4782,10 +4802,14 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I114" t="inlineStr"/>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>BV1b1KmzUE9y</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5795,7 +5819,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2025/03/19，2025/07/07，2025/08/12，2025/08/26，2025/09/13，2025/09/17，2025/10/10，2025/11/21，2025/12/11，2026/1/2，2026/1/15，2026/1/28</t>
+          <t>2025/03/19，2025/07/07，2025/08/12，2025/08/26，2025/09/13，2025/09/17，2025/10/10，2025/11/21，2025/12/11，2026/1/2，2026/1/15，2026/1/28，2026/2/19</t>
         </is>
       </c>
       <c r="F142" t="inlineStr"/>
@@ -5806,7 +5830,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -6243,7 +6267,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/04/04，2025/05/19，2025/06/08，2025/06/12，2025/07/13，2025/08/28，2025/09/26，2025/10/25，2025/11/19，2025/11/27，2026/1/22，2026/1/25</t>
+          <t>2025/03/20，2025/04/04，2025/05/19，2025/06/08，2025/06/12，2025/07/13，2025/08/28，2025/09/26，2025/10/25，2025/11/19，2025/11/27，2026/1/22，2026/1/25，2026/2/19</t>
         </is>
       </c>
       <c r="F154" t="inlineStr"/>
@@ -6254,7 +6278,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -7014,7 +7038,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>2025/03/21，2025/04/06，2025/04/18，2025/04/25，2025/05/27，2025/07/11，2025/07/24，2025/08/09，2025/09/15，2025/09/21，2025/10/11，2025/10/24，2025/11/3，2025/11/22，2026/1/22</t>
+          <t>2025/03/21，2025/04/06，2025/04/18，2025/04/25，2025/05/27，2025/07/11，2025/07/24，2025/08/09，2025/09/15，2025/09/21，2025/10/11，2025/10/24，2025/11/3，2025/11/22，2026/1/22，2026/2/19</t>
         </is>
       </c>
       <c r="F175" t="inlineStr"/>
@@ -7025,10 +7049,14 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="I175" t="inlineStr"/>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>BV1v84TzcEMv</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8022,7 +8050,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>2025/03/25，2025/04/18，2025/06/02</t>
+          <t>2025/03/25，2025/04/18，2025/06/02，2026/2/19</t>
         </is>
       </c>
       <c r="F203" t="inlineStr"/>
@@ -8033,10 +8061,14 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I203" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>BV1oK5EzwExE</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -8275,7 +8307,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/28，2025/04/29，2025/05/12，2025/06/06，2025/06/16，2025/07/24，2025/08/01，2025/09/05，2025/09/26，2025/10/28，2025/12/5，2026/1/9</t>
+          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/28，2025/04/29，2025/05/12，2025/06/06，2025/06/16，2025/07/24，2025/08/01，2025/09/05，2025/09/26，2025/10/28，2025/12/5，2026/1/9，2026/2/19</t>
         </is>
       </c>
       <c r="F210" t="inlineStr"/>
@@ -8286,10 +8318,14 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="I210" t="inlineStr"/>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>BV1FCa8zEEue</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -8750,7 +8786,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>2025/03/28，2025/06/07，2025/06/13，2025/06/23，2025/07/20，2025/10/24，2025/11/9，2026/1/9</t>
+          <t>2025/03/28，2025/06/07，2025/06/13，2025/06/23，2025/07/20，2025/10/24，2025/11/9，2026/1/9，2026/2/19</t>
         </is>
       </c>
       <c r="F223" t="inlineStr"/>
@@ -8761,10 +8797,14 @@
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I223" t="inlineStr"/>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>BV14HKhzcET9</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -10113,7 +10153,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5，2026/2/2，2026/2/9</t>
+          <t>2025/04/01，2025/10/17，2025/10/22，2025/10/25，2025/11/21，2025/12/11，2026/1/2，2026/1/5，2026/2/2，2026/2/9，2026/2/19</t>
         </is>
       </c>
       <c r="F260" t="inlineStr"/>
@@ -10124,7 +10164,7 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
@@ -13546,7 +13586,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>2025/04/17，2025/05/01，2025/05/26，2025/07/03，2025/07/27，2025/09/18，2025/10/17，2025/11/21，2026/1/12，2026/1/24</t>
+          <t>2025/04/17，2025/05/01，2025/05/26，2025/07/03，2025/07/27，2025/09/18，2025/10/17，2025/11/21，2026/1/12，2026/1/24，2026/2/19</t>
         </is>
       </c>
       <c r="F355" t="inlineStr"/>
@@ -13557,7 +13597,7 @@
       </c>
       <c r="H355" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I355" t="inlineStr">
@@ -15734,7 +15774,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>2025/05/02，2025/05/15，2025/06/14</t>
+          <t>2025/05/02，2025/05/15，2025/06/14，2026/2/19</t>
         </is>
       </c>
       <c r="F415" t="inlineStr"/>
@@ -15745,10 +15785,14 @@
       </c>
       <c r="H415" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I415" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>BV1cvEnzREJb</t>
+        </is>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
@@ -19730,7 +19774,11 @@
           <t>색안경 (STEREOTYPE)</t>
         </is>
       </c>
-      <c r="C527" t="inlineStr"/>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>有色眼镜</t>
+        </is>
+      </c>
       <c r="D527" t="inlineStr">
         <is>
           <t>STAYC</t>
@@ -20462,7 +20510,7 @@
       </c>
       <c r="E547" t="inlineStr">
         <is>
-          <t>2025/06/26，2025/06/27，2025/07/14，2025/07/17，2025/08/23，2025/09/21，2025/10/28，2025/11/10，2026/1/14，2026/1/22</t>
+          <t>2025/06/26，2025/06/27，2025/07/14，2025/07/17，2025/08/23，2025/09/21，2025/10/28，2025/11/10，2026/1/14，2026/1/22，2026/2/19</t>
         </is>
       </c>
       <c r="F547" t="inlineStr"/>
@@ -20473,10 +20521,14 @@
       </c>
       <c r="H547" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I547" t="inlineStr"/>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="I547" t="inlineStr">
+        <is>
+          <t>BV1iLJdzEEWk</t>
+        </is>
+      </c>
     </row>
     <row r="548">
       <c r="A548" t="inlineStr">
@@ -22108,7 +22160,7 @@
       </c>
       <c r="E593" t="inlineStr">
         <is>
-          <t>2025/07/17，2025/07/24，2025/07/28，2025/08/01，2025/08/04，2025/08/09，2025/08/13，2025/08/26，2025/08/29，2025/09/19，2025/09/29，2025/10/11，2025/10/22，2025/10/28，2025/11/10，2025/11/28，2025/12/16</t>
+          <t>2025/07/17，2025/07/24，2025/07/28，2025/08/01，2025/08/04，2025/08/09，2025/08/13，2025/08/26，2025/08/29，2025/09/19，2025/09/29，2025/10/11，2025/10/22，2025/10/28，2025/11/10，2025/11/28，2025/12/16，2026/2/19</t>
         </is>
       </c>
       <c r="F593" t="inlineStr"/>
@@ -22119,7 +22171,7 @@
       </c>
       <c r="H593" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I593" t="inlineStr">
@@ -22388,7 +22440,11 @@
           <t>One Spot</t>
         </is>
       </c>
-      <c r="C601" t="inlineStr"/>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>美美桑内</t>
+        </is>
+      </c>
       <c r="D601" t="inlineStr">
         <is>
           <t>沈佳润</t>
@@ -22396,7 +22452,7 @@
       </c>
       <c r="E601" t="inlineStr">
         <is>
-          <t>2025/07/26，2025/07/28，2025/08/26，2025/09/10</t>
+          <t>2025/07/26，2025/07/28，2025/08/26，2025/09/10，2026/2/19</t>
         </is>
       </c>
       <c r="F601" t="inlineStr"/>
@@ -22407,10 +22463,14 @@
       </c>
       <c r="H601" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I601" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I601" t="inlineStr">
+        <is>
+          <t>BV14L8nzZEcB</t>
+        </is>
+      </c>
     </row>
     <row r="602">
       <c r="A602" t="inlineStr">
@@ -23194,7 +23254,7 @@
       </c>
       <c r="E623" t="inlineStr">
         <is>
-          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9，2026/1/29</t>
+          <t>2025/08/26，2025/08/16，2025/11/13，2025/12/9，2026/1/29，2026/2/19</t>
         </is>
       </c>
       <c r="F623" t="inlineStr"/>
@@ -23205,7 +23265,7 @@
       </c>
       <c r="H623" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I623" t="inlineStr">
@@ -25785,7 +25845,11 @@
           <t>2025/10/13</t>
         </is>
       </c>
-      <c r="F695" t="inlineStr"/>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>点歌大概率不唱</t>
+        </is>
+      </c>
       <c r="G695" t="inlineStr">
         <is>
           <t>华语</t>
@@ -27762,18 +27826,18 @@
     <row r="751">
       <c r="A751" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>751</t>
         </is>
       </c>
       <c r="B751" t="inlineStr">
         <is>
-          <t>千千阙歌</t>
+          <t>九张机</t>
         </is>
       </c>
       <c r="C751" t="inlineStr"/>
       <c r="D751" t="inlineStr">
         <is>
-          <t>陈慧娴</t>
+          <t>叶炫清</t>
         </is>
       </c>
       <c r="E751" t="inlineStr">
@@ -27797,29 +27861,29 @@
     <row r="752">
       <c r="A752" t="inlineStr">
         <is>
-          <t>751</t>
+          <t>752</t>
         </is>
       </c>
       <c r="B752" t="inlineStr">
         <is>
-          <t>九张机</t>
+          <t>Hey Jude</t>
         </is>
       </c>
       <c r="C752" t="inlineStr"/>
       <c r="D752" t="inlineStr">
         <is>
-          <t>叶炫清</t>
+          <t>The Beatles</t>
         </is>
       </c>
       <c r="E752" t="inlineStr">
         <is>
-          <t>2025/11/28</t>
+          <t>2025/12/2</t>
         </is>
       </c>
       <c r="F752" t="inlineStr"/>
       <c r="G752" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H752" t="inlineStr">
@@ -27832,23 +27896,23 @@
     <row r="753">
       <c r="A753" t="inlineStr">
         <is>
-          <t>752</t>
+          <t>753</t>
         </is>
       </c>
       <c r="B753" t="inlineStr">
         <is>
-          <t>Hey Jude</t>
+          <t>Loves Me Not</t>
         </is>
       </c>
       <c r="C753" t="inlineStr"/>
       <c r="D753" t="inlineStr">
         <is>
-          <t>The Beatles</t>
+          <t>t.A.T.u.</t>
         </is>
       </c>
       <c r="E753" t="inlineStr">
         <is>
-          <t>2025/12/2</t>
+          <t>2025/12/4</t>
         </is>
       </c>
       <c r="F753" t="inlineStr"/>
@@ -27867,18 +27931,18 @@
     <row r="754">
       <c r="A754" t="inlineStr">
         <is>
-          <t>753</t>
+          <t>754</t>
         </is>
       </c>
       <c r="B754" t="inlineStr">
         <is>
-          <t>Loves Me Not</t>
+          <t>不怕不怕</t>
         </is>
       </c>
       <c r="C754" t="inlineStr"/>
       <c r="D754" t="inlineStr">
         <is>
-          <t>t.A.T.u.</t>
+          <t>美美jocie</t>
         </is>
       </c>
       <c r="E754" t="inlineStr">
@@ -27889,7 +27953,7 @@
       <c r="F754" t="inlineStr"/>
       <c r="G754" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H754" t="inlineStr">
@@ -27902,23 +27966,23 @@
     <row r="755">
       <c r="A755" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>755</t>
         </is>
       </c>
       <c r="B755" t="inlineStr">
         <is>
-          <t>不怕不怕</t>
+          <t>卜卦</t>
         </is>
       </c>
       <c r="C755" t="inlineStr"/>
       <c r="D755" t="inlineStr">
         <is>
-          <t>美美jocie</t>
+          <t>崔子格</t>
         </is>
       </c>
       <c r="E755" t="inlineStr">
         <is>
-          <t>2025/12/4</t>
+          <t>2025/12/5</t>
         </is>
       </c>
       <c r="F755" t="inlineStr"/>
@@ -27937,34 +28001,38 @@
     <row r="756">
       <c r="A756" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>756</t>
         </is>
       </c>
       <c r="B756" t="inlineStr">
         <is>
-          <t>卜卦</t>
-        </is>
-      </c>
-      <c r="C756" t="inlineStr"/>
+          <t>届かない恋</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>无法传达的恋爱</t>
+        </is>
+      </c>
       <c r="D756" t="inlineStr">
         <is>
-          <t>崔子格</t>
+          <t>上原玲奈</t>
         </is>
       </c>
       <c r="E756" t="inlineStr">
         <is>
-          <t>2025/12/5</t>
+          <t>2025/12/9，2026/2/2</t>
         </is>
       </c>
       <c r="F756" t="inlineStr"/>
       <c r="G756" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>日语</t>
         </is>
       </c>
       <c r="H756" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I756" t="inlineStr"/>
@@ -27972,62 +28040,62 @@
     <row r="757">
       <c r="A757" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>757</t>
         </is>
       </c>
       <c r="B757" t="inlineStr">
         <is>
-          <t>届かない恋</t>
-        </is>
-      </c>
-      <c r="C757" t="inlineStr">
-        <is>
-          <t>无法传达的恋爱</t>
-        </is>
-      </c>
+          <t>听见</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr"/>
       <c r="D757" t="inlineStr">
         <is>
-          <t>上原玲奈</t>
+          <t>方雅贤</t>
         </is>
       </c>
       <c r="E757" t="inlineStr">
         <is>
-          <t>2025/12/9，2026/2/2</t>
+          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5，2026/2/10</t>
         </is>
       </c>
       <c r="F757" t="inlineStr"/>
       <c r="G757" t="inlineStr">
         <is>
-          <t>日语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H757" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I757" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I757" t="inlineStr">
+        <is>
+          <t>BV1cWmnB5Etm</t>
+        </is>
+      </c>
     </row>
     <row r="758">
       <c r="A758" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>758</t>
         </is>
       </c>
       <c r="B758" t="inlineStr">
         <is>
-          <t>听见</t>
+          <t>神探</t>
         </is>
       </c>
       <c r="C758" t="inlineStr"/>
       <c r="D758" t="inlineStr">
         <is>
-          <t>方雅贤</t>
+          <t>丁世光</t>
         </is>
       </c>
       <c r="E758" t="inlineStr">
         <is>
-          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5，2026/2/10</t>
+          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/29，2026/2/9</t>
         </is>
       </c>
       <c r="F758" t="inlineStr"/>
@@ -28038,35 +28106,35 @@
       </c>
       <c r="H758" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I758" t="inlineStr">
         <is>
-          <t>BV1cWmnB5Etm</t>
+          <t>BV1FekxB5Etj</t>
         </is>
       </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>759</t>
         </is>
       </c>
       <c r="B759" t="inlineStr">
         <is>
-          <t>神探</t>
+          <t>我的天坑</t>
         </is>
       </c>
       <c r="C759" t="inlineStr"/>
       <c r="D759" t="inlineStr">
         <is>
-          <t>丁世光</t>
+          <t>南征北战NZBZ</t>
         </is>
       </c>
       <c r="E759" t="inlineStr">
         <is>
-          <t>2025/12/11，2025/12/12，2025/12/17，2026/1/2，2026/1/5，2026/1/11，2026/1/17，2026/1/29，2026/2/9</t>
+          <t>2025/12/12</t>
         </is>
       </c>
       <c r="F759" t="inlineStr"/>
@@ -28077,30 +28145,26 @@
       </c>
       <c r="H759" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I759" t="inlineStr">
-        <is>
-          <t>BV1FekxB5Etj</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I759" t="inlineStr"/>
     </row>
     <row r="760">
       <c r="A760" t="inlineStr">
         <is>
-          <t>759</t>
+          <t>760</t>
         </is>
       </c>
       <c r="B760" t="inlineStr">
         <is>
-          <t>我的天坑</t>
+          <t>同桌的你</t>
         </is>
       </c>
       <c r="C760" t="inlineStr"/>
       <c r="D760" t="inlineStr">
         <is>
-          <t>南征北战NZBZ</t>
+          <t>老狼</t>
         </is>
       </c>
       <c r="E760" t="inlineStr">
@@ -28124,18 +28188,18 @@
     <row r="761">
       <c r="A761" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>761</t>
         </is>
       </c>
       <c r="B761" t="inlineStr">
         <is>
-          <t>同桌的你</t>
+          <t>北京东路的日子</t>
         </is>
       </c>
       <c r="C761" t="inlineStr"/>
       <c r="D761" t="inlineStr">
         <is>
-          <t>老狼</t>
+          <t>群星</t>
         </is>
       </c>
       <c r="E761" t="inlineStr">
@@ -28159,18 +28223,18 @@
     <row r="762">
       <c r="A762" t="inlineStr">
         <is>
-          <t>761</t>
+          <t>762</t>
         </is>
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>北京东路的日子</t>
+          <t>倔强</t>
         </is>
       </c>
       <c r="C762" t="inlineStr"/>
       <c r="D762" t="inlineStr">
         <is>
-          <t>群星</t>
+          <t>五月天</t>
         </is>
       </c>
       <c r="E762" t="inlineStr">
@@ -28194,18 +28258,18 @@
     <row r="763">
       <c r="A763" t="inlineStr">
         <is>
-          <t>762</t>
+          <t>763</t>
         </is>
       </c>
       <c r="B763" t="inlineStr">
         <is>
-          <t>倔强</t>
+          <t>Brand new me</t>
         </is>
       </c>
       <c r="C763" t="inlineStr"/>
       <c r="D763" t="inlineStr">
         <is>
-          <t>五月天</t>
+          <t>Alicia Keys</t>
         </is>
       </c>
       <c r="E763" t="inlineStr">
@@ -28216,7 +28280,7 @@
       <c r="F763" t="inlineStr"/>
       <c r="G763" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H763" t="inlineStr">
@@ -28229,29 +28293,29 @@
     <row r="764">
       <c r="A764" t="inlineStr">
         <is>
-          <t>763</t>
+          <t>764</t>
         </is>
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>Brand new me</t>
+          <t>太难唱了</t>
         </is>
       </c>
       <c r="C764" t="inlineStr"/>
       <c r="D764" t="inlineStr">
         <is>
-          <t>Alicia Keys</t>
+          <t>彭佳慧</t>
         </is>
       </c>
       <c r="E764" t="inlineStr">
         <is>
-          <t>2025/12/12</t>
+          <t>2025/12/16</t>
         </is>
       </c>
       <c r="F764" t="inlineStr"/>
       <c r="G764" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H764" t="inlineStr">
@@ -28264,23 +28328,23 @@
     <row r="765">
       <c r="A765" t="inlineStr">
         <is>
-          <t>764</t>
+          <t>765</t>
         </is>
       </c>
       <c r="B765" t="inlineStr">
         <is>
-          <t>太难唱了</t>
+          <t>他一定很爱你</t>
         </is>
       </c>
       <c r="C765" t="inlineStr"/>
       <c r="D765" t="inlineStr">
         <is>
-          <t>彭佳慧</t>
+          <t>阿杜</t>
         </is>
       </c>
       <c r="E765" t="inlineStr">
         <is>
-          <t>2025/12/16</t>
+          <t>2025/12/17</t>
         </is>
       </c>
       <c r="F765" t="inlineStr"/>
@@ -28299,97 +28363,101 @@
     <row r="766">
       <c r="A766" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>766</t>
         </is>
       </c>
       <c r="B766" t="inlineStr">
         <is>
-          <t>他一定很爱你</t>
+          <t>Please Please Please</t>
         </is>
       </c>
       <c r="C766" t="inlineStr"/>
       <c r="D766" t="inlineStr">
         <is>
-          <t>阿杜</t>
+          <t>Sabrina Carpenter</t>
         </is>
       </c>
       <c r="E766" t="inlineStr">
         <is>
-          <t>2025/12/17</t>
+          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23，2026/1/29</t>
         </is>
       </c>
       <c r="F766" t="inlineStr"/>
       <c r="G766" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H766" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I766" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I766" t="inlineStr">
+        <is>
+          <t>BV1K8isBiExx</t>
+        </is>
+      </c>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
         <is>
-          <t>766</t>
+          <t>767</t>
         </is>
       </c>
       <c r="B767" t="inlineStr">
         <is>
-          <t>Please Please Please</t>
+          <t>流浪者之歌</t>
         </is>
       </c>
       <c r="C767" t="inlineStr"/>
       <c r="D767" t="inlineStr">
         <is>
-          <t>Sabrina Carpenter</t>
+          <t>F.I.R.飞儿乐团</t>
         </is>
       </c>
       <c r="E767" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/24，2025/12/26，2026/1/2，2026/1/9，2026/1/23，2026/1/29</t>
+          <t>2025/12/19，2026/2/8</t>
         </is>
       </c>
       <c r="F767" t="inlineStr"/>
       <c r="G767" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H767" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I767" t="inlineStr">
         <is>
-          <t>BV1K8isBiExx</t>
+          <t>BV1WVqrBLEc2</t>
         </is>
       </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
         <is>
-          <t>767</t>
+          <t>768</t>
         </is>
       </c>
       <c r="B768" t="inlineStr">
         <is>
-          <t>流浪者之歌</t>
+          <t>气球</t>
         </is>
       </c>
       <c r="C768" t="inlineStr"/>
       <c r="D768" t="inlineStr">
         <is>
-          <t>F.I.R.飞儿乐团</t>
+          <t>许哲珮</t>
         </is>
       </c>
       <c r="E768" t="inlineStr">
         <is>
-          <t>2025/12/19，2026/2/8</t>
+          <t>2025/12/19</t>
         </is>
       </c>
       <c r="F768" t="inlineStr"/>
@@ -28400,35 +28468,31 @@
       </c>
       <c r="H768" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I768" t="inlineStr">
-        <is>
-          <t>BV1WVqrBLEc2</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I768" t="inlineStr"/>
     </row>
     <row r="769">
       <c r="A769" t="inlineStr">
         <is>
-          <t>768</t>
+          <t>769</t>
         </is>
       </c>
       <c r="B769" t="inlineStr">
         <is>
-          <t>气球</t>
+          <t>一样的月光</t>
         </is>
       </c>
       <c r="C769" t="inlineStr"/>
       <c r="D769" t="inlineStr">
         <is>
-          <t>许哲珮</t>
+          <t>徐佳莹</t>
         </is>
       </c>
       <c r="E769" t="inlineStr">
         <is>
-          <t>2025/12/19</t>
+          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25，2026/2/9</t>
         </is>
       </c>
       <c r="F769" t="inlineStr"/>
@@ -28439,70 +28503,74 @@
       </c>
       <c r="H769" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I769" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I769" t="inlineStr">
+        <is>
+          <t>BV1oKiwBXE1L</t>
+        </is>
+      </c>
     </row>
     <row r="770">
       <c r="A770" t="inlineStr">
         <is>
-          <t>769</t>
+          <t>770</t>
         </is>
       </c>
       <c r="B770" t="inlineStr">
         <is>
-          <t>一样的月光</t>
+          <t>BIRDS OF A FEATHER</t>
         </is>
       </c>
       <c r="C770" t="inlineStr"/>
       <c r="D770" t="inlineStr">
         <is>
-          <t>徐佳莹</t>
+          <t>Billie Eilish</t>
         </is>
       </c>
       <c r="E770" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25，2026/2/9</t>
+          <t>2025/12/24，2025/12/24，2025/12/26，2026/1/2，2026/1/10</t>
         </is>
       </c>
       <c r="F770" t="inlineStr"/>
       <c r="G770" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H770" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I770" t="inlineStr">
         <is>
-          <t>BV1oKiwBXE1L</t>
+          <t>BV1GiicB5EFK</t>
         </is>
       </c>
     </row>
     <row r="771">
       <c r="A771" t="inlineStr">
         <is>
-          <t>770</t>
+          <t>771</t>
         </is>
       </c>
       <c r="B771" t="inlineStr">
         <is>
-          <t>BIRDS OF A FEATHER</t>
+          <t>Catch Me If You Can</t>
         </is>
       </c>
       <c r="C771" t="inlineStr"/>
       <c r="D771" t="inlineStr">
         <is>
-          <t>Billie Eilish</t>
+          <t>鸣潮先约电台</t>
         </is>
       </c>
       <c r="E771" t="inlineStr">
         <is>
-          <t>2025/12/24，2025/12/24，2025/12/26，2026/1/2，2026/1/10</t>
+          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7，2026/2/19</t>
         </is>
       </c>
       <c r="F771" t="inlineStr"/>
@@ -28513,74 +28581,74 @@
       </c>
       <c r="H771" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I771" t="inlineStr">
         <is>
-          <t>BV1GiicB5EFK</t>
+          <t>BV1pfzcBgERV</t>
         </is>
       </c>
     </row>
     <row r="772">
       <c r="A772" t="inlineStr">
         <is>
-          <t>771</t>
+          <t>772</t>
         </is>
       </c>
       <c r="B772" t="inlineStr">
         <is>
-          <t>Catch Me If You Can</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C772" t="inlineStr"/>
       <c r="D772" t="inlineStr">
         <is>
-          <t>鸣潮先约电台</t>
+          <t>队长/黄礼格</t>
         </is>
       </c>
       <c r="E772" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7</t>
+          <t>2025/12/26，2026/1/19，2026/2/9</t>
         </is>
       </c>
       <c r="F772" t="inlineStr"/>
       <c r="G772" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H772" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I772" t="inlineStr">
         <is>
-          <t>BV1pfzcBgERV</t>
+          <t>BV1VUcuzvEaU</t>
         </is>
       </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
         <is>
-          <t>772</t>
+          <t>773</t>
         </is>
       </c>
       <c r="B773" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>鱼仔</t>
         </is>
       </c>
       <c r="C773" t="inlineStr"/>
       <c r="D773" t="inlineStr">
         <is>
-          <t>队长/黄礼格</t>
+          <t>卢广仲</t>
         </is>
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/19，2026/2/9</t>
+          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31，2026/2/10</t>
         </is>
       </c>
       <c r="F773" t="inlineStr"/>
@@ -28591,35 +28659,35 @@
       </c>
       <c r="H773" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I773" t="inlineStr">
         <is>
-          <t>BV1VUcuzvEaU</t>
+          <t>BV1mNBfBBEkr</t>
         </is>
       </c>
     </row>
     <row r="774">
       <c r="A774" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>774</t>
         </is>
       </c>
       <c r="B774" t="inlineStr">
         <is>
-          <t>鱼仔</t>
+          <t>Always Online</t>
         </is>
       </c>
       <c r="C774" t="inlineStr"/>
       <c r="D774" t="inlineStr">
         <is>
-          <t>卢广仲</t>
+          <t>林俊杰</t>
         </is>
       </c>
       <c r="E774" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31，2026/2/10</t>
+          <t>2025/12/30</t>
         </is>
       </c>
       <c r="F774" t="inlineStr"/>
@@ -28630,35 +28698,31 @@
       </c>
       <c r="H774" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I774" t="inlineStr">
-        <is>
-          <t>BV1mNBfBBEkr</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I774" t="inlineStr"/>
     </row>
     <row r="775">
       <c r="A775" t="inlineStr">
         <is>
-          <t>774</t>
+          <t>775</t>
         </is>
       </c>
       <c r="B775" t="inlineStr">
         <is>
-          <t>Always Online</t>
+          <t>如愿</t>
         </is>
       </c>
       <c r="C775" t="inlineStr"/>
       <c r="D775" t="inlineStr">
         <is>
-          <t>林俊杰</t>
+          <t>王菲</t>
         </is>
       </c>
       <c r="E775" t="inlineStr">
         <is>
-          <t>2025/12/30</t>
+          <t>2026/1/5</t>
         </is>
       </c>
       <c r="F775" t="inlineStr"/>
@@ -28677,97 +28741,101 @@
     <row r="776">
       <c r="A776" t="inlineStr">
         <is>
-          <t>775</t>
+          <t>776</t>
         </is>
       </c>
       <c r="B776" t="inlineStr">
         <is>
-          <t>如愿</t>
+          <t>NOT CUTE ANYMORE</t>
         </is>
       </c>
       <c r="C776" t="inlineStr"/>
       <c r="D776" t="inlineStr">
         <is>
-          <t>王菲</t>
+          <t>ILLIT</t>
         </is>
       </c>
       <c r="E776" t="inlineStr">
         <is>
-          <t>2026/1/5</t>
+          <t>2025/12/27，2026/1/5，2026/1/6，2026/1/14，2026/1/23，2026/2/9</t>
         </is>
       </c>
       <c r="F776" t="inlineStr"/>
       <c r="G776" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>韩语</t>
         </is>
       </c>
       <c r="H776" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I776" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I776" t="inlineStr">
+        <is>
+          <t>BV1NrqABkEk4</t>
+        </is>
+      </c>
     </row>
     <row r="777">
       <c r="A777" t="inlineStr">
         <is>
-          <t>776</t>
+          <t>777</t>
         </is>
       </c>
       <c r="B777" t="inlineStr">
         <is>
-          <t>NOT CUTE ANYMORE</t>
+          <t>莫名其妙爱上你</t>
         </is>
       </c>
       <c r="C777" t="inlineStr"/>
       <c r="D777" t="inlineStr">
         <is>
-          <t>ILLIT</t>
+          <t>朱主爱</t>
         </is>
       </c>
       <c r="E777" t="inlineStr">
         <is>
-          <t>2025/12/27，2026/1/5，2026/1/6，2026/1/14，2026/1/23，2026/2/9</t>
+          <t>2026/1/14</t>
         </is>
       </c>
       <c r="F777" t="inlineStr"/>
       <c r="G777" t="inlineStr">
         <is>
-          <t>韩语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H777" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I777" t="inlineStr">
         <is>
-          <t>BV1NrqABkEk4</t>
+          <t>BV1c6rWBBEyT</t>
         </is>
       </c>
     </row>
     <row r="778">
       <c r="A778" t="inlineStr">
         <is>
-          <t>777</t>
+          <t>778</t>
         </is>
       </c>
       <c r="B778" t="inlineStr">
         <is>
-          <t>莫名其妙爱上你</t>
+          <t>三理之歌</t>
         </is>
       </c>
       <c r="C778" t="inlineStr"/>
       <c r="D778" t="inlineStr">
         <is>
-          <t>朱主爱</t>
+          <t>库里之歌</t>
         </is>
       </c>
       <c r="E778" t="inlineStr">
         <is>
-          <t>2026/1/14</t>
+          <t>2026/1/15，2026/1/29</t>
         </is>
       </c>
       <c r="F778" t="inlineStr"/>
@@ -28778,35 +28846,35 @@
       </c>
       <c r="H778" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I778" t="inlineStr">
         <is>
-          <t>BV1c6rWBBEyT</t>
+          <t>BV1kwkFBgEVE</t>
         </is>
       </c>
     </row>
     <row r="779">
       <c r="A779" t="inlineStr">
         <is>
-          <t>778</t>
+          <t>779</t>
         </is>
       </c>
       <c r="B779" t="inlineStr">
         <is>
-          <t>三理之歌</t>
+          <t>坏女孩</t>
         </is>
       </c>
       <c r="C779" t="inlineStr"/>
       <c r="D779" t="inlineStr">
         <is>
-          <t>库里之歌</t>
+          <t>徐良</t>
         </is>
       </c>
       <c r="E779" t="inlineStr">
         <is>
-          <t>2026/1/15，2026/1/29</t>
+          <t>2026/1/19</t>
         </is>
       </c>
       <c r="F779" t="inlineStr"/>
@@ -28817,35 +28885,31 @@
       </c>
       <c r="H779" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I779" t="inlineStr">
-        <is>
-          <t>BV1kwkFBgEVE</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I779" t="inlineStr"/>
     </row>
     <row r="780">
       <c r="A780" t="inlineStr">
         <is>
-          <t>779</t>
+          <t>780</t>
         </is>
       </c>
       <c r="B780" t="inlineStr">
         <is>
-          <t>坏女孩</t>
+          <t>分手快乐</t>
         </is>
       </c>
       <c r="C780" t="inlineStr"/>
       <c r="D780" t="inlineStr">
         <is>
-          <t>徐良</t>
+          <t>梁静茹</t>
         </is>
       </c>
       <c r="E780" t="inlineStr">
         <is>
-          <t>2026/1/19</t>
+          <t>2026/1/21</t>
         </is>
       </c>
       <c r="F780" t="inlineStr"/>
@@ -28864,23 +28928,23 @@
     <row r="781">
       <c r="A781" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>781</t>
         </is>
       </c>
       <c r="B781" t="inlineStr">
         <is>
-          <t>分手快乐</t>
+          <t>我只在乎你</t>
         </is>
       </c>
       <c r="C781" t="inlineStr"/>
       <c r="D781" t="inlineStr">
         <is>
-          <t>梁静茹</t>
+          <t>邓丽君</t>
         </is>
       </c>
       <c r="E781" t="inlineStr">
         <is>
-          <t>2026/1/21</t>
+          <t>2026/1/23</t>
         </is>
       </c>
       <c r="F781" t="inlineStr"/>
@@ -28899,34 +28963,34 @@
     <row r="782">
       <c r="A782" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>782</t>
         </is>
       </c>
       <c r="B782" t="inlineStr">
         <is>
-          <t>我只在乎你</t>
+          <t>死别</t>
         </is>
       </c>
       <c r="C782" t="inlineStr"/>
       <c r="D782" t="inlineStr">
         <is>
-          <t>邓丽君</t>
+          <t>シャノン</t>
         </is>
       </c>
       <c r="E782" t="inlineStr">
         <is>
-          <t>2026/1/23</t>
+          <t>2026/1/23，2026/1/25，2026/2/5，2026/2/9</t>
         </is>
       </c>
       <c r="F782" t="inlineStr"/>
       <c r="G782" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>日语</t>
         </is>
       </c>
       <c r="H782" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I782" t="inlineStr"/>
@@ -28934,34 +28998,34 @@
     <row r="783">
       <c r="A783" t="inlineStr">
         <is>
-          <t>782</t>
+          <t>783</t>
         </is>
       </c>
       <c r="B783" t="inlineStr">
         <is>
-          <t>死别</t>
+          <t>情歌</t>
         </is>
       </c>
       <c r="C783" t="inlineStr"/>
       <c r="D783" t="inlineStr">
         <is>
-          <t>シャノン</t>
+          <t>梁静茹</t>
         </is>
       </c>
       <c r="E783" t="inlineStr">
         <is>
-          <t>2026/1/23，2026/1/25，2026/2/5，2026/2/9</t>
+          <t>2026/1/23</t>
         </is>
       </c>
       <c r="F783" t="inlineStr"/>
       <c r="G783" t="inlineStr">
         <is>
-          <t>日语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H783" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I783" t="inlineStr"/>
@@ -28969,23 +29033,23 @@
     <row r="784">
       <c r="A784" t="inlineStr">
         <is>
-          <t>783</t>
+          <t>784</t>
         </is>
       </c>
       <c r="B784" t="inlineStr">
         <is>
-          <t>情歌</t>
+          <t>几分之几</t>
         </is>
       </c>
       <c r="C784" t="inlineStr"/>
       <c r="D784" t="inlineStr">
         <is>
-          <t>梁静茹</t>
+          <t>卢广仲</t>
         </is>
       </c>
       <c r="E784" t="inlineStr">
         <is>
-          <t>2026/1/23</t>
+          <t>2026/1/24，2026/1/25，2026/1/26，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19</t>
         </is>
       </c>
       <c r="F784" t="inlineStr"/>
@@ -28996,31 +29060,35 @@
       </c>
       <c r="H784" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I784" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I784" t="inlineStr">
+        <is>
+          <t>BV1sEzxBCEua</t>
+        </is>
+      </c>
     </row>
     <row r="785">
       <c r="A785" t="inlineStr">
         <is>
-          <t>784</t>
+          <t>785</t>
         </is>
       </c>
       <c r="B785" t="inlineStr">
         <is>
-          <t>几分之几</t>
+          <t>爱不单行</t>
         </is>
       </c>
       <c r="C785" t="inlineStr"/>
       <c r="D785" t="inlineStr">
         <is>
-          <t>卢广仲</t>
+          <t>罗志祥</t>
         </is>
       </c>
       <c r="E785" t="inlineStr">
         <is>
-          <t>2026/1/24，2026/1/25，2026/1/26，2026/2/2，2026/2/7，2026/2/10，2026/2/14</t>
+          <t>2026/1/24，2026/2/8</t>
         </is>
       </c>
       <c r="F785" t="inlineStr"/>
@@ -29031,168 +29099,164 @@
       </c>
       <c r="H785" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I785" t="inlineStr">
         <is>
-          <t>BV1sEzxBCEua</t>
+          <t>BV1zPz1BRExW</t>
         </is>
       </c>
     </row>
     <row r="786">
       <c r="A786" t="inlineStr">
         <is>
-          <t>785</t>
+          <t>786</t>
         </is>
       </c>
       <c r="B786" t="inlineStr">
         <is>
-          <t>爱不单行</t>
-        </is>
-      </c>
-      <c r="C786" t="inlineStr"/>
+          <t>STAR WALKIN'</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>逐星</t>
+        </is>
+      </c>
       <c r="D786" t="inlineStr">
         <is>
-          <t>罗志祥</t>
+          <t>Lil Nas X</t>
         </is>
       </c>
       <c r="E786" t="inlineStr">
         <is>
-          <t>2026/1/24，2026/2/8</t>
+          <t>2026/1/25</t>
         </is>
       </c>
       <c r="F786" t="inlineStr"/>
       <c r="G786" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I786" t="inlineStr">
-        <is>
-          <t>BV1zPz1BRExW</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I786" t="inlineStr"/>
     </row>
     <row r="787">
       <c r="A787" t="inlineStr">
         <is>
-          <t>786</t>
+          <t>787</t>
         </is>
       </c>
       <c r="B787" t="inlineStr">
         <is>
-          <t>STAR WALKIN'</t>
-        </is>
-      </c>
-      <c r="C787" t="inlineStr">
-        <is>
-          <t>逐星</t>
-        </is>
-      </c>
+          <t>阳光彩虹小白马</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr"/>
       <c r="D787" t="inlineStr">
         <is>
-          <t>Lil Nas X</t>
+          <t>大张伟</t>
         </is>
       </c>
       <c r="E787" t="inlineStr">
         <is>
-          <t>2026/1/25</t>
+          <t>2026/1/25，2026/2/10</t>
         </is>
       </c>
       <c r="F787" t="inlineStr"/>
       <c r="G787" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H787" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I787" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I787" t="inlineStr">
+        <is>
+          <t>BV1Gnc4zmEjA</t>
+        </is>
+      </c>
     </row>
     <row r="788">
       <c r="A788" t="inlineStr">
         <is>
-          <t>787</t>
+          <t>788</t>
         </is>
       </c>
       <c r="B788" t="inlineStr">
         <is>
-          <t>阳光彩虹小白马</t>
+          <t>Lulala! Lululala!</t>
         </is>
       </c>
       <c r="C788" t="inlineStr"/>
       <c r="D788" t="inlineStr">
         <is>
-          <t>大张伟</t>
+          <t>鸣潮先约电台</t>
         </is>
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/2/10</t>
+          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8，2026/2/19</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
       <c r="G788" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I788" t="inlineStr">
         <is>
-          <t>BV1Gnc4zmEjA</t>
+          <t>BV1Dv6qBsEXr</t>
         </is>
       </c>
     </row>
     <row r="789">
-      <c r="A789" t="inlineStr">
-        <is>
-          <t>788</t>
-        </is>
-      </c>
+      <c r="A789" t="inlineStr"/>
       <c r="B789" t="inlineStr">
         <is>
-          <t>Lulala! Lululala!</t>
+          <t>爱要坦荡荡(R&amp;B版)</t>
         </is>
       </c>
       <c r="C789" t="inlineStr"/>
       <c r="D789" t="inlineStr">
         <is>
-          <t>鸣潮先约电台</t>
+          <t>顾叮当</t>
         </is>
       </c>
       <c r="E789" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8</t>
+          <t>2026/1/29</t>
         </is>
       </c>
       <c r="F789" t="inlineStr"/>
       <c r="G789" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H789" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I789" t="inlineStr">
         <is>
-          <t>BV1Dv6qBsEXr</t>
+          <t>BV1Xx6cBRE14</t>
         </is>
       </c>
     </row>
@@ -29200,24 +29264,24 @@
       <c r="A790" t="inlineStr"/>
       <c r="B790" t="inlineStr">
         <is>
-          <t>爱要坦荡荡(R&amp;B版)</t>
+          <t>Long Live</t>
         </is>
       </c>
       <c r="C790" t="inlineStr"/>
       <c r="D790" t="inlineStr">
         <is>
-          <t>顾叮当</t>
+          <t>Taylor Swift</t>
         </is>
       </c>
       <c r="E790" t="inlineStr">
         <is>
-          <t>2026/1/29</t>
+          <t>2026/1/30</t>
         </is>
       </c>
       <c r="F790" t="inlineStr"/>
       <c r="G790" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H790" t="inlineStr">
@@ -29225,59 +29289,59 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I790" t="inlineStr">
-        <is>
-          <t>BV1Xx6cBRE14</t>
-        </is>
-      </c>
+      <c r="I790" t="inlineStr"/>
     </row>
     <row r="791">
       <c r="A791" t="inlineStr"/>
       <c r="B791" t="inlineStr">
         <is>
-          <t>Long Live</t>
+          <t>身不由己</t>
         </is>
       </c>
       <c r="C791" t="inlineStr"/>
       <c r="D791" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>大都会乐团</t>
         </is>
       </c>
       <c r="E791" t="inlineStr">
         <is>
-          <t>2026/1/30</t>
+          <t>2026/2/2，2026/2/5，2026/2/9</t>
         </is>
       </c>
       <c r="F791" t="inlineStr"/>
       <c r="G791" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H791" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I791" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I791" t="inlineStr">
+        <is>
+          <t>BV1fxFMzqEDd</t>
+        </is>
+      </c>
     </row>
     <row r="792">
       <c r="A792" t="inlineStr"/>
       <c r="B792" t="inlineStr">
         <is>
-          <t>身不由己</t>
+          <t>乐鸣东方</t>
         </is>
       </c>
       <c r="C792" t="inlineStr"/>
       <c r="D792" t="inlineStr">
         <is>
-          <t>大都会乐团</t>
+          <t>洛天依</t>
         </is>
       </c>
       <c r="E792" t="inlineStr">
         <is>
-          <t>2026/2/2，2026/2/5，2026/2/9</t>
+          <t>2026/2/7</t>
         </is>
       </c>
       <c r="F792" t="inlineStr"/>
@@ -29288,26 +29352,22 @@
       </c>
       <c r="H792" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I792" t="inlineStr">
-        <is>
-          <t>BV1fxFMzqEDd</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I792" t="inlineStr"/>
     </row>
     <row r="793">
       <c r="A793" t="inlineStr"/>
       <c r="B793" t="inlineStr">
         <is>
-          <t>乐鸣东方</t>
+          <t>爱的飞行日记</t>
         </is>
       </c>
       <c r="C793" t="inlineStr"/>
       <c r="D793" t="inlineStr">
         <is>
-          <t>洛天依</t>
+          <t>周杰伦</t>
         </is>
       </c>
       <c r="E793" t="inlineStr">
@@ -29326,24 +29386,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I793" t="inlineStr"/>
+      <c r="I793" t="inlineStr">
+        <is>
+          <t>BV1wGF4zFEBM</t>
+        </is>
+      </c>
     </row>
     <row r="794">
       <c r="A794" t="inlineStr"/>
       <c r="B794" t="inlineStr">
         <is>
-          <t>爱的飞行日记</t>
+          <t>相亲相爱</t>
         </is>
       </c>
       <c r="C794" t="inlineStr"/>
       <c r="D794" t="inlineStr">
         <is>
-          <t>周杰伦</t>
+          <t>陈慧琳/张惠妹/孙楠/古淖文</t>
         </is>
       </c>
       <c r="E794" t="inlineStr">
         <is>
-          <t>2026/2/7</t>
+          <t>2026/2/8</t>
         </is>
       </c>
       <c r="F794" t="inlineStr"/>
@@ -29359,7 +29423,7 @@
       </c>
       <c r="I794" t="inlineStr">
         <is>
-          <t>BV1wGF4zFEBM</t>
+          <t>BV1U9cTzpEjm</t>
         </is>
       </c>
     </row>
@@ -29367,18 +29431,18 @@
       <c r="A795" t="inlineStr"/>
       <c r="B795" t="inlineStr">
         <is>
-          <t>相亲相爱</t>
+          <t>混入人类计划</t>
         </is>
       </c>
       <c r="C795" t="inlineStr"/>
       <c r="D795" t="inlineStr">
         <is>
-          <t>陈慧琳/张惠妹/孙楠/古淖文</t>
+          <t>ChiliChill</t>
         </is>
       </c>
       <c r="E795" t="inlineStr">
         <is>
-          <t>2026/2/8</t>
+          <t>2026/2/8，2026/2/9，2026/2/14</t>
         </is>
       </c>
       <c r="F795" t="inlineStr"/>
@@ -29389,12 +29453,12 @@
       </c>
       <c r="H795" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I795" t="inlineStr">
         <is>
-          <t>BV1U9cTzpEjm</t>
+          <t>BV1JncczQEuJ</t>
         </is>
       </c>
     </row>
@@ -29402,34 +29466,34 @@
       <c r="A796" t="inlineStr"/>
       <c r="B796" t="inlineStr">
         <is>
-          <t>混入人类计划</t>
+          <t>纸飞机</t>
         </is>
       </c>
       <c r="C796" t="inlineStr"/>
       <c r="D796" t="inlineStr">
         <is>
-          <t>ChiliChill</t>
+          <t>鸣潮先约电台/飞行雪绒</t>
         </is>
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/14</t>
+          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
       <c r="G796" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
         <is>
-          <t>BV1JncczQEuJ</t>
+          <t>BV1W4cuzSE8Y</t>
         </is>
       </c>
     </row>
@@ -29437,34 +29501,34 @@
       <c r="A797" t="inlineStr"/>
       <c r="B797" t="inlineStr">
         <is>
-          <t>纸飞机</t>
+          <t>刻在我心底的名字</t>
         </is>
       </c>
       <c r="C797" t="inlineStr"/>
       <c r="D797" t="inlineStr">
         <is>
-          <t>鸣潮先约电台/飞行雪绒</t>
+          <t>卢广仲</t>
         </is>
       </c>
       <c r="E797" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14</t>
+          <t>2026/2/9</t>
         </is>
       </c>
       <c r="F797" t="inlineStr"/>
       <c r="G797" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H797" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I797" t="inlineStr">
         <is>
-          <t>BV1W4cuzSE8Y</t>
+          <t>BV1EkcszREeP</t>
         </is>
       </c>
     </row>
@@ -29472,18 +29536,18 @@
       <c r="A798" t="inlineStr"/>
       <c r="B798" t="inlineStr">
         <is>
-          <t>刻在我心底的名字</t>
+          <t>词不达意</t>
         </is>
       </c>
       <c r="C798" t="inlineStr"/>
       <c r="D798" t="inlineStr">
         <is>
-          <t>卢广仲</t>
+          <t>林忆莲</t>
         </is>
       </c>
       <c r="E798" t="inlineStr">
         <is>
-          <t>2026/2/9</t>
+          <t>2026/2/12</t>
         </is>
       </c>
       <c r="F798" t="inlineStr"/>
@@ -29499,7 +29563,7 @@
       </c>
       <c r="I798" t="inlineStr">
         <is>
-          <t>BV1EkcszREeP</t>
+          <t>BV1BNcBz4ECH</t>
         </is>
       </c>
     </row>
@@ -29507,24 +29571,28 @@
       <c r="A799" t="inlineStr"/>
       <c r="B799" t="inlineStr">
         <is>
-          <t>词不达意</t>
-        </is>
-      </c>
-      <c r="C799" t="inlineStr"/>
+          <t>RUNNING FOR YOUR LIFE</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>无所遁藏</t>
+        </is>
+      </c>
       <c r="D799" t="inlineStr">
         <is>
-          <t>林忆莲</t>
+          <t>鸣潮先约电台/Casey Lee Williams</t>
         </is>
       </c>
       <c r="E799" t="inlineStr">
         <is>
-          <t>2026/2/12</t>
+          <t>2026/2/14</t>
         </is>
       </c>
       <c r="F799" t="inlineStr"/>
       <c r="G799" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="H799" t="inlineStr">
@@ -29534,7 +29602,7 @@
       </c>
       <c r="I799" t="inlineStr">
         <is>
-          <t>BV1BNcBz4ECH</t>
+          <t>BV14GZEBgErZ</t>
         </is>
       </c>
     </row>
@@ -29542,38 +29610,34 @@
       <c r="A800" t="inlineStr"/>
       <c r="B800" t="inlineStr">
         <is>
-          <t>RUNNING FOR YOUR LIFE</t>
-        </is>
-      </c>
-      <c r="C800" t="inlineStr">
-        <is>
-          <t>无所遁藏</t>
-        </is>
-      </c>
+          <t>发财发福中国年</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr"/>
       <c r="D800" t="inlineStr">
         <is>
-          <t>鸣潮先约电台/Casey Lee Williams</t>
+          <t>中国娃娃</t>
         </is>
       </c>
       <c r="E800" t="inlineStr">
         <is>
-          <t>2026/2/14</t>
+          <t>2026/2/17，2026/2/19</t>
         </is>
       </c>
       <c r="F800" t="inlineStr"/>
       <c r="G800" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>华语</t>
         </is>
       </c>
       <c r="H800" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I800" t="inlineStr">
         <is>
-          <t>BV14GZEBgErZ</t>
+          <t>BV1EYZ1B6ECT</t>
         </is>
       </c>
     </row>
@@ -29581,13 +29645,13 @@
       <c r="A801" t="inlineStr"/>
       <c r="B801" t="inlineStr">
         <is>
-          <t>发财发福中国年</t>
+          <t>恭喜发财</t>
         </is>
       </c>
       <c r="C801" t="inlineStr"/>
       <c r="D801" t="inlineStr">
         <is>
-          <t>中国娃娃</t>
+          <t>刘德华</t>
         </is>
       </c>
       <c r="E801" t="inlineStr">
@@ -29606,34 +29670,30 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I801" t="inlineStr">
-        <is>
-          <t>BV1EYZ1B6ECT</t>
-        </is>
-      </c>
+      <c r="I801" t="inlineStr"/>
     </row>
     <row r="802">
       <c r="A802" t="inlineStr"/>
       <c r="B802" t="inlineStr">
         <is>
-          <t>恭喜发财</t>
+          <t>迎春花</t>
         </is>
       </c>
       <c r="C802" t="inlineStr"/>
       <c r="D802" t="inlineStr">
         <is>
-          <t>刘德华</t>
+          <t>卓依婷</t>
         </is>
       </c>
       <c r="E802" t="inlineStr">
         <is>
-          <t>2026/2/17</t>
+          <t>2026/2/19</t>
         </is>
       </c>
       <c r="F802" t="inlineStr"/>
       <c r="G802" t="inlineStr">
         <is>
-          <t>华语</t>
+          <t>粤语</t>
         </is>
       </c>
       <c r="H802" t="inlineStr">
@@ -29641,7 +29701,46 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I802" t="inlineStr"/>
+      <c r="I802" t="inlineStr">
+        <is>
+          <t>BV1gnZBBiEmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr"/>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>天堂</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr"/>
+      <c r="D803" t="inlineStr">
+        <is>
+          <t>腾格尔</t>
+        </is>
+      </c>
+      <c r="E803" t="inlineStr">
+        <is>
+          <t>2026/2/19</t>
+        </is>
+      </c>
+      <c r="F803" t="inlineStr"/>
+      <c r="G803" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H803" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I803" t="inlineStr">
+        <is>
+          <t>BV166ZBBQEWz</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 20, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I803"/>
+  <dimension ref="A1:I805"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +583,7 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>英语，韩语</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/14，2025/04/15，2025/05/03，2025/05/19，2025/07/18，2025/07/28，2025/08/28，2025/09/22，2025/10/19，2025/10/26，2025/11/9，2025/12/30</t>
+          <t>2025/03/04，2025/03/14，2025/04/15，2025/05/03，2025/05/19，2025/07/18，2025/07/28，2025/08/28，2025/09/22，2025/10/19，2025/10/26，2025/11/9，2025/12/30，2026/2/20</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29，2026/2/9</t>
+          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29，2026/2/9，2026/2/20</t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>36</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -11515,7 +11515,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>2025/04/06，2025/04/25，2025/07/25，2025/08/28，2025/09/12</t>
+          <t>2025/04/06，2025/04/25，2025/07/25，2025/08/28，2025/09/12，2026/2/20</t>
         </is>
       </c>
       <c r="F298" t="inlineStr"/>
@@ -11526,10 +11526,14 @@
       </c>
       <c r="H298" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I298" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>BV1P3b9z2EZJ</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -13263,7 +13267,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>2025/04/15，2025/05/13，2025/07/14，2025/09/18，2026/1/1，2026/1/9</t>
+          <t>2025/04/15，2025/05/13，2025/07/14，2025/09/18，2026/1/1，2026/1/9，2026/2/20</t>
         </is>
       </c>
       <c r="F346" t="inlineStr"/>
@@ -13274,10 +13278,14 @@
       </c>
       <c r="H346" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I346" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>BV1narMBZEG9</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -29442,7 +29450,7 @@
       </c>
       <c r="E795" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/14</t>
+          <t>2026/2/8，2026/2/9，2026/2/14，2026/2/20</t>
         </is>
       </c>
       <c r="F795" t="inlineStr"/>
@@ -29453,7 +29461,7 @@
       </c>
       <c r="H795" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I795" t="inlineStr">
@@ -29739,6 +29747,72 @@
       <c r="I803" t="inlineStr">
         <is>
           <t>BV166ZBBQEWz</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr"/>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>退后</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr"/>
+      <c r="D804" t="inlineStr">
+        <is>
+          <t>周杰伦</t>
+        </is>
+      </c>
+      <c r="E804" t="inlineStr">
+        <is>
+          <t>2026/2/20</t>
+        </is>
+      </c>
+      <c r="F804" t="inlineStr"/>
+      <c r="G804" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H804" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I804" t="inlineStr"/>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr"/>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>最近还好吗</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr"/>
+      <c r="D805" t="inlineStr">
+        <is>
+          <t>S.H.E</t>
+        </is>
+      </c>
+      <c r="E805" t="inlineStr">
+        <is>
+          <t>2026/2/20</t>
+        </is>
+      </c>
+      <c r="F805" t="inlineStr"/>
+      <c r="G805" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H805" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I805" t="inlineStr">
+        <is>
+          <t>BV14Tf3BWEef</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add some BV numbers
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -1502,7 +1502,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>BV1cG9pYkE8m</t>
+          <t>BV1cG9pYkE8m，BV1B1fGBjEvg</t>
         </is>
       </c>
     </row>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>BV19KmPBDERd</t>
+          <t>BV19KmPBDERd，BV1B1fGBjEtL</t>
         </is>
       </c>
     </row>
@@ -11531,7 +11531,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>BV1P3b9z2EZJ</t>
+          <t>BV1P3b9z2EZJ，BV1zkfGBEE1x</t>
         </is>
       </c>
     </row>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>BV1narMBZEG9</t>
+          <t>BV1narMBZEG9，BV1z6fGBSE1m</t>
         </is>
       </c>
     </row>
@@ -29466,7 +29466,7 @@
       </c>
       <c r="I795" t="inlineStr">
         <is>
-          <t>BV1JncczQEuJ</t>
+          <t>BV1JncczQEuJ，BV1c6fGBDEG1</t>
         </is>
       </c>
     </row>
@@ -29779,7 +29779,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I804" t="inlineStr"/>
+      <c r="I804" t="inlineStr">
+        <is>
+          <t>BV1zkfGBEELD</t>
+        </is>
+      </c>
     </row>
     <row r="805">
       <c r="A805" t="inlineStr"/>

</xml_diff>

<commit_message>
Update song list to Feb 22, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I805"/>
+  <dimension ref="A1:I806"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11624,7 +11624,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>2025/04/06，2025/04/19，2025/05/03，2025/08/01，2025/10/31</t>
+          <t>2025/04/06，2025/04/19，2025/05/03，2025/08/01，2025/10/31，2025/12/15，2026/2/22</t>
         </is>
       </c>
       <c r="F301" t="inlineStr"/>
@@ -11635,10 +11635,14 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I301" t="inlineStr"/>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>BV1SuqVB5EoV</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -16743,7 +16747,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>2025/05/17，2025/05/31，2025/06/15，2025/07/23，2025/09/11，2026/1/1，2026/2/10</t>
+          <t>2025/05/17，2025/05/31，2025/06/15，2025/07/23，2025/09/11，2026/1/1，2026/2/10，2026/2/22</t>
         </is>
       </c>
       <c r="F442" t="inlineStr"/>
@@ -16754,7 +16758,7 @@
       </c>
       <c r="H442" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I442" t="inlineStr">
@@ -29314,7 +29318,7 @@
       </c>
       <c r="E791" t="inlineStr">
         <is>
-          <t>2026/2/2，2026/2/5，2026/2/9</t>
+          <t>2026/2/2，2026/2/5，2026/2/9，2026/2/22</t>
         </is>
       </c>
       <c r="F791" t="inlineStr"/>
@@ -29325,7 +29329,7 @@
       </c>
       <c r="H791" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I791" t="inlineStr">
@@ -29819,6 +29823,37 @@
           <t>BV14Tf3BWEef</t>
         </is>
       </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr"/>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>持续瞬间的永恒</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr"/>
+      <c r="D806" t="inlineStr">
+        <is>
+          <t>鸣潮先约电台/jixwang/markmilian/Sophia</t>
+        </is>
+      </c>
+      <c r="E806" t="inlineStr">
+        <is>
+          <t>2026/2/22</t>
+        </is>
+      </c>
+      <c r="F806" t="inlineStr"/>
+      <c r="G806" t="inlineStr">
+        <is>
+          <t>英语</t>
+        </is>
+      </c>
+      <c r="H806" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I806" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 23, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I806"/>
+  <dimension ref="A1:I808"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/05/01，2025/05/08，2025/05/26，2025/06/05，2025/06/23，2025/06/26，2025/07/03，2025/07/20，2025/07/26，2025/08/03，2025/08/12，2025/08/30，2025/09/21，2025/09/29，2025/11/9，2025/11/12，2025/11/27，2025/12/4，2025/12/28，2026/1/22，2026/2/2</t>
+          <t>2025/03/04，2025/05/01，2025/05/08，2025/05/26，2025/06/05，2025/06/23，2025/06/26，2025/07/03，2025/07/20，2025/07/26，2025/08/03，2025/08/12，2025/08/30，2025/09/21，2025/09/29，2025/11/9，2025/11/12，2025/11/27，2025/12/4，2025/12/28，2026/1/22，2026/2/2，2026/2/23</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/04/14，2025/05/09，2025/06/13，2025/06/19，2025/06/27，2025/07/10，2025/09/10，2025/09/19，2025/11/14，2025/12/31</t>
+          <t>2025/03/04，2025/04/14，2025/05/09，2025/06/13，2025/06/19，2025/06/27，2025/07/10，2025/09/10，2025/09/19，2025/11/14，2025/12/31，2026/2/23</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1380,12 +1380,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>BV1r4oLYfEjE</t>
+          <t>BV1r4oLYfEjE，BV1Asf6BvEo3</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/14，2025/04/15，2025/05/03，2025/05/19，2025/07/18，2025/07/28，2025/08/28，2025/09/22，2025/10/19，2025/10/26，2025/11/9，2025/12/30，2026/2/20</t>
+          <t>2025/03/04，2025/03/14，2025/04/15，2025/05/03，2025/05/19，2025/07/18，2025/07/28，2025/08/28，2025/09/22，2025/10/19，2025/10/26，2025/11/9，2025/12/30，2026/2/20，2026/2/23</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/17，2025/03/28，2025/03/29，2025/04/13，2025/04/15，2025/04/18，2025/04/28，2025/05/22，2025/06/02，2025/06/03，2025/06/10，2025/06/12，2025/06/20，2025/06/20，2025/06/27，2025/07/05，2025/07/09，2025/07/13，2025/08/04，2025/08/08，2025/08/12，2025/08/24，2025/09/06，2025/10/07，2025/10/24，2025/11/24，2025/12/4，2025/12/24，2026/1/15</t>
+          <t>2025/03/07，2025/03/17，2025/03/28，2025/03/29，2025/04/13，2025/04/15，2025/04/18，2025/04/28，2025/05/22，2025/06/02，2025/06/03，2025/06/10，2025/06/12，2025/06/20，2025/06/20，2025/06/27，2025/07/05，2025/07/09，2025/07/13，2025/08/04，2025/08/08，2025/08/12，2025/08/24，2025/09/06，2025/10/07，2025/10/24，2025/11/24，2025/12/4，2025/12/24，2026/1/15，2026/2/23</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/04，2025/04/12，2025/04/18，2025/04/24，2025/06/17，2025/06/19，2025/07/11，2025/07/18，2025/08/28，2025/09/05，2025/09/08，2025/09/27，2025/10/03，2025/12/11，2025/12/30，2026/1/21，2026/1/25，2026/2/10</t>
+          <t>2025/03/07，2025/04/04，2025/04/12，2025/04/18，2025/04/24，2025/06/17，2025/06/19，2025/07/11，2025/07/18，2025/08/28，2025/09/05，2025/09/08，2025/09/27，2025/10/03，2025/12/11，2025/12/30，2026/1/21，2026/1/25，2026/2/10，2026/2/23</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/04/11，2025/04/29，2025/08/01，2025/10/26，2026/2/19</t>
+          <t>2025/03/07，2025/04/11，2025/04/29，2025/08/01，2025/10/26，2026/2/19，2026/2/23</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025/03/09，2025/03/14，2025/04/07，2025/04/15，2025/04/27，2025/05/12，2025/05/27，2025/06/05，2025/06/08，2025/07/20，2025/08/01，2025/09/21，2025/09/28，2025/10/07，2025/10/18，2025/10/24，2025/11/10，2025/12/1，2026/1/16，2026/2/2</t>
+          <t>2025/03/09，2025/03/14，2025/04/07，2025/04/15，2025/04/27，2025/05/12，2025/05/27，2025/06/05，2025/06/08，2025/07/20，2025/08/01，2025/09/21，2025/09/28，2025/10/07，2025/10/18，2025/10/24，2025/11/10，2025/12/1，2026/1/16，2026/2/2，2026/2/23</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29，2026/2/9，2026/2/20</t>
+          <t>2025/03/17，2025/03/28，2025/04/15，2025/04/19，2025/04/25，2025/05/01，2025/05/18，2025/05/25，2025/05/29，2025/06/05，2025/06/12，2025/06/22，2025/07/03，2025/07/11，2025/07/18，2025/07/22，2025/07/31，2025/08/01，2025/08/02，2025/08/03，2025/08/12，2025/09/03，2025/09/11，2025/09/18，2025/09/26，2025/10/03，2025/10/09，2025/10/20，2025/11/12，2025/12/7，2025/12/23，2026/1/5，2026/1/21，2026/1/29，2026/2/9，2026/2/20，2026/2/23</t>
         </is>
       </c>
       <c r="F130" t="inlineStr"/>
@@ -5386,12 +5386,12 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>37</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>BV19KmPBDERd，BV1B1fGBjEtL</t>
+          <t>BV1A1fzBwEjQ，BV19KmPBDERd，BV1B1fGBjEtL</t>
         </is>
       </c>
     </row>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16，2026/2/2</t>
+          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16，2026/2/2，2026/2/23</t>
         </is>
       </c>
       <c r="F153" t="inlineStr"/>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10</t>
+          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10，2026/2/23</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
@@ -6395,7 +6395,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23，2026/1/29</t>
+          <t>2025/03/22，2025/04/05，2025/04/17，2025/04/21，2025/04/22，2025/04/25，2025/05/08，2025/05/15，2025/05/25，2025/05/29，2025/06/03，2025/06/13，2025/06/23，2025/07/06，2025/07/15，2025/08/03，2025/08/16，2025/09/03，2025/09/10，2025/09/30，2025/10/16，2025/10/22，2025/10/30，2025/11/18，2025/12/2，2025/12/5，2025/12/30，2026/1/23，2026/1/29，2026/2/23</t>
         </is>
       </c>
       <c r="F184" t="inlineStr"/>
@@ -7376,12 +7376,12 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>BV1Xr2xBVEqN</t>
+          <t>BV1Xr2xBVEqN，BV1Csf6BeE7B</t>
         </is>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/24，2025/05/13，2025/06/02，2025/06/27，2025/07/14，2025/08/26，2025/09/02，2025/10/03，2025/10/17，2025/11/21，2026/2/14</t>
+          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/24，2025/05/13，2025/06/02，2025/06/27，2025/07/14，2025/08/26，2025/09/02，2025/10/03，2025/10/17，2025/11/21，2026/2/14，2026/2/23</t>
         </is>
       </c>
       <c r="F208" t="inlineStr"/>
@@ -8240,12 +8240,12 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>BV1Z5UEBvEPF</t>
+          <t>BV1Z5UEBvEPF，BV12Ef6BBEgR</t>
         </is>
       </c>
     </row>
@@ -11624,7 +11624,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>2025/04/06，2025/04/19，2025/05/03，2025/08/01，2025/10/31，2025/12/15，2026/2/22</t>
+          <t>2025/04/06，2025/04/19，2025/05/03，2025/08/01，2025/10/31，2025/12/15，2026/2/22，2026/2/23</t>
         </is>
       </c>
       <c r="F301" t="inlineStr"/>
@@ -11635,7 +11635,7 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I301" t="inlineStr">
@@ -12033,7 +12033,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>2025/04/08，2025/05/12，2025/08/22，2025/10/01，2025/10/17</t>
+          <t>2025/04/08，2025/05/12，2025/08/22，2025/10/01，2025/10/17，2026/2/23</t>
         </is>
       </c>
       <c r="F312" t="inlineStr"/>
@@ -12044,10 +12044,14 @@
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I312" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>BV1cnWpzrEtD，BV1FSfzBbEpH</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -13057,7 +13061,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>2025/04/13，2025/07/13，2025/07/18，2025/08/02，2025/09/04，2025/09/12，2025/10/17，2025/11/28，2026/1/22</t>
+          <t>2025/04/13，2025/07/13，2025/07/18，2025/08/02，2025/09/04，2025/09/12，2025/10/17，2025/11/28，2026/1/22，2026/2/23</t>
         </is>
       </c>
       <c r="F340" t="inlineStr"/>
@@ -13068,10 +13072,14 @@
       </c>
       <c r="H340" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I340" t="inlineStr"/>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>BV1GBaQzcE39</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -13598,7 +13606,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>2025/04/17，2025/05/01，2025/05/26，2025/07/03，2025/07/27，2025/09/18，2025/10/17，2025/11/21，2026/1/12，2026/1/24，2026/2/19</t>
+          <t>2025/04/17，2025/05/01，2025/05/26，2025/07/03，2025/07/27，2025/09/18，2025/10/17，2025/11/21，2026/1/12，2026/1/24，2026/2/19，2026/2/23</t>
         </is>
       </c>
       <c r="F355" t="inlineStr"/>
@@ -13609,12 +13617,12 @@
       </c>
       <c r="H355" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t>BV13E33zFES7</t>
+          <t>BV13E33zFES7，BV1Knf6BMELa</t>
         </is>
       </c>
     </row>
@@ -16763,7 +16771,7 @@
       </c>
       <c r="I442" t="inlineStr">
         <is>
-          <t>BV1J67NzGEDg</t>
+          <t>BV1J67NzGEDg，BV173fNB4EZX</t>
         </is>
       </c>
     </row>
@@ -18755,7 +18763,7 @@
       </c>
       <c r="E498" t="inlineStr">
         <is>
-          <t>2025/06/01，2026/1/23，2026/2/2</t>
+          <t>2025/06/01，2026/1/23，2026/2/2，2026/2/23</t>
         </is>
       </c>
       <c r="F498" t="inlineStr"/>
@@ -18766,12 +18774,12 @@
       </c>
       <c r="H498" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I498" t="inlineStr">
         <is>
-          <t>BV1VuzuB1EQf</t>
+          <t>BV1w2fzBhEHL，BV1VuzuB1EQf</t>
         </is>
       </c>
     </row>
@@ -21954,7 +21962,7 @@
       </c>
       <c r="E587" t="inlineStr">
         <is>
-          <t>2025/07/14，2025/07/17，2025/07/18，2025/07/24，2025/07/28，2025/08/02，2025/08/03，2025/08/21，2025/09/05，2025/09/18，2025/09/30，2025/10/19，2025/11/3，2025/11/22，2026/1/5，2026/2/18</t>
+          <t>2025/07/14，2025/07/17，2025/07/18，2025/07/24，2025/07/28，2025/08/02，2025/08/03，2025/08/21，2025/09/05，2025/09/18，2025/09/30，2025/10/19，2025/11/3，2025/11/22，2026/1/5，2026/2/18，2026/2/23</t>
         </is>
       </c>
       <c r="F587" t="inlineStr"/>
@@ -21965,7 +21973,7 @@
       </c>
       <c r="H587" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I587" t="inlineStr">
@@ -23554,7 +23562,7 @@
       </c>
       <c r="E631" t="inlineStr">
         <is>
-          <t>2025/09/10，2025/09/22，2025/09/24，2025/10/23，2025/12/6，2026/1/24，2026/2/5</t>
+          <t>2025/09/10，2025/09/22，2025/09/24，2025/10/23，2025/12/6，2026/1/24，2026/2/5，2026/2/23</t>
         </is>
       </c>
       <c r="F631" t="inlineStr"/>
@@ -23565,7 +23573,7 @@
       </c>
       <c r="H631" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I631" t="inlineStr">
@@ -24235,7 +24243,7 @@
       </c>
       <c r="E650" t="inlineStr">
         <is>
-          <t>2025/09/17，2025/10/11，2025/10/13，2025/10/20，2025/10/25，2025/11/21，2025/12/17</t>
+          <t>2025/09/17，2025/10/11，2025/10/13，2025/10/20，2025/10/25，2025/11/21，2025/12/17，2026/2/23</t>
         </is>
       </c>
       <c r="F650" t="inlineStr"/>
@@ -24246,10 +24254,14 @@
       </c>
       <c r="H650" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I650" t="inlineStr"/>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I650" t="inlineStr">
+        <is>
+          <t>BV1aZWyzREbb，BV1mLf6B6EYy</t>
+        </is>
+      </c>
     </row>
     <row r="651">
       <c r="A651" t="inlineStr">
@@ -26632,7 +26644,7 @@
       </c>
       <c r="E717" t="inlineStr">
         <is>
-          <t>2025/10/24，2025/10/25，2025/10/28，2025/11/12，2025/11/26，2026/1/2，2026/1/5，2026/1/9</t>
+          <t>2025/10/24，2025/10/25，2025/10/28，2025/11/12，2025/11/26，2026/1/2，2026/1/5，2026/1/9，2026/2/23</t>
         </is>
       </c>
       <c r="F717" t="inlineStr"/>
@@ -26643,12 +26655,12 @@
       </c>
       <c r="H717" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I717" t="inlineStr">
         <is>
-          <t>BV1TBihBsEo5</t>
+          <t>BV1TBihBsEo5，BV1ksf6BeE2k</t>
         </is>
       </c>
     </row>
@@ -26710,7 +26722,7 @@
       </c>
       <c r="E719" t="inlineStr">
         <is>
-          <t>2025/10/25，2025/12/2</t>
+          <t>2025/10/25，2025/12/2，2026/2/23</t>
         </is>
       </c>
       <c r="F719" t="inlineStr"/>
@@ -26721,10 +26733,14 @@
       </c>
       <c r="H719" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I719" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I719" t="inlineStr">
+        <is>
+          <t>BV1oV2iBGEn4</t>
+        </is>
+      </c>
     </row>
     <row r="720">
       <c r="A720" t="inlineStr">
@@ -28504,7 +28520,7 @@
       </c>
       <c r="E769" t="inlineStr">
         <is>
-          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25，2026/2/9</t>
+          <t>2025/12/19，2025/12/23，2025/12/26，2026/1/2，2026/1/5，2026/1/11，2026/1/25，2026/2/9，2026/2/23</t>
         </is>
       </c>
       <c r="F769" t="inlineStr"/>
@@ -28515,12 +28531,12 @@
       </c>
       <c r="H769" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I769" t="inlineStr">
         <is>
-          <t>BV1oKiwBXE1L</t>
+          <t>BV1oKiwBXE1L，BV1Csf6BeEYe</t>
         </is>
       </c>
     </row>
@@ -28660,7 +28676,7 @@
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31，2026/2/10</t>
+          <t>2025/12/26，2026/1/10，2026/1/22，2026/1/23，2026/1/31，2026/2/10，2026/2/23</t>
         </is>
       </c>
       <c r="F773" t="inlineStr"/>
@@ -28671,7 +28687,7 @@
       </c>
       <c r="H773" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I773" t="inlineStr">
@@ -29217,7 +29233,7 @@
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8，2026/2/19</t>
+          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8，2026/2/19，2026/2/23</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
@@ -29228,7 +29244,7 @@
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I788" t="inlineStr">
@@ -29489,7 +29505,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19</t>
+          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19，2026/2/23</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29500,12 +29516,12 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
         <is>
-          <t>BV1W4cuzSE8Y</t>
+          <t>BV1W4cuzSE8Y，BV12Ef6BBE5C</t>
         </is>
       </c>
     </row>
@@ -29839,7 +29855,7 @@
       </c>
       <c r="E806" t="inlineStr">
         <is>
-          <t>2026/2/22</t>
+          <t>2026/2/22，2026/2/23</t>
         </is>
       </c>
       <c r="F806" t="inlineStr"/>
@@ -29850,10 +29866,84 @@
       </c>
       <c r="H806" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I806" t="inlineStr">
+        <is>
+          <t>BV1K7f6BgE9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr"/>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>安静</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr"/>
+      <c r="D807" t="inlineStr">
+        <is>
+          <t>周杰伦</t>
+        </is>
+      </c>
+      <c r="E807" t="inlineStr">
+        <is>
+          <t>2026/2/23</t>
+        </is>
+      </c>
+      <c r="F807" t="inlineStr"/>
+      <c r="G807" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H807" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I806" t="inlineStr"/>
+      <c r="I807" t="inlineStr">
+        <is>
+          <t>BV11nf6BTE4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr"/>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>可惜没如果</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr"/>
+      <c r="D808" t="inlineStr">
+        <is>
+          <t>林俊杰</t>
+        </is>
+      </c>
+      <c r="E808" t="inlineStr">
+        <is>
+          <t>2026/2/23</t>
+        </is>
+      </c>
+      <c r="F808" t="inlineStr"/>
+      <c r="G808" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H808" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I808" t="inlineStr">
+        <is>
+          <t>BV1w1fzBwEhj</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 24, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -2835,7 +2835,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19，2026/2/24</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>37</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/03/14，2025/03/29，2025/04/19，2025/04/26，2025/05/09，2025/05/19，2025/05/22，2025/05/25，2025/07/03，2025/07/05，2025/07/28，2025/08/04，2025/08/21，2025/09/30，2025/11/14，2025/11/17，2026/2/10</t>
+          <t>2025/03/13，2025/03/14，2025/03/29，2025/04/19，2025/04/26，2025/05/09，2025/05/19，2025/05/22，2025/05/25，2025/07/03，2025/07/05，2025/07/28，2025/08/04，2025/08/21，2025/09/30，2025/11/14，2025/11/17，2026/2/10，2026/2/24</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -28598,7 +28598,7 @@
       </c>
       <c r="E771" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7，2026/2/19</t>
+          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7，2026/2/19，2026/2/24，2026/2/24</t>
         </is>
       </c>
       <c r="F771" t="inlineStr"/>
@@ -28609,12 +28609,12 @@
       </c>
       <c r="H771" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I771" t="inlineStr">
         <is>
-          <t>BV1pfzcBgERV</t>
+          <t>BV1pfzcBgERV，BV1aff2BvEZF</t>
         </is>
       </c>
     </row>
@@ -29505,7 +29505,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19，2026/2/23</t>
+          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19，2026/2/23，2026/2/24</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29516,7 +29516,7 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
@@ -29614,7 +29614,7 @@
       </c>
       <c r="E799" t="inlineStr">
         <is>
-          <t>2026/2/14</t>
+          <t>2026/2/14，2026/2/24</t>
         </is>
       </c>
       <c r="F799" t="inlineStr"/>
@@ -29625,7 +29625,7 @@
       </c>
       <c r="H799" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I799" t="inlineStr">
@@ -29855,7 +29855,7 @@
       </c>
       <c r="E806" t="inlineStr">
         <is>
-          <t>2026/2/22，2026/2/23</t>
+          <t>2026/2/22，2026/2/23，2026/2/24</t>
         </is>
       </c>
       <c r="F806" t="inlineStr"/>
@@ -29866,7 +29866,7 @@
       </c>
       <c r="H806" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I806" t="inlineStr">

</xml_diff>

<commit_message>
Update song list to Feb 25, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I808"/>
+  <dimension ref="A1:I809"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -940,7 +940,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/12，2025/03/17，2025/03/28，2025/04/07，2025/04/19，2025/04/26，2025/05/06，2025/05/16，2025/05/22，2025/05/30，2025/06/21，2025/07/06，2025/08/22，2025/09/06，2025/09/21，2025/10/23，2025/11/10，2025/11/13，2025/12/4，2026/1/24，2026/1/24，2026/2/19</t>
+          <t>2025/03/04，2025/03/12，2025/03/17，2025/03/28，2025/04/07，2025/04/19，2025/04/26，2025/05/06，2025/05/16，2025/05/22，2025/05/30，2025/06/21，2025/07/06，2025/08/22，2025/09/06，2025/09/21，2025/10/23，2025/11/10，2025/11/13，2025/12/4，2026/1/24，2026/1/24，2026/2/19，2026/2/25</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -951,7 +951,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/17，2025/03/21，2025/04/04，2025/04/14，2025/04/19，2025/04/25，2025/05/08，2025/05/09，2025/05/19，2025/05/27，2025/05/29，2025/06/08，2025/06/09，2025/07/11，2025/07/14，2025/08/04，2025/08/08，2025/08/12，2025/09/18，2025/10/03，2025/10/10，2025/10/23，2025/11/13，2025/11/28，2025/12/13，2025/12/28，2026/1/9，2026/1/28</t>
+          <t>2025/03/04，2025/03/17，2025/03/21，2025/04/04，2025/04/14，2025/04/19，2025/04/25，2025/05/08，2025/05/09，2025/05/19，2025/05/27，2025/05/29，2025/06/08，2025/06/09，2025/07/11，2025/07/14，2025/08/04，2025/08/08，2025/08/12，2025/09/18，2025/10/03，2025/10/10，2025/10/23，2025/11/13，2025/11/28，2025/12/13，2025/12/28，2026/1/9，2026/1/28，2026/2/25</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/03/21，2025/04/19，2025/05/11，2025/06/03，2026/1/19，2026/1/25</t>
+          <t>2025/03/06，2025/03/21，2025/04/19，2025/05/11，2025/06/03，2026/1/19，2026/1/25，2026/2/25</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/04/03，2025/04/14，2025/05/05，2025/05/15，2025/05/29，2025/06/20，2025/06/27，2025/08/07，2025/08/24，2025/09/17，2025/10/16，2025/11/10，2025/12/9，2025/12/17，2026/1/21，2026/2/12</t>
+          <t>2025/03/06，2025/04/03，2025/04/14，2025/05/05，2025/05/15，2025/05/29，2025/06/20，2025/06/27，2025/08/07，2025/08/24，2025/09/17，2025/10/16，2025/11/10，2025/12/9，2025/12/17，2026/1/21，2026/2/12，2026/2/25</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/04/06，2025/04/13，2025/04/22，2025/05/08，2025/05/09，2025/05/30，2025/06/08，2025/08/04，2025/09/18，2025/10/12，2025/11/21，2026/1/24，2026/2/14</t>
+          <t>2025/03/06，2025/04/06，2025/04/13，2025/04/22，2025/05/08，2025/05/09，2025/05/30，2025/06/08，2025/08/04，2025/09/18，2025/10/12，2025/11/21，2026/1/24，2026/2/14，2026/2/25</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19，2026/2/24</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19，2026/2/24，2026/2/25</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>38</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -6228,7 +6228,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16，2026/2/2，2026/2/23</t>
+          <t>2025/03/20，2025/05/19，2025/06/12，2025/06/19，2025/06/23，2025/07/11，2025/08/03，2025/08/12，2025/08/21，2025/09/15，2025/10/07，2025/12/2，2026/1/16，2026/2/2，2026/2/23，2026/2/25</t>
         </is>
       </c>
       <c r="F153" t="inlineStr"/>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10，2026/2/23</t>
+          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10，2026/2/23，2026/2/25</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
@@ -6395,7 +6395,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
@@ -8229,7 +8229,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/24，2025/05/13，2025/06/02，2025/06/27，2025/07/14，2025/08/26，2025/09/02，2025/10/03，2025/10/17，2025/11/21，2026/2/14，2026/2/23</t>
+          <t>2025/03/27，2025/04/03，2025/04/15，2025/04/24，2025/05/13，2025/06/02，2025/06/27，2025/07/14，2025/08/26，2025/09/02，2025/10/03，2025/10/17，2025/11/21，2026/2/14，2026/2/23，2026/2/25</t>
         </is>
       </c>
       <c r="F208" t="inlineStr"/>
@@ -8240,7 +8240,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">
@@ -10009,7 +10009,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/04/28，2025/05/22，2025/06/08，2025/06/27，2025/07/08，2025/08/01，2025/09/03，2025/09/28，2025/10/16，2025/10/23，2025/10/31，2025/12/19，2025/12/31，2026/1/21</t>
+          <t>2025/04/01，2025/04/28，2025/05/22，2025/06/08，2025/06/27，2025/07/08，2025/08/01，2025/09/03，2025/09/28，2025/10/16，2025/10/23，2025/10/31，2025/12/19，2025/12/31，2026/1/21，2026/2/25</t>
         </is>
       </c>
       <c r="F256" t="inlineStr"/>
@@ -10020,10 +10020,14 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="I256" t="inlineStr"/>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>BV1ocznBSE1q</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -17008,7 +17012,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>2025/05/18</t>
+          <t>2025/05/18，2026/2/25</t>
         </is>
       </c>
       <c r="F449" t="inlineStr"/>
@@ -17019,10 +17023,14 @@
       </c>
       <c r="H449" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I449" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>BV1HENXzUEiK</t>
+        </is>
+      </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
@@ -17872,7 +17880,7 @@
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t>2025/05/27，2025/05/29，2025/05/30，2025/05/31，2025/06/02，2025/06/03，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/11，2025/07/22，2025/08/21，2025/09/10，2025/09/26，2025/10/03，2025/10/11，2025/10/26，2025/11/7，2025/12/7，2025/12/23，2026/1/9，2026/1/24，2026/2/9</t>
+          <t>2025/05/27，2025/05/29，2025/05/30，2025/05/31，2025/06/02，2025/06/03，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/11，2025/07/22，2025/08/21，2025/09/10，2025/09/26，2025/10/03，2025/10/11，2025/10/26，2025/11/7，2025/12/7，2025/12/23，2026/1/9，2026/1/24，2026/2/9，2026/2/25</t>
         </is>
       </c>
       <c r="F473" t="inlineStr"/>
@@ -17883,7 +17891,7 @@
       </c>
       <c r="H473" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>27</t>
         </is>
       </c>
       <c r="I473" t="inlineStr">
@@ -21246,7 +21254,7 @@
       </c>
       <c r="E567" t="inlineStr">
         <is>
-          <t>2025/07/03，2025/07/07，2025/07/26，2025/08/28，2025/09/14，2025/10/11，2025/11/26，2025/12/9，2026/1/9，2026/1/23，2026/2/12</t>
+          <t>2025/07/03，2025/07/07，2025/07/26，2025/08/28，2025/09/14，2025/10/11，2025/11/26，2025/12/9，2026/1/9，2026/1/23，2026/2/12，2026/2/25</t>
         </is>
       </c>
       <c r="F567" t="inlineStr"/>
@@ -21257,7 +21265,7 @@
       </c>
       <c r="H567" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="I567" t="inlineStr">
@@ -22394,7 +22402,7 @@
       </c>
       <c r="E599" t="inlineStr">
         <is>
-          <t>2025/07/23，2025/12/12</t>
+          <t>2025/07/23，2025/12/12，2026/2/25</t>
         </is>
       </c>
       <c r="F599" t="inlineStr"/>
@@ -22405,10 +22413,14 @@
       </c>
       <c r="H599" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I599" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I599" t="inlineStr">
+        <is>
+          <t>BV1opmUBmE8R</t>
+        </is>
+      </c>
     </row>
     <row r="600">
       <c r="A600" t="inlineStr">
@@ -23204,7 +23216,7 @@
       </c>
       <c r="E621" t="inlineStr">
         <is>
-          <t>2025/08/24，2025/09/20，2025/10/07，2025/11/9，2025/11/21</t>
+          <t>2025/08/24，2025/09/20，2025/10/07，2025/11/9，2025/11/21，2026/2/25</t>
         </is>
       </c>
       <c r="F621" t="inlineStr"/>
@@ -23215,10 +23227,14 @@
       </c>
       <c r="H621" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I621" t="inlineStr"/>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I621" t="inlineStr">
+        <is>
+          <t>BV1J2kRBZEgH</t>
+        </is>
+      </c>
     </row>
     <row r="622">
       <c r="A622" t="inlineStr">
@@ -25150,7 +25166,7 @@
       </c>
       <c r="E675" t="inlineStr">
         <is>
-          <t>2025/09/26，2025/11/18，2026/1/9</t>
+          <t>2025/09/26，2025/11/18，2026/1/9，2026/2/25</t>
         </is>
       </c>
       <c r="F675" t="inlineStr"/>
@@ -25161,10 +25177,14 @@
       </c>
       <c r="H675" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I675" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I675" t="inlineStr">
+        <is>
+          <t>BV1xoyVBoE8C</t>
+        </is>
+      </c>
     </row>
     <row r="676">
       <c r="A676" t="inlineStr">
@@ -28084,7 +28104,7 @@
       </c>
       <c r="E757" t="inlineStr">
         <is>
-          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5，2026/2/10</t>
+          <t>2025/12/9，2025/12/17，2026/1/14，2026/1/23，2026/2/5，2026/2/10，2026/2/25</t>
         </is>
       </c>
       <c r="F757" t="inlineStr"/>
@@ -28095,7 +28115,7 @@
       </c>
       <c r="H757" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I757" t="inlineStr">
@@ -28598,7 +28618,7 @@
       </c>
       <c r="E771" t="inlineStr">
         <is>
-          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7，2026/2/19，2026/2/24，2026/2/24</t>
+          <t>2025/12/26，2026/1/5，2026/1/19，2026/1/21，2026/1/22，2026/1/24，2026/2/7，2026/2/19，2026/2/24，2026/2/24，2026/2/25</t>
         </is>
       </c>
       <c r="F771" t="inlineStr"/>
@@ -28609,7 +28629,7 @@
       </c>
       <c r="H771" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I771" t="inlineStr">
@@ -29233,7 +29253,7 @@
       </c>
       <c r="E788" t="inlineStr">
         <is>
-          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8，2026/2/19，2026/2/23</t>
+          <t>2026/1/25，2026/1/30，2026/2/2，2026/2/8，2026/2/19，2026/2/23，2026/2/25</t>
         </is>
       </c>
       <c r="F788" t="inlineStr"/>
@@ -29244,7 +29264,7 @@
       </c>
       <c r="H788" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I788" t="inlineStr">
@@ -29505,7 +29525,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19，2026/2/23，2026/2/24</t>
+          <t>2026/2/8，2026/2/9，2026/2/12，2026/2/14，2026/2/19，2026/2/23，2026/2/24，2026/2/25</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29516,7 +29536,7 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
@@ -29855,7 +29875,7 @@
       </c>
       <c r="E806" t="inlineStr">
         <is>
-          <t>2026/2/22，2026/2/23，2026/2/24</t>
+          <t>2026/2/22，2026/2/23，2026/2/24，2026/2/25</t>
         </is>
       </c>
       <c r="F806" t="inlineStr"/>
@@ -29866,7 +29886,7 @@
       </c>
       <c r="H806" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I806" t="inlineStr">
@@ -29942,6 +29962,41 @@
       <c r="I808" t="inlineStr">
         <is>
           <t>BV1w1fzBwEhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr"/>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>星炬不熄</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr"/>
+      <c r="D809" t="inlineStr">
+        <is>
+          <t>鸣潮先约电台/飞行雪绒/星炬学院毕业生</t>
+        </is>
+      </c>
+      <c r="E809" t="inlineStr">
+        <is>
+          <t>2026/2/25</t>
+        </is>
+      </c>
+      <c r="F809" t="inlineStr"/>
+      <c r="G809" t="inlineStr">
+        <is>
+          <t>华语</t>
+        </is>
+      </c>
+      <c r="H809" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I809" t="inlineStr">
+        <is>
+          <t>BV1WDfaByEfD</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update song list to Feb 27, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I808"/>
+  <dimension ref="A1:I809"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025/03/04，2025/03/25，2025/04/29，2025/05/09，2025/05/13，2025/05/22，2025/05/26，2025/05/30，2025/06/08，2025/06/13，2025/06/20，2025/07/05，2025/07/14，2025/07/20，2025/08/01，2025/08/30，2025/09/12，2025/09/17，2025/09/02，2025/09/22，2025/09/24，2025/10/03，2025/10/12，2025/11/14，2025/11/21，2025/11/28，2025/12/17，2026/1/10，2026/1/22，2026/2/10，2026/2/14，2026/2/14</t>
+          <t>2025/03/04，2025/03/25，2025/04/29，2025/05/09，2025/05/13，2025/05/22，2025/05/26，2025/05/30，2025/06/08，2025/06/13，2025/06/20，2025/07/05，2025/07/14，2025/07/20，2025/08/01，2025/08/30，2025/09/12，2025/09/17，2025/09/02，2025/09/22，2025/09/24，2025/10/03，2025/10/12，2025/11/14，2025/11/21，2025/11/28，2025/12/17，2026/1/10，2026/1/22，2026/2/10，2026/2/14，2026/2/14，2026/2/27</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TICKING AWAY (VCT ANTHEM 2023)</t>
+          <t>TICKING AWAY</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2231,10 +2231,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025/03/06，2025/03/28，2025/04/19，2025/04/24，2025/05/03，2025/05/15，2025/05/16，2025/05/22，2025/05/30，2025/06/14，2025/06/19，2025/06/26，2025/07/18，2025/08/04，2025/09/10，2025/09/18，2025/10/03，2026/2/7，2026/2/9</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
+          <t>2025/03/06，2025/03/28，2025/04/19，2025/04/24，2025/05/03，2025/05/15，2025/05/16，2025/05/22，2025/05/30，2025/06/14，2025/06/19，2025/06/26，2025/07/18，2025/08/04，2025/09/10，2025/09/18，2025/10/03，2026/2/7，2026/2/9，2026/2/27</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2023无畏契约全球冠军赛主题曲</t>
+        </is>
+      </c>
       <c r="G46" t="inlineStr">
         <is>
           <t>英语</t>
@@ -2242,7 +2246,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2839,7 +2843,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19，2026/2/24，2026/2/25</t>
+          <t>2025/03/07，2025/03/21，2025/04/04，2025/04/18，2025/04/29，2025/05/08，2025/05/22，2025/05/25，2025/06/06，2025/06/08，2025/06/13，2025/06/13，2025/06/26，2025/07/03，2025/07/05，2025/07/11，2025/07/14，2025/07/26，2025/08/02，2025/08/12，2025/08/21，2025/09/17，2025/11/9，2025/12/4，2025/12/16，2025/12/31，2026/1/9，2026/1/15，2026/1/21，2026/1/23，2026/1/29，2026/2/2，2026/2/7，2026/2/10，2026/2/14，2026/2/19，2026/2/24，2026/2/25，2026/2/27</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2850,7 +2854,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>39</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4203,7 +4207,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2025/03/13，2025/05/12，2025/05/22，2025/06/16，2025/06/30，2025/08/01，2025/08/16，2025/09/19，2025/10/05，2025/11/18，2025/12/23，2026/1/9</t>
+          <t>2025/03/13，2025/05/12，2025/05/22，2025/06/16，2025/06/30，2025/08/01，2025/08/16，2025/09/19，2025/10/05，2025/11/18，2025/12/23，2026/1/9，2026/2/27</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -4214,10 +4218,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr"/>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>BV1cRB1BoENX</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4869,7 +4877,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2025/03/14，2025/04/05，2025/07/22</t>
+          <t>2025/03/14，2025/04/05，2025/07/22，2026/2/27</t>
         </is>
       </c>
       <c r="F116" t="inlineStr"/>
@@ -4880,10 +4888,14 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I116" t="inlineStr"/>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>BV1QhgpzdEb7</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6388,7 +6400,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10，2026/2/23，2026/2/25</t>
+          <t>2025/03/20，2025/04/04，2025/05/03，2025/05/22，2025/06/05，2025/07/25，2025/08/26，2025/08/16，2025/09/21，2025/10/03，2025/11/12，2026/1/23，2026/1/26，2026/2/7，2026/2/10，2026/2/23，2026/2/25，2026/2/27</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
@@ -6399,7 +6411,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
@@ -10013,7 +10025,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>2025/04/01，2025/04/28，2025/05/22，2025/06/08，2025/06/27，2025/07/08，2025/08/01，2025/09/03，2025/09/28，2025/10/16，2025/10/23，2025/10/31，2025/12/19，2025/12/31，2026/1/21，2026/2/25</t>
+          <t>2025/04/01，2025/04/28，2025/05/22，2025/06/08，2025/06/27，2025/07/08，2025/08/01，2025/09/03，2025/09/28，2025/10/16，2025/10/23，2025/10/31，2025/12/19，2025/12/31，2026/1/21，2026/2/25，2026/2/27</t>
         </is>
       </c>
       <c r="F256" t="inlineStr"/>
@@ -10024,7 +10036,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -11418,7 +11430,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>2025/04/05，2025/04/19，2025/05/20，2025/07/11，2025/09/12，2025/12/9，2025/12/16</t>
+          <t>2025/04/05，2025/04/19，2025/05/20，2025/07/11，2025/09/12，2025/12/9，2025/12/16，2026/2/27</t>
         </is>
       </c>
       <c r="F295" t="inlineStr"/>
@@ -11429,7 +11441,7 @@
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I295" t="inlineStr"/>
@@ -13980,7 +13992,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>2025/04/18，2025/05/18，2025/06/19，2025/07/15，2025/08/01，2025/09/17，2025/10/28，2025/11/13，2025/11/14，2026/2/10</t>
+          <t>2025/04/18，2025/05/18，2025/06/19，2025/07/15，2025/08/01，2025/09/17，2025/10/28，2025/11/13，2025/11/14，2026/2/10，2026/2/27</t>
         </is>
       </c>
       <c r="F365" t="inlineStr"/>
@@ -13991,7 +14003,7 @@
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I365" t="inlineStr">
@@ -15327,7 +15339,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24，2026/1/29</t>
+          <t>2025/04/27，2025/05/04，2025/05/26，2025/06/08，2025/08/28，2025/10/18，2025/11/18，2025/12/24，2026/1/29，2026/2/27</t>
         </is>
       </c>
       <c r="F402" t="inlineStr"/>
@@ -15338,7 +15350,7 @@
       </c>
       <c r="H402" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I402" t="inlineStr">
@@ -22048,7 +22060,7 @@
       </c>
       <c r="E589" t="inlineStr">
         <is>
-          <t>2025/07/15，2026/1/5，2026/1/10，2026/1/25，2026/2/10</t>
+          <t>2025/07/15，2026/1/5，2026/1/10，2026/1/25，2026/2/10，2026/2/27</t>
         </is>
       </c>
       <c r="F589" t="inlineStr"/>
@@ -22059,7 +22071,7 @@
       </c>
       <c r="H589" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I589" t="inlineStr">
@@ -24119,7 +24131,7 @@
       </c>
       <c r="E646" t="inlineStr">
         <is>
-          <t>2025/09/13，2025/09/13，2025/09/13，2025/09/17，2025/09/18，2025/09/20，2025/09/21，2025/09/24，2025/09/29，2025/10/10，2025/10/13，2025/10/22，2025/10/30，2025/11/3，2025/11/13，2025/11/24，2025/12/5，2025/12/12，2025/12/17，2026/1/6，2026/1/15，2026/1/24</t>
+          <t>2025/09/13，2025/09/13，2025/09/13，2025/09/17，2025/09/18，2025/09/20，2025/09/21，2025/09/24，2025/09/29，2025/10/10，2025/10/13，2025/10/22，2025/10/30，2025/11/3，2025/11/13，2025/11/24，2025/12/5，2025/12/12，2025/12/17，2026/1/6，2026/1/15，2026/1/24，2026/2/27</t>
         </is>
       </c>
       <c r="F646" t="inlineStr"/>
@@ -24130,7 +24142,7 @@
       </c>
       <c r="H646" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I646" t="inlineStr">
@@ -29529,7 +29541,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>2026/2/9</t>
+          <t>2026/2/9，2026/2/27</t>
         </is>
       </c>
       <c r="F796" t="inlineStr"/>
@@ -29540,12 +29552,12 @@
       </c>
       <c r="H796" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I796" t="inlineStr">
         <is>
-          <t>BV1EkcszREeP</t>
+          <t>BV1EkcszREeP，BV11dAQz2ESx</t>
         </is>
       </c>
     </row>
@@ -29955,7 +29967,7 @@
       <c r="F808" t="inlineStr"/>
       <c r="G808" t="inlineStr">
         <is>
-          <t>华语，韩语</t>
+          <t>华语，日语，英语，韩语</t>
         </is>
       </c>
       <c r="H808" t="inlineStr">
@@ -29968,6 +29980,37 @@
           <t>BV1WDfaByEfD</t>
         </is>
       </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr"/>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Everglow</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr"/>
+      <c r="D809" t="inlineStr">
+        <is>
+          <t>Coldplay</t>
+        </is>
+      </c>
+      <c r="E809" t="inlineStr">
+        <is>
+          <t>2026/2/27</t>
+        </is>
+      </c>
+      <c r="F809" t="inlineStr"/>
+      <c r="G809" t="inlineStr">
+        <is>
+          <t>英语</t>
+        </is>
+      </c>
+      <c r="H809" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I809" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update song list to Feb 28, 2026
</commit_message>
<xml_diff>
--- a/scripts/Book1.xlsx
+++ b/scripts/Book1.xlsx
@@ -4893,7 +4893,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>BV1QhgpzdEb7</t>
+          <t>BV1kcAXzVEWt，BV1QhgpzdEb7</t>
         </is>
       </c>
     </row>
@@ -11444,7 +11444,11 @@
           <t>8</t>
         </is>
       </c>
-      <c r="I295" t="inlineStr"/>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>BV16NAXz6EZ7</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -14008,7 +14012,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t>BV1UgF9zLEPz</t>
+          <t>BV1rwAXzkEr1，BV1UgF9zLEPz</t>
         </is>
       </c>
     </row>
@@ -29471,7 +29475,7 @@
       </c>
       <c r="E794" t="inlineStr">
         <is>
-          <t>2026/2/8，2026/2/9，2026/2/14，2026/2/20</t>
+          <t>2026/2/8，2026/2/9，2026/2/14，2026/2/20，2026/2/28</t>
         </is>
       </c>
       <c r="F794" t="inlineStr"/>
@@ -29482,7 +29486,7 @@
       </c>
       <c r="H794" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I794" t="inlineStr">
@@ -29961,7 +29965,7 @@
       </c>
       <c r="E808" t="inlineStr">
         <is>
-          <t>2026/2/25</t>
+          <t>2026/2/25，2026/2/28</t>
         </is>
       </c>
       <c r="F808" t="inlineStr"/>
@@ -29972,7 +29976,7 @@
       </c>
       <c r="H808" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I808" t="inlineStr">
@@ -30010,7 +30014,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I809" t="inlineStr"/>
+      <c r="I809" t="inlineStr">
+        <is>
+          <t>BV1kcAXzVEXm</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>